<commit_message>
Adding more puzzle results.
</commit_message>
<xml_diff>
--- a/Results/Mixed Bag Solver Puzzle Results.xlsx
+++ b/Results/Mixed Bag Solver Puzzle Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="165" windowWidth="27960" windowHeight="12540" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="165" windowWidth="27960" windowHeight="12540" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cho Best Buddies" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="120">
   <si>
     <t>Solver Type</t>
   </si>
@@ -367,6 +367,21 @@
   </si>
   <si>
     <t>pomeranz_805_7 | pomeranz_805_9 | pomeranz_805_19</t>
+  </si>
+  <si>
+    <t>pomeranz_805_7 | pomeranz_805_12</t>
+  </si>
+  <si>
+    <t>pomeranz_805_2 | pomeranz_805_15</t>
+  </si>
+  <si>
+    <t>pomeranz_805_1 | pomeranz_805_15</t>
+  </si>
+  <si>
+    <t>pomeranz_805_8 | pomeranz_805_9</t>
+  </si>
+  <si>
+    <t>pomeranz_805_4 | pomeranz_805_19</t>
   </si>
 </sst>
 </file>
@@ -899,7 +914,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -935,6 +950,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1285,14 +1301,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.375" customWidth="1"/>
+    <col min="2" max="2" width="10.375" customWidth="1"/>
+    <col min="3" max="3" width="13.75" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.25" customWidth="1"/>
+    <col min="7" max="7" width="18.125" customWidth="1"/>
+    <col min="8" max="8" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1895,14 +1911,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="13.75" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="8" customWidth="1"/>
     <col min="5" max="5" width="16" style="8" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="17.25" style="8" customWidth="1"/>
+    <col min="7" max="7" width="18.125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="17.375" style="8" customWidth="1"/>
     <col min="9" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
@@ -2505,16 +2521,16 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="13.375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="13.875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="17.125" style="8" customWidth="1"/>
     <col min="4" max="4" width="14" style="8" customWidth="1"/>
-    <col min="5" max="6" width="18.7109375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="8" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="8"/>
+    <col min="5" max="6" width="18.75" style="8" customWidth="1"/>
+    <col min="7" max="7" width="20.625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="19.625" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="9.125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3118,31 +3134,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="7" customWidth="1"/>
     <col min="2" max="2" width="9" style="7"/>
-    <col min="3" max="3" width="29.140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="14.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="15.28515625" style="7" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.140625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="9.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="13" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="11.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="12.42578125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="15.28515625" style="7" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.140625" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="9.42578125" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="20" width="12.42578125" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="11.42578125" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="12.42578125" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="15.5703125" style="7" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="17.42578125" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="15.85546875" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="29.125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.25" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21.875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="21.875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="15.25" style="7" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="9.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="13" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="15.25" style="7" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.125" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.375" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="20" width="12.375" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="11.375" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="12.375" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="15.625" style="7" customWidth="1"/>
+    <col min="24" max="24" width="12.25" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="17.375" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.875" style="7" customWidth="1" outlineLevel="1"/>
     <col min="28" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
@@ -6635,59 +6651,59 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW55"/>
+  <dimension ref="A1:AW65"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="8" customWidth="1"/>
     <col min="2" max="2" width="9" style="8"/>
-    <col min="3" max="3" width="46.28515625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="46.25" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="8" customWidth="1"/>
     <col min="5" max="5" width="19" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.28515625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.140625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.28515625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.140625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.5703125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.28515625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.85546875" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.85546875" style="8" customWidth="1"/>
-    <col min="29" max="29" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21.875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="14.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.625" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.25" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.875" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.875" style="8" customWidth="1"/>
+    <col min="29" max="29" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.875" style="8" customWidth="1" collapsed="1"/>
     <col min="50" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
@@ -6911,7 +6927,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:F47" si="0">D3-E3</f>
+        <f t="shared" ref="F3" si="0">D3-E3</f>
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -8234,7 +8250,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="5">
-        <f>D12-E12</f>
+        <f t="shared" ref="F12:F27" si="1">D12-E12</f>
         <v>0</v>
       </c>
       <c r="G12" s="5" t="s">
@@ -8381,7 +8397,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="5">
-        <f>D13-E13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
@@ -8528,7 +8544,7 @@
         <v>3</v>
       </c>
       <c r="F14" s="4">
-        <f>D14-E14</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="G14" s="4" t="s">
@@ -8676,7 +8692,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="5">
-        <f>D15-E15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G15" s="5" t="s">
@@ -8823,7 +8839,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="5">
-        <f>D16-E16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
@@ -8970,7 +8986,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="5">
-        <f>D17-E17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
@@ -9117,7 +9133,7 @@
         <v>2</v>
       </c>
       <c r="F18" s="5">
-        <f>D18-E18</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G18" s="5" t="s">
@@ -9264,7 +9280,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="5">
-        <f>D19-E19</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G19" s="5" t="s">
@@ -9411,7 +9427,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="5">
-        <f>D20-E20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G20" s="5" t="s">
@@ -9558,7 +9574,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="5">
-        <f>D21-E21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G21" s="5" t="s">
@@ -9705,7 +9721,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="5">
-        <f>D22-E22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G22" s="5" t="s">
@@ -9852,7 +9868,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="5">
-        <f>D23-E23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G23" s="5" t="s">
@@ -9999,7 +10015,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="5">
-        <f>D24-E24</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G24" s="5" t="s">
@@ -10146,7 +10162,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="5">
-        <f>D25-E25</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G25" s="5" t="s">
@@ -10293,7 +10309,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="5">
-        <f>D26-E26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G26" s="5" t="s">
@@ -10440,7 +10456,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="5">
-        <f>D27-E27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G27" s="5" t="s">
@@ -12200,7 +12216,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="5">
-        <f>D39-E39</f>
+        <f t="shared" ref="F39:F55" si="2">D39-E39</f>
         <v>0</v>
       </c>
       <c r="G39" s="5" t="s">
@@ -12347,7 +12363,7 @@
         <v>2</v>
       </c>
       <c r="F40" s="5">
-        <f>D40-E40</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G40" s="5" t="s">
@@ -12494,7 +12510,7 @@
         <v>2</v>
       </c>
       <c r="F41" s="5">
-        <f>D41-E41</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G41" s="5" t="s">
@@ -12641,7 +12657,7 @@
         <v>2</v>
       </c>
       <c r="F42" s="5">
-        <f>D42-E42</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G42" s="5" t="s">
@@ -12788,7 +12804,7 @@
         <v>2</v>
       </c>
       <c r="F43" s="5">
-        <f>D43-E43</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G43" s="5" t="s">
@@ -12935,7 +12951,7 @@
         <v>2</v>
       </c>
       <c r="F44" s="5">
-        <f>D44-E44</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G44" s="5" t="s">
@@ -13082,7 +13098,7 @@
         <v>2</v>
       </c>
       <c r="F45" s="5">
-        <f>D45-E45</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G45" s="5" t="s">
@@ -13229,7 +13245,7 @@
         <v>2</v>
       </c>
       <c r="F46" s="5">
-        <f>D46-E46</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G46" s="5" t="s">
@@ -13376,7 +13392,7 @@
         <v>2</v>
       </c>
       <c r="F47" s="5">
-        <f>D47-E47</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G47" s="5" t="s">
@@ -13523,7 +13539,7 @@
         <v>2</v>
       </c>
       <c r="F48" s="5">
-        <f>D48-E48</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G48" s="5" t="s">
@@ -13671,7 +13687,7 @@
         <v>2</v>
       </c>
       <c r="F49" s="5">
-        <f>D49-E49</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G49" s="5" t="s">
@@ -13818,7 +13834,7 @@
         <v>2</v>
       </c>
       <c r="F50" s="5">
-        <f>D50-E50</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G50" s="5" t="s">
@@ -13965,7 +13981,7 @@
         <v>2</v>
       </c>
       <c r="F51" s="5">
-        <f>D51-E51</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G51" s="5" t="s">
@@ -14112,7 +14128,7 @@
         <v>2</v>
       </c>
       <c r="F52" s="5">
-        <f>D52-E52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G52" s="5" t="s">
@@ -14259,7 +14275,7 @@
         <v>2</v>
       </c>
       <c r="F53" s="5">
-        <f>D53-E53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G53" s="5" t="s">
@@ -14406,7 +14422,7 @@
         <v>2</v>
       </c>
       <c r="F54" s="5">
-        <f>D54-E54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G54" s="5" t="s">
@@ -14553,7 +14569,7 @@
         <v>2</v>
       </c>
       <c r="F55" s="5">
-        <f>D55-E55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G55" s="5" t="s">
@@ -14681,6 +14697,1466 @@
       </c>
       <c r="AV55" s="5">
         <v>3164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:48" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="4">
+        <v>2</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D56" s="4">
+        <v>2</v>
+      </c>
+      <c r="E56" s="4">
+        <v>3</v>
+      </c>
+      <c r="F56" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H56" s="4">
+        <v>805</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J56" s="4">
+        <v>806</v>
+      </c>
+      <c r="K56" s="4">
+        <v>0</v>
+      </c>
+      <c r="L56" s="4">
+        <v>1.24069478908E-3</v>
+      </c>
+      <c r="M56" s="4">
+        <v>0.99875930521099998</v>
+      </c>
+      <c r="N56" s="4">
+        <v>0</v>
+      </c>
+      <c r="O56" s="4">
+        <v>0</v>
+      </c>
+      <c r="P56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q56" s="4">
+        <v>806</v>
+      </c>
+      <c r="R56" s="4">
+        <v>0.99875930521099998</v>
+      </c>
+      <c r="S56" s="4">
+        <v>1.24069478908E-3</v>
+      </c>
+      <c r="T56" s="4">
+        <v>0</v>
+      </c>
+      <c r="U56" s="4">
+        <v>0</v>
+      </c>
+      <c r="V56" s="4">
+        <v>0</v>
+      </c>
+      <c r="W56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="X56" s="4">
+        <v>809</v>
+      </c>
+      <c r="Y56" s="4">
+        <v>0.99474660074200005</v>
+      </c>
+      <c r="Z56" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA56" s="4">
+        <v>4</v>
+      </c>
+      <c r="AB56" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC56" s="4">
+        <v>805</v>
+      </c>
+      <c r="AD56" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE56" s="4">
+        <v>805</v>
+      </c>
+      <c r="AF56" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG56" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH56" s="4">
+        <v>0.56770186335399997</v>
+      </c>
+      <c r="AI56" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ56" s="4">
+        <v>348</v>
+      </c>
+      <c r="AK56" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL56" s="4">
+        <v>805</v>
+      </c>
+      <c r="AM56" s="4">
+        <v>3.7267080745299998E-3</v>
+      </c>
+      <c r="AN56" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO56" s="4">
+        <v>0.56397515527999997</v>
+      </c>
+      <c r="AP56" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ56" s="4">
+        <v>348</v>
+      </c>
+      <c r="AR56" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS56" s="4">
+        <v>457</v>
+      </c>
+      <c r="AT56" s="4">
+        <v>0.392546583851</v>
+      </c>
+      <c r="AU56" s="4">
+        <v>348</v>
+      </c>
+      <c r="AV56" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="5">
+        <v>2</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D57" s="5">
+        <v>2</v>
+      </c>
+      <c r="E57" s="5">
+        <v>2</v>
+      </c>
+      <c r="F57" s="5">
+        <v>0</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H57" s="5">
+        <v>805</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J57" s="5">
+        <v>1601</v>
+      </c>
+      <c r="K57" s="5">
+        <v>0.40162398500899998</v>
+      </c>
+      <c r="L57" s="5">
+        <v>0.49718925671500003</v>
+      </c>
+      <c r="M57" s="5">
+        <v>0</v>
+      </c>
+      <c r="N57" s="5">
+        <v>0</v>
+      </c>
+      <c r="O57" s="5">
+        <v>162</v>
+      </c>
+      <c r="P57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q57" s="5">
+        <v>1601</v>
+      </c>
+      <c r="R57" s="5">
+        <v>0.40162398500899998</v>
+      </c>
+      <c r="S57" s="5">
+        <v>0.49718925671500003</v>
+      </c>
+      <c r="T57" s="5">
+        <v>0</v>
+      </c>
+      <c r="U57" s="5">
+        <v>0</v>
+      </c>
+      <c r="V57" s="5">
+        <v>162</v>
+      </c>
+      <c r="W57" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X57" s="5">
+        <v>198</v>
+      </c>
+      <c r="Y57" s="5">
+        <v>0.179845422117</v>
+      </c>
+      <c r="Z57" s="5">
+        <v>643</v>
+      </c>
+      <c r="AA57" s="5">
+        <v>36</v>
+      </c>
+      <c r="AB57" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC57" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE57" s="5">
+        <v>1448</v>
+      </c>
+      <c r="AF57" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG57" s="5">
+        <v>0.44406077348099998</v>
+      </c>
+      <c r="AH57" s="5">
+        <v>0.54972375690599995</v>
+      </c>
+      <c r="AI57" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ57" s="5">
+        <v>9</v>
+      </c>
+      <c r="AK57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL57" s="5">
+        <v>1448</v>
+      </c>
+      <c r="AM57" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN57" s="5">
+        <v>0.44406077348099998</v>
+      </c>
+      <c r="AO57" s="5">
+        <v>0.54972375690599995</v>
+      </c>
+      <c r="AP57" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ57" s="5">
+        <v>9</v>
+      </c>
+      <c r="AR57" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS57" s="5">
+        <v>3368</v>
+      </c>
+      <c r="AT57" s="5">
+        <v>0.16382884216800001</v>
+      </c>
+      <c r="AU57" s="5">
+        <v>9</v>
+      </c>
+      <c r="AV57" s="5">
+        <v>2572</v>
+      </c>
+    </row>
+    <row r="58" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="5">
+        <v>2</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D58" s="5">
+        <v>2</v>
+      </c>
+      <c r="E58" s="5">
+        <v>2</v>
+      </c>
+      <c r="F58" s="5">
+        <v>0</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H58" s="5">
+        <v>805</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J58" s="5">
+        <v>805</v>
+      </c>
+      <c r="K58" s="5">
+        <v>0</v>
+      </c>
+      <c r="L58" s="5">
+        <v>0</v>
+      </c>
+      <c r="M58" s="5">
+        <v>1</v>
+      </c>
+      <c r="N58" s="5">
+        <v>0</v>
+      </c>
+      <c r="O58" s="5">
+        <v>0</v>
+      </c>
+      <c r="P58" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q58" s="5">
+        <v>805</v>
+      </c>
+      <c r="R58" s="5">
+        <v>0</v>
+      </c>
+      <c r="S58" s="5">
+        <v>0</v>
+      </c>
+      <c r="T58" s="5">
+        <v>1</v>
+      </c>
+      <c r="U58" s="5">
+        <v>0</v>
+      </c>
+      <c r="V58" s="5">
+        <v>0</v>
+      </c>
+      <c r="W58" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X58" s="5">
+        <v>805</v>
+      </c>
+      <c r="Y58" s="5">
+        <v>0.86739130434800005</v>
+      </c>
+      <c r="Z58" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA58" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB58" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC58" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD58" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE58" s="5">
+        <v>805</v>
+      </c>
+      <c r="AF58" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG58" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH58" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI58" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ58" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK58" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL58" s="5">
+        <v>805</v>
+      </c>
+      <c r="AM58" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN58" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO58" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP58" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ58" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR58" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS58" s="5">
+        <v>805</v>
+      </c>
+      <c r="AT58" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU58" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV58" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="5">
+        <v>2</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D59" s="5">
+        <v>2</v>
+      </c>
+      <c r="E59" s="5">
+        <v>2</v>
+      </c>
+      <c r="F59" s="5">
+        <v>0</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H59" s="5">
+        <v>805</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J59" s="5">
+        <v>1610</v>
+      </c>
+      <c r="K59" s="5">
+        <v>0</v>
+      </c>
+      <c r="L59" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="M59" s="5">
+        <v>0.46086956521700001</v>
+      </c>
+      <c r="N59" s="5">
+        <v>0</v>
+      </c>
+      <c r="O59" s="5">
+        <v>63</v>
+      </c>
+      <c r="P59" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q59" s="5">
+        <v>1610</v>
+      </c>
+      <c r="R59" s="5">
+        <v>6.2111801242199999E-3</v>
+      </c>
+      <c r="S59" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="T59" s="5">
+        <v>0.45465838509299999</v>
+      </c>
+      <c r="U59" s="5">
+        <v>0</v>
+      </c>
+      <c r="V59" s="5">
+        <v>63</v>
+      </c>
+      <c r="W59" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X59" s="5">
+        <v>3962</v>
+      </c>
+      <c r="Y59" s="5">
+        <v>0.15937888198799999</v>
+      </c>
+      <c r="Z59" s="5">
+        <v>63</v>
+      </c>
+      <c r="AA59" s="5">
+        <v>3220</v>
+      </c>
+      <c r="AB59" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC59" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD59" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE59" s="5">
+        <v>1547</v>
+      </c>
+      <c r="AF59" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG59" s="5">
+        <v>0.47963800904999998</v>
+      </c>
+      <c r="AH59" s="5">
+        <v>0.52036199095000002</v>
+      </c>
+      <c r="AI59" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ59" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK59" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL59" s="5">
+        <v>1547</v>
+      </c>
+      <c r="AM59" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN59" s="5">
+        <v>0.47963800904999998</v>
+      </c>
+      <c r="AO59" s="5">
+        <v>0.52036199095000002</v>
+      </c>
+      <c r="AP59" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ59" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR59" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS59" s="5">
+        <v>3773</v>
+      </c>
+      <c r="AT59" s="5">
+        <v>0.210243837795</v>
+      </c>
+      <c r="AU59" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV59" s="5">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="60" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" s="5">
+        <v>2</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60" s="5">
+        <v>2</v>
+      </c>
+      <c r="E60" s="5">
+        <v>2</v>
+      </c>
+      <c r="F60" s="5">
+        <v>0</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H60" s="5">
+        <v>805</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J60" s="5">
+        <v>805</v>
+      </c>
+      <c r="K60" s="5">
+        <v>4.9689440993800002E-3</v>
+      </c>
+      <c r="L60" s="5">
+        <v>0</v>
+      </c>
+      <c r="M60" s="5">
+        <v>0.96645962732900004</v>
+      </c>
+      <c r="N60" s="5">
+        <v>1.2422360248399999E-3</v>
+      </c>
+      <c r="O60" s="5">
+        <v>22</v>
+      </c>
+      <c r="P60" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q60" s="5">
+        <v>805</v>
+      </c>
+      <c r="R60" s="5">
+        <v>0.74409937888199995</v>
+      </c>
+      <c r="S60" s="5">
+        <v>0</v>
+      </c>
+      <c r="T60" s="5">
+        <v>0.22857142857099999</v>
+      </c>
+      <c r="U60" s="5">
+        <v>0</v>
+      </c>
+      <c r="V60" s="5">
+        <v>22</v>
+      </c>
+      <c r="W60" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X60" s="5">
+        <v>783</v>
+      </c>
+      <c r="Y60" s="5">
+        <v>0.77981366459599999</v>
+      </c>
+      <c r="Z60" s="5">
+        <v>22</v>
+      </c>
+      <c r="AA60" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB60" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC60" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD60" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE60" s="5">
+        <v>827</v>
+      </c>
+      <c r="AF60" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG60" s="5">
+        <v>2.6602176541699999E-2</v>
+      </c>
+      <c r="AH60" s="5">
+        <v>0.97339782345799997</v>
+      </c>
+      <c r="AI60" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ60" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK60" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL60" s="5">
+        <v>827</v>
+      </c>
+      <c r="AM60" s="5">
+        <v>0.97339782345799997</v>
+      </c>
+      <c r="AN60" s="5">
+        <v>2.6602176541699999E-2</v>
+      </c>
+      <c r="AO60" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP60" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ60" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR60" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS60" s="5">
+        <v>893</v>
+      </c>
+      <c r="AT60" s="5">
+        <v>0.89529675251999996</v>
+      </c>
+      <c r="AU60" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV60" s="5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="5">
+        <v>2</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D61" s="5">
+        <v>2</v>
+      </c>
+      <c r="E61" s="5">
+        <v>2</v>
+      </c>
+      <c r="F61" s="5">
+        <v>0</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H61" s="5">
+        <v>805</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J61" s="5">
+        <v>1610</v>
+      </c>
+      <c r="K61" s="5">
+        <v>0</v>
+      </c>
+      <c r="L61" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="M61" s="5">
+        <v>0.394409937888</v>
+      </c>
+      <c r="N61" s="5">
+        <v>0</v>
+      </c>
+      <c r="O61" s="5">
+        <v>170</v>
+      </c>
+      <c r="P61" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q61" s="5">
+        <v>805</v>
+      </c>
+      <c r="R61" s="5">
+        <v>2.4844720496900001E-3</v>
+      </c>
+      <c r="S61" s="5">
+        <v>0</v>
+      </c>
+      <c r="T61" s="5">
+        <v>0.20869565217399999</v>
+      </c>
+      <c r="U61" s="5">
+        <v>0</v>
+      </c>
+      <c r="V61" s="5">
+        <v>635</v>
+      </c>
+      <c r="W61" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X61" s="5">
+        <v>3855</v>
+      </c>
+      <c r="Y61" s="5">
+        <v>0.13155279503100001</v>
+      </c>
+      <c r="Z61" s="5">
+        <v>170</v>
+      </c>
+      <c r="AA61" s="5">
+        <v>3220</v>
+      </c>
+      <c r="AB61" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC61" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD61" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE61" s="5">
+        <v>1440</v>
+      </c>
+      <c r="AF61" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG61" s="5">
+        <v>0.440972222222</v>
+      </c>
+      <c r="AH61" s="5">
+        <v>0.55902777777799995</v>
+      </c>
+      <c r="AI61" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ61" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK61" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL61" s="5">
+        <v>1440</v>
+      </c>
+      <c r="AM61" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN61" s="5">
+        <v>0.440972222222</v>
+      </c>
+      <c r="AO61" s="5">
+        <v>0.55902777777799995</v>
+      </c>
+      <c r="AP61" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ61" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR61" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS61" s="5">
+        <v>3345</v>
+      </c>
+      <c r="AT61" s="5">
+        <v>0.22683109118100001</v>
+      </c>
+      <c r="AU61" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV61" s="5">
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="62" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="5">
+        <v>2</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" s="5">
+        <v>2</v>
+      </c>
+      <c r="E62" s="5">
+        <v>2</v>
+      </c>
+      <c r="F62" s="5">
+        <v>0</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H62" s="5">
+        <v>805</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J62" s="5">
+        <v>807</v>
+      </c>
+      <c r="K62" s="5">
+        <v>0.99752168525399998</v>
+      </c>
+      <c r="L62" s="5">
+        <v>2.4783147459699999E-3</v>
+      </c>
+      <c r="M62" s="5">
+        <v>0</v>
+      </c>
+      <c r="N62" s="5">
+        <v>0</v>
+      </c>
+      <c r="O62" s="5">
+        <v>0</v>
+      </c>
+      <c r="P62" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q62" s="5">
+        <v>807</v>
+      </c>
+      <c r="R62" s="5">
+        <v>0.99752168525399998</v>
+      </c>
+      <c r="S62" s="5">
+        <v>2.4783147459699999E-3</v>
+      </c>
+      <c r="T62" s="5">
+        <v>0</v>
+      </c>
+      <c r="U62" s="5">
+        <v>0</v>
+      </c>
+      <c r="V62" s="5">
+        <v>0</v>
+      </c>
+      <c r="W62" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X62" s="5">
+        <v>813</v>
+      </c>
+      <c r="Y62" s="5">
+        <v>0.98954489544900004</v>
+      </c>
+      <c r="Z62" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA62" s="5">
+        <v>8</v>
+      </c>
+      <c r="AB62" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC62" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD62" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE62" s="5">
+        <v>805</v>
+      </c>
+      <c r="AF62" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG62" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH62" s="5">
+        <v>0.99751552794999998</v>
+      </c>
+      <c r="AI62" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ62" s="5">
+        <v>2</v>
+      </c>
+      <c r="AK62" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL62" s="5">
+        <v>805</v>
+      </c>
+      <c r="AM62" s="5">
+        <v>0.79751552795000002</v>
+      </c>
+      <c r="AN62" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO62" s="5">
+        <v>0.198757763975</v>
+      </c>
+      <c r="AP62" s="5">
+        <v>1.2422360248399999E-3</v>
+      </c>
+      <c r="AQ62" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR62" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS62" s="5">
+        <v>803</v>
+      </c>
+      <c r="AT62" s="5">
+        <v>0.86956521739100001</v>
+      </c>
+      <c r="AU62" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV62" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="5">
+        <v>2</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D63" s="5">
+        <v>2</v>
+      </c>
+      <c r="E63" s="5">
+        <v>2</v>
+      </c>
+      <c r="F63" s="5">
+        <v>0</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H63" s="5">
+        <v>805</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J63" s="5">
+        <v>1608</v>
+      </c>
+      <c r="K63" s="5">
+        <v>0</v>
+      </c>
+      <c r="L63" s="5">
+        <v>0.49937810945299999</v>
+      </c>
+      <c r="M63" s="5">
+        <v>0.480721393035</v>
+      </c>
+      <c r="N63" s="5">
+        <v>0</v>
+      </c>
+      <c r="O63" s="5">
+        <v>32</v>
+      </c>
+      <c r="P63" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q63" s="5">
+        <v>1608</v>
+      </c>
+      <c r="R63" s="5">
+        <v>0.480721393035</v>
+      </c>
+      <c r="S63" s="5">
+        <v>0.49937810945299999</v>
+      </c>
+      <c r="T63" s="5">
+        <v>0</v>
+      </c>
+      <c r="U63" s="5">
+        <v>0</v>
+      </c>
+      <c r="V63" s="5">
+        <v>32</v>
+      </c>
+      <c r="W63" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X63" s="5">
+        <v>3985</v>
+      </c>
+      <c r="Y63" s="5">
+        <v>0.18801344286800001</v>
+      </c>
+      <c r="Z63" s="5">
+        <v>32</v>
+      </c>
+      <c r="AA63" s="5">
+        <v>3212</v>
+      </c>
+      <c r="AB63" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC63" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD63" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE63" s="5">
+        <v>1578</v>
+      </c>
+      <c r="AF63" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG63" s="5">
+        <v>0.489860583016</v>
+      </c>
+      <c r="AH63" s="5">
+        <v>0.50887198986100002</v>
+      </c>
+      <c r="AI63" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ63" s="5">
+        <v>2</v>
+      </c>
+      <c r="AK63" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL63" s="5">
+        <v>1578</v>
+      </c>
+      <c r="AM63" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN63" s="5">
+        <v>0.489860583016</v>
+      </c>
+      <c r="AO63" s="5">
+        <v>0.50887198986100002</v>
+      </c>
+      <c r="AP63" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ63" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR63" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS63" s="5">
+        <v>3895</v>
+      </c>
+      <c r="AT63" s="5">
+        <v>0.17975365665900001</v>
+      </c>
+      <c r="AU63" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV63" s="5">
+        <v>3092</v>
+      </c>
+    </row>
+    <row r="64" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" s="5">
+        <v>2</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64" s="5">
+        <v>2</v>
+      </c>
+      <c r="E64" s="5">
+        <v>2</v>
+      </c>
+      <c r="F64" s="5">
+        <v>0</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H64" s="5">
+        <v>805</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J64" s="5">
+        <v>805</v>
+      </c>
+      <c r="K64" s="5">
+        <v>0</v>
+      </c>
+      <c r="L64" s="5">
+        <v>0</v>
+      </c>
+      <c r="M64" s="5">
+        <v>0.99751552794999998</v>
+      </c>
+      <c r="N64" s="5">
+        <v>2.4844720496900001E-3</v>
+      </c>
+      <c r="O64" s="5">
+        <v>0</v>
+      </c>
+      <c r="P64" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q64" s="5">
+        <v>805</v>
+      </c>
+      <c r="R64" s="5">
+        <v>0.44472049689400001</v>
+      </c>
+      <c r="S64" s="5">
+        <v>0</v>
+      </c>
+      <c r="T64" s="5">
+        <v>0.55527950310600005</v>
+      </c>
+      <c r="U64" s="5">
+        <v>0</v>
+      </c>
+      <c r="V64" s="5">
+        <v>0</v>
+      </c>
+      <c r="W64" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X64" s="5">
+        <v>805</v>
+      </c>
+      <c r="Y64" s="5">
+        <v>0.73664596273299998</v>
+      </c>
+      <c r="Z64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB64" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC64" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD64" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE64" s="5">
+        <v>805</v>
+      </c>
+      <c r="AF64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH64" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK64" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL64" s="5">
+        <v>805</v>
+      </c>
+      <c r="AM64" s="5">
+        <v>0.99006211180100001</v>
+      </c>
+      <c r="AN64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO64" s="5">
+        <v>9.9378881987600004E-3</v>
+      </c>
+      <c r="AP64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR64" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS64" s="5">
+        <v>805</v>
+      </c>
+      <c r="AT64" s="5">
+        <v>0.99378881987599998</v>
+      </c>
+      <c r="AU64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV64" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="5">
+        <v>2</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D65" s="5">
+        <v>2</v>
+      </c>
+      <c r="E65" s="5">
+        <v>2</v>
+      </c>
+      <c r="F65" s="5">
+        <v>0</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H65" s="5">
+        <v>805</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J65" s="5">
+        <v>1509</v>
+      </c>
+      <c r="K65" s="5">
+        <v>0</v>
+      </c>
+      <c r="L65" s="5">
+        <v>0.46653412856199999</v>
+      </c>
+      <c r="M65" s="5">
+        <v>0.474486414844</v>
+      </c>
+      <c r="N65" s="5">
+        <v>0</v>
+      </c>
+      <c r="O65" s="5">
+        <v>89</v>
+      </c>
+      <c r="P65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q65" s="5">
+        <v>1509</v>
+      </c>
+      <c r="R65" s="5">
+        <v>0</v>
+      </c>
+      <c r="S65" s="5">
+        <v>0.46653412856199999</v>
+      </c>
+      <c r="T65" s="5">
+        <v>0.474486414844</v>
+      </c>
+      <c r="U65" s="5">
+        <v>0</v>
+      </c>
+      <c r="V65" s="5">
+        <v>89</v>
+      </c>
+      <c r="W65" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X65" s="5">
+        <v>3532</v>
+      </c>
+      <c r="Y65" s="5">
+        <v>0.13138635736000001</v>
+      </c>
+      <c r="Z65" s="5">
+        <v>89</v>
+      </c>
+      <c r="AA65" s="5">
+        <v>2816</v>
+      </c>
+      <c r="AB65" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC65" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE65" s="5">
+        <v>1521</v>
+      </c>
+      <c r="AF65" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG65" s="5">
+        <v>0.470742932281</v>
+      </c>
+      <c r="AH65" s="5">
+        <v>0.46285338593000003</v>
+      </c>
+      <c r="AI65" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ65" s="5">
+        <v>101</v>
+      </c>
+      <c r="AK65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL65" s="5">
+        <v>1521</v>
+      </c>
+      <c r="AM65" s="5">
+        <v>0.45759368836300002</v>
+      </c>
+      <c r="AN65" s="5">
+        <v>0.470742932281</v>
+      </c>
+      <c r="AO65" s="5">
+        <v>5.2596975673900002E-3</v>
+      </c>
+      <c r="AP65" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ65" s="5">
+        <v>101</v>
+      </c>
+      <c r="AR65" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS65" s="5">
+        <v>3568</v>
+      </c>
+      <c r="AT65" s="5">
+        <v>0.18710820386999999</v>
+      </c>
+      <c r="AU65" s="5">
+        <v>101</v>
+      </c>
+      <c r="AV65" s="5">
+        <v>2864</v>
       </c>
     </row>
   </sheetData>
@@ -14706,75 +16182,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="8" customWidth="1"/>
     <col min="2" max="2" width="9" style="8"/>
-    <col min="3" max="3" width="56.28515625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="56.25" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="8" customWidth="1"/>
     <col min="5" max="5" width="19" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.28515625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.140625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.28515625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.140625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.5703125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.28515625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.85546875" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.85546875" style="8" customWidth="1"/>
-    <col min="29" max="29" width="14.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.28515625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.140625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.28515625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.140625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.5703125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.28515625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.7109375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.85546875" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.85546875" style="8" customWidth="1"/>
-    <col min="50" max="50" width="14.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.28515625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.140625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.28515625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.140625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.5703125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.28515625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.7109375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.85546875" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="6" width="25.375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21.875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="14.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.625" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.25" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.875" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.875" style="8" customWidth="1"/>
+    <col min="29" max="29" width="14.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.625" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.25" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.75" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.875" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.875" style="8" customWidth="1"/>
+    <col min="50" max="50" width="14.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.625" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.25" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.75" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.875" style="8" customWidth="1" outlineLevel="2"/>
     <col min="70" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
@@ -16767,94 +18243,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="8" customWidth="1"/>
     <col min="2" max="2" width="9" style="8"/>
-    <col min="3" max="3" width="46.28515625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="46.25" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="8" customWidth="1"/>
     <col min="5" max="5" width="19" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="70" max="70" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="72" max="72" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="74" max="74" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="75" max="76" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="77" max="77" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="78" max="78" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="79" max="79" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="80" max="80" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="81" max="81" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="82" max="83" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="84" max="84" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="85" max="85" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="86" max="86" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="88" max="88" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="89" max="89" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="90" max="90" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="6" width="25.375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21.875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="70" max="70" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="72" max="72" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="74" max="74" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="75" max="76" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="77" max="77" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="78" max="78" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="79" max="79" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="80" max="80" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="81" max="81" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="82" max="83" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="84" max="84" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="85" max="85" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="86" max="86" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="88" max="88" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="89" max="89" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="90" max="90" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="91" max="91" width="9" style="8" collapsed="1"/>
     <col min="92" max="16384" width="9" style="8"/>
   </cols>
@@ -17784,12 +19260,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AK1:AQ1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AD1:AJ1"/>
     <mergeCell ref="CH1:CL1"/>
     <mergeCell ref="AR1:AV1"/>
     <mergeCell ref="AY1:BE1"/>
@@ -17797,6 +19267,12 @@
     <mergeCell ref="BM1:BQ1"/>
     <mergeCell ref="BT1:BZ1"/>
     <mergeCell ref="CA1:CG1"/>
+    <mergeCell ref="AK1:AQ1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AD1:AJ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17807,112 +19283,112 @@
   <dimension ref="A1:DI4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="CL11" sqref="CL11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="8" customWidth="1"/>
     <col min="2" max="2" width="9" style="8"/>
-    <col min="3" max="3" width="46.28515625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="46.25" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="8" customWidth="1"/>
     <col min="5" max="5" width="19" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="70" max="70" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="14.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="72" max="72" width="15.28515625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="14.140625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="74" max="74" width="9.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="75" max="76" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="77" max="77" width="11.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="78" max="78" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="79" max="79" width="15.28515625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="80" max="80" width="14.140625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="81" max="81" width="9.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="82" max="83" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="84" max="84" width="11.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="85" max="85" width="12.42578125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="86" max="86" width="15.5703125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="12.28515625" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="88" max="88" width="17.42578125" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="89" max="89" width="14.7109375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="90" max="90" width="15.85546875" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="91" max="91" width="21.85546875" style="8" customWidth="1"/>
-    <col min="92" max="92" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="93" max="93" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="94" max="94" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="95" max="95" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="96" max="97" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="98" max="98" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="99" max="99" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="100" max="100" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="101" max="101" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="102" max="102" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="103" max="104" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="105" max="105" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="106" max="106" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="107" max="107" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="108" max="108" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="109" max="109" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="110" max="110" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="111" max="111" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="6" width="25.375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21.875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="70" max="70" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="14.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="72" max="72" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="74" max="74" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="75" max="76" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="77" max="77" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="78" max="78" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="79" max="79" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="80" max="80" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="81" max="81" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="82" max="83" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="84" max="84" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="85" max="85" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="86" max="86" width="15.625" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="12.25" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="88" max="88" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="89" max="89" width="14.75" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="90" max="90" width="15.875" style="8" customWidth="1" outlineLevel="2"/>
+    <col min="91" max="91" width="21.875" style="8" customWidth="1"/>
+    <col min="92" max="92" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="93" max="93" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="94" max="94" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="95" max="95" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="96" max="97" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="98" max="98" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="99" max="99" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="100" max="100" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="101" max="101" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="102" max="102" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="103" max="104" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="105" max="105" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="106" max="106" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="107" max="107" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="108" max="108" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="109" max="109" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="110" max="110" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="111" max="111" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="112" max="112" width="9" style="8" collapsed="1"/>
     <col min="113" max="16384" width="9" style="8"/>
   </cols>
@@ -19058,11 +20534,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="CO1:CU1"/>
     <mergeCell ref="CV1:DB1"/>
     <mergeCell ref="DC1:DG1"/>
     <mergeCell ref="AD1:AJ1"/>
@@ -19074,6 +20545,11 @@
     <mergeCell ref="BF1:BL1"/>
     <mergeCell ref="AY1:BE1"/>
     <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="CO1:CU1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19089,202 +20565,202 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="8" customWidth="1"/>
     <col min="2" max="2" width="9" style="8"/>
-    <col min="3" max="3" width="46.28515625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="46.25" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="8" customWidth="1"/>
     <col min="5" max="5" width="19" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="70" max="70" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="72" max="72" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="74" max="74" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="75" max="76" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="77" max="77" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="78" max="78" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="79" max="79" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="80" max="80" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="81" max="81" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="82" max="83" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="84" max="84" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="85" max="85" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="86" max="86" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="88" max="88" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="89" max="89" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="90" max="90" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="91" max="91" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="92" max="92" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="93" max="93" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="94" max="94" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="95" max="95" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="96" max="97" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="98" max="98" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="99" max="99" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="100" max="100" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="101" max="101" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="102" max="102" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="103" max="104" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="105" max="105" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="106" max="106" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="107" max="107" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="108" max="108" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="109" max="109" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="110" max="110" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="111" max="111" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="112" max="112" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="113" max="113" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="114" max="114" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="115" max="115" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="116" max="116" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="117" max="118" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="119" max="119" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="120" max="120" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="121" max="121" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="122" max="122" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="123" max="123" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="124" max="125" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="126" max="126" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="127" max="127" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="128" max="128" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="129" max="129" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="130" max="130" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="131" max="131" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="132" max="132" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="133" max="133" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="134" max="134" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="135" max="135" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="136" max="136" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="137" max="137" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="138" max="139" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="140" max="140" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="141" max="141" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="142" max="142" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="143" max="143" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="144" max="144" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="145" max="146" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="147" max="147" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="148" max="148" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="149" max="149" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="150" max="150" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="151" max="151" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="152" max="152" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="153" max="153" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="154" max="154" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="155" max="155" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="156" max="156" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="157" max="157" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="158" max="158" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="159" max="160" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="161" max="161" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="162" max="162" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="163" max="163" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="164" max="164" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="165" max="165" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="166" max="167" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="168" max="168" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="169" max="169" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="170" max="170" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="171" max="171" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="172" max="172" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="173" max="173" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="174" max="174" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="175" max="175" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="176" max="176" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="177" max="177" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="178" max="178" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="179" max="179" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="180" max="181" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="182" max="182" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="183" max="183" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="184" max="184" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="185" max="185" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="186" max="186" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="187" max="188" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="189" max="189" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="190" max="190" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="191" max="191" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="192" max="192" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="193" max="193" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="194" max="194" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="195" max="195" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="196" max="196" width="21.85546875" style="8" customWidth="1" collapsed="1"/>
-    <col min="197" max="197" width="14.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="198" max="198" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="199" max="199" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="200" max="200" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="201" max="202" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="203" max="203" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="204" max="204" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="205" max="205" width="15.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="206" max="206" width="14.140625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="207" max="207" width="9.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="208" max="209" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="210" max="210" width="11.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="211" max="211" width="12.42578125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="212" max="212" width="15.5703125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="213" max="213" width="12.28515625" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="214" max="214" width="17.42578125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="215" max="215" width="14.7109375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="216" max="216" width="15.85546875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="6" width="25.375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21.875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="70" max="70" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="72" max="72" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="74" max="74" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="75" max="76" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="77" max="77" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="78" max="78" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="79" max="79" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="80" max="80" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="81" max="81" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="82" max="83" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="84" max="84" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="85" max="85" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="86" max="86" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="88" max="88" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="89" max="89" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="90" max="90" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="91" max="91" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="92" max="92" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="93" max="93" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="94" max="94" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="95" max="95" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="96" max="97" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="98" max="98" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="99" max="99" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="100" max="100" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="101" max="101" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="102" max="102" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="103" max="104" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="105" max="105" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="106" max="106" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="107" max="107" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="108" max="108" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="109" max="109" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="110" max="110" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="111" max="111" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="112" max="112" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="113" max="113" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="114" max="114" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="115" max="115" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="116" max="116" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="117" max="118" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="119" max="119" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="120" max="120" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="121" max="121" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="122" max="122" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="123" max="123" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="124" max="125" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="126" max="126" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="127" max="127" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="128" max="128" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="129" max="129" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="130" max="130" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="131" max="131" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="132" max="132" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="133" max="133" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="134" max="134" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="135" max="135" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="136" max="136" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="137" max="137" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="138" max="139" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="140" max="140" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="141" max="141" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="142" max="142" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="143" max="143" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="144" max="144" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="145" max="146" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="147" max="147" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="148" max="148" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="149" max="149" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="150" max="150" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="151" max="151" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="152" max="152" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="153" max="153" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="154" max="154" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="155" max="155" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="156" max="156" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="157" max="157" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="158" max="158" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="159" max="160" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="161" max="161" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="162" max="162" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="163" max="163" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="164" max="164" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="165" max="165" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="166" max="167" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="168" max="168" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="169" max="169" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="170" max="170" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="171" max="171" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="172" max="172" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="173" max="173" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="174" max="174" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="175" max="175" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="176" max="176" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="177" max="177" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="178" max="178" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="179" max="179" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="180" max="181" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="182" max="182" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="183" max="183" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="184" max="184" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="185" max="185" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="186" max="186" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="187" max="188" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="189" max="189" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="190" max="190" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="191" max="191" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="192" max="192" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="193" max="193" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="194" max="194" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="195" max="195" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="196" max="196" width="21.875" style="8" customWidth="1" collapsed="1"/>
+    <col min="197" max="197" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="198" max="198" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="199" max="199" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="200" max="200" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="201" max="202" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="203" max="203" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="204" max="204" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="205" max="205" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="206" max="206" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="207" max="207" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="208" max="209" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="210" max="210" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="211" max="211" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="212" max="212" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="213" max="213" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="214" max="214" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="215" max="215" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="216" max="216" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="217" max="217" width="9" style="8" collapsed="1"/>
     <col min="218" max="16384" width="9" style="8"/>
   </cols>
@@ -20848,6 +22324,25 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="HD1:HH1"/>
+    <mergeCell ref="FN1:FR1"/>
+    <mergeCell ref="FU1:GA1"/>
+    <mergeCell ref="GB1:GH1"/>
+    <mergeCell ref="GI1:GM1"/>
+    <mergeCell ref="GP1:GV1"/>
+    <mergeCell ref="GW1:HC1"/>
+    <mergeCell ref="FG1:FM1"/>
+    <mergeCell ref="CH1:CL1"/>
+    <mergeCell ref="CO1:CU1"/>
+    <mergeCell ref="CV1:DB1"/>
+    <mergeCell ref="DC1:DG1"/>
+    <mergeCell ref="DJ1:DP1"/>
+    <mergeCell ref="DQ1:DW1"/>
+    <mergeCell ref="DX1:EB1"/>
+    <mergeCell ref="EE1:EK1"/>
+    <mergeCell ref="EL1:ER1"/>
+    <mergeCell ref="ES1:EW1"/>
+    <mergeCell ref="EZ1:FF1"/>
     <mergeCell ref="CA1:CG1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="I1:O1"/>
@@ -20860,25 +22355,6 @@
     <mergeCell ref="BF1:BL1"/>
     <mergeCell ref="BM1:BQ1"/>
     <mergeCell ref="BT1:BZ1"/>
-    <mergeCell ref="FG1:FM1"/>
-    <mergeCell ref="CH1:CL1"/>
-    <mergeCell ref="CO1:CU1"/>
-    <mergeCell ref="CV1:DB1"/>
-    <mergeCell ref="DC1:DG1"/>
-    <mergeCell ref="DJ1:DP1"/>
-    <mergeCell ref="DQ1:DW1"/>
-    <mergeCell ref="DX1:EB1"/>
-    <mergeCell ref="EE1:EK1"/>
-    <mergeCell ref="EL1:ER1"/>
-    <mergeCell ref="ES1:EW1"/>
-    <mergeCell ref="EZ1:FF1"/>
-    <mergeCell ref="HD1:HH1"/>
-    <mergeCell ref="FN1:FR1"/>
-    <mergeCell ref="FU1:GA1"/>
-    <mergeCell ref="GB1:GH1"/>
-    <mergeCell ref="GI1:GM1"/>
-    <mergeCell ref="GP1:GV1"/>
-    <mergeCell ref="GW1:HC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating the puzzle results with an additional 3 puzzle result.
</commit_message>
<xml_diff>
--- a/Results/Mixed Bag Solver Puzzle Results.xlsx
+++ b/Results/Mixed Bag Solver Puzzle Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="165" windowWidth="27960" windowHeight="12540" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="165" windowWidth="27960" windowHeight="12540" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cho Best Buddies" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1798" uniqueCount="121">
   <si>
     <t>Solver Type</t>
   </si>
@@ -383,12 +383,15 @@
   <si>
     <t>pomeranz_805_4 | pomeranz_805_19</t>
   </si>
+  <si>
+    <t>pomeranz_805_7 | pomeranz_805_15 | pomeranz_805_16</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,18 +401,75 @@
     </font>
     <font>
       <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Cambria"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="major"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -437,14 +497,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -452,13 +512,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -473,41 +526,11 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <scheme val="major"/>
     </font>
     <font>
       <b/>
@@ -519,7 +542,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -534,22 +557,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor indexed="13"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="56"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
     <fill>
@@ -564,169 +734,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -736,6 +759,60 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -766,17 +843,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -798,45 +884,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -845,156 +892,129 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1301,14 +1321,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.375" customWidth="1"/>
-    <col min="2" max="2" width="10.375" customWidth="1"/>
-    <col min="3" max="3" width="13.75" customWidth="1"/>
-    <col min="4" max="4" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="17.25" customWidth="1"/>
-    <col min="7" max="7" width="18.125" customWidth="1"/>
-    <col min="8" max="8" width="17.375" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1353,7 +1373,7 @@
       <c r="E2" s="3">
         <v>97.49</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="7">
         <f>100*(1-H2/84)</f>
         <v>91.666666666666657</v>
       </c>
@@ -1381,7 +1401,7 @@
       <c r="E3" s="5">
         <v>97.59</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <f t="shared" ref="F3:F21" si="0">100*(1-H3/84)</f>
         <v>94.047619047619051</v>
       </c>
@@ -1409,7 +1429,7 @@
       <c r="E4" s="5">
         <v>99.04</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <f t="shared" si="0"/>
         <v>96.428571428571431</v>
       </c>
@@ -1437,7 +1457,7 @@
       <c r="E5" s="5">
         <v>99.77</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <f t="shared" si="0"/>
         <v>92.857142857142861</v>
       </c>
@@ -1465,7 +1485,7 @@
       <c r="E6" s="5">
         <v>99.41</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <f t="shared" si="0"/>
         <v>88.095238095238088</v>
       </c>
@@ -1493,7 +1513,7 @@
       <c r="E7" s="5">
         <v>96.86</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <f t="shared" si="0"/>
         <v>94.047619047619051</v>
       </c>
@@ -1521,7 +1541,7 @@
       <c r="E8" s="5">
         <v>98.59</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="9">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -1549,7 +1569,7 @@
       <c r="E9" s="5">
         <v>99.87</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <f t="shared" si="0"/>
         <v>90.476190476190482</v>
       </c>
@@ -1577,7 +1597,7 @@
       <c r="E10" s="5">
         <v>98.57</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="9">
         <f t="shared" si="0"/>
         <v>85.714285714285722</v>
       </c>
@@ -1605,7 +1625,7 @@
       <c r="E11" s="3">
         <v>99.15</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <f>100*(1-H11/84)</f>
         <v>98.80952380952381</v>
       </c>
@@ -1633,7 +1653,7 @@
       <c r="E12" s="5">
         <v>99.24</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="9">
         <f t="shared" si="0"/>
         <v>95.238095238095227</v>
       </c>
@@ -1661,7 +1681,7 @@
       <c r="E13" s="5">
         <v>97.39</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="9">
         <f t="shared" si="0"/>
         <v>89.285714285714292</v>
       </c>
@@ -1689,7 +1709,7 @@
       <c r="E14" s="5">
         <v>99.29</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="9">
         <f>100*(1-H14/84)</f>
         <v>100</v>
       </c>
@@ -1717,7 +1737,7 @@
       <c r="E15" s="5">
         <v>99.6</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="9">
         <f t="shared" si="0"/>
         <v>90.476190476190482</v>
       </c>
@@ -1745,7 +1765,7 @@
       <c r="E16" s="5">
         <v>98.57</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="9">
         <f t="shared" si="0"/>
         <v>90.476190476190482</v>
       </c>
@@ -1773,7 +1793,7 @@
       <c r="E17" s="5">
         <v>99.38</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="9">
         <f t="shared" si="0"/>
         <v>95.238095238095227</v>
       </c>
@@ -1801,7 +1821,7 @@
       <c r="E18" s="5">
         <v>99.26</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="9">
         <f t="shared" si="0"/>
         <v>92.857142857142861</v>
       </c>
@@ -1829,7 +1849,7 @@
       <c r="E19" s="5">
         <v>98.99</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="9">
         <f t="shared" si="0"/>
         <v>91.666666666666657</v>
       </c>
@@ -1857,7 +1877,7 @@
       <c r="E20" s="5">
         <v>99.8</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="9">
         <f t="shared" si="0"/>
         <v>94.047619047619051</v>
       </c>
@@ -1885,7 +1905,7 @@
       <c r="E21" s="5">
         <v>99.93</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="9">
         <f t="shared" si="0"/>
         <v>86.904761904761912</v>
       </c>
@@ -1897,6 +1917,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1911,15 +1932,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="13.75" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="16" style="8" customWidth="1"/>
-    <col min="6" max="6" width="17.25" style="8" customWidth="1"/>
-    <col min="7" max="7" width="18.125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="17.375" style="8" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="8"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1964,7 +1984,7 @@
       <c r="E2" s="3">
         <v>98.62</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="7">
         <f>100*(1-H2/94)</f>
         <v>88.297872340425528</v>
       </c>
@@ -1992,7 +2012,7 @@
       <c r="E3" s="5">
         <v>98.71</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="7">
         <f t="shared" ref="F3:F21" si="0">100*(1-H3/94)</f>
         <v>96.808510638297875</v>
       </c>
@@ -2020,7 +2040,7 @@
       <c r="E4" s="5">
         <v>94.24</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <f t="shared" si="0"/>
         <v>93.61702127659575</v>
       </c>
@@ -2048,7 +2068,7 @@
       <c r="E5" s="5">
         <v>98.87</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <f t="shared" si="0"/>
         <v>95.744680851063833</v>
       </c>
@@ -2076,7 +2096,7 @@
       <c r="E6" s="5">
         <v>97.42</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <f t="shared" si="0"/>
         <v>92.553191489361694</v>
       </c>
@@ -2104,7 +2124,7 @@
       <c r="E7" s="5">
         <v>98.97</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <f t="shared" si="0"/>
         <v>92.553191489361694</v>
       </c>
@@ -2132,7 +2152,7 @@
       <c r="E8" s="4">
         <v>99.85</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="8">
         <f t="shared" si="0"/>
         <v>96.808510638297875</v>
       </c>
@@ -2160,7 +2180,7 @@
       <c r="E9" s="5">
         <v>94.49</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <f t="shared" si="0"/>
         <v>91.489361702127653</v>
       </c>
@@ -2188,7 +2208,7 @@
       <c r="E10" s="5">
         <v>95.79</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <f t="shared" si="0"/>
         <v>98.936170212765958</v>
       </c>
@@ -2216,7 +2236,7 @@
       <c r="E11" s="3">
         <v>99.3</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <f t="shared" si="0"/>
         <v>86.170212765957444</v>
       </c>
@@ -2244,7 +2264,7 @@
       <c r="E12" s="5">
         <v>99.65</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <f t="shared" si="0"/>
         <v>97.872340425531917</v>
       </c>
@@ -2272,7 +2292,7 @@
       <c r="E13" s="5">
         <v>98.74</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="7">
         <f t="shared" si="0"/>
         <v>91.489361702127653</v>
       </c>
@@ -2300,7 +2320,7 @@
       <c r="E14" s="5">
         <v>99.02</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <f t="shared" si="0"/>
         <v>94.680851063829792</v>
       </c>
@@ -2328,7 +2348,7 @@
       <c r="E15" s="4">
         <v>99.56</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="8">
         <f t="shared" si="0"/>
         <v>89.361702127659569</v>
       </c>
@@ -2356,7 +2376,7 @@
       <c r="E16" s="4">
         <v>99.59</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="8">
         <f t="shared" si="0"/>
         <v>89.361702127659569</v>
       </c>
@@ -2384,7 +2404,7 @@
       <c r="E17" s="4">
         <v>99.63</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="8">
         <f t="shared" si="0"/>
         <v>94.680851063829792</v>
       </c>
@@ -2412,7 +2432,7 @@
       <c r="E18" s="5">
         <v>96.52</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <f t="shared" si="0"/>
         <v>92.553191489361694</v>
       </c>
@@ -2440,7 +2460,7 @@
       <c r="E19" s="5">
         <v>98.25</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="7">
         <f t="shared" si="0"/>
         <v>98.936170212765958</v>
       </c>
@@ -2468,7 +2488,7 @@
       <c r="E20" s="5">
         <v>98.9</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <f t="shared" si="0"/>
         <v>93.61702127659575</v>
       </c>
@@ -2496,7 +2516,7 @@
       <c r="E21" s="5">
         <v>98.07</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="7">
         <f t="shared" si="0"/>
         <v>91.489361702127653</v>
       </c>
@@ -2508,6 +2528,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2521,16 +2542,15 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="13.875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="17.125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="14" style="8" customWidth="1"/>
-    <col min="5" max="6" width="18.75" style="8" customWidth="1"/>
-    <col min="7" max="7" width="20.625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="19.625" style="8" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="8"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2575,7 +2595,7 @@
       <c r="E2" s="3">
         <v>96.62</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="7">
         <f>100*(1-H2/116)</f>
         <v>91.379310344827587</v>
       </c>
@@ -2603,7 +2623,7 @@
       <c r="E3" s="3">
         <v>97.82</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="7">
         <f t="shared" ref="F3:F21" si="0">100*(1-H3/116)</f>
         <v>95.689655172413794</v>
       </c>
@@ -2631,7 +2651,7 @@
       <c r="E4" s="4">
         <v>94.94</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="8">
         <f t="shared" si="0"/>
         <v>87.931034482758619</v>
       </c>
@@ -2659,7 +2679,7 @@
       <c r="E5" s="3">
         <v>94.92</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <f t="shared" si="0"/>
         <v>94.827586206896555</v>
       </c>
@@ -2687,7 +2707,7 @@
       <c r="E6" s="3">
         <v>98.88</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <f t="shared" si="0"/>
         <v>92.241379310344826</v>
       </c>
@@ -2715,7 +2735,7 @@
       <c r="E7" s="3">
         <v>98.35</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <f t="shared" si="0"/>
         <v>95.689655172413794</v>
       </c>
@@ -2743,7 +2763,7 @@
       <c r="E8" s="3">
         <v>99.52</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <f t="shared" si="0"/>
         <v>98.275862068965509</v>
       </c>
@@ -2771,7 +2791,7 @@
       <c r="E9" s="3">
         <v>99.04</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <f t="shared" si="0"/>
         <v>98.275862068965509</v>
       </c>
@@ -2799,7 +2819,7 @@
       <c r="E10" s="3">
         <v>97.71</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <f t="shared" si="0"/>
         <v>92.241379310344826</v>
       </c>
@@ -2827,7 +2847,7 @@
       <c r="E11" s="3">
         <v>99.44</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <f t="shared" si="0"/>
         <v>96.551724137931032</v>
       </c>
@@ -2855,7 +2875,7 @@
       <c r="E12" s="3">
         <v>99.1</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <f t="shared" si="0"/>
         <v>97.41379310344827</v>
       </c>
@@ -2883,7 +2903,7 @@
       <c r="E13" s="4">
         <v>97.68</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="8">
         <f t="shared" si="0"/>
         <v>92.241379310344826</v>
       </c>
@@ -2911,7 +2931,7 @@
       <c r="E14" s="3">
         <v>99.8</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <f t="shared" si="0"/>
         <v>95.689655172413794</v>
       </c>
@@ -2939,7 +2959,7 @@
       <c r="E15" s="3">
         <v>99.93</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <f t="shared" si="0"/>
         <v>98.275862068965509</v>
       </c>
@@ -2967,7 +2987,7 @@
       <c r="E16" s="3">
         <v>99.06</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="7">
         <f t="shared" si="0"/>
         <v>93.965517241379317</v>
       </c>
@@ -2995,7 +3015,7 @@
       <c r="E17" s="4">
         <v>95.53</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="8">
         <f t="shared" si="0"/>
         <v>84.482758620689651</v>
       </c>
@@ -3023,7 +3043,7 @@
       <c r="E18" s="3">
         <v>99.03</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <f t="shared" si="0"/>
         <v>92.241379310344826</v>
       </c>
@@ -3051,7 +3071,7 @@
       <c r="E19" s="3">
         <v>98.73</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="7">
         <f t="shared" si="0"/>
         <v>88.793103448275872</v>
       </c>
@@ -3079,7 +3099,7 @@
       <c r="E20" s="3">
         <v>99.41</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <f t="shared" si="0"/>
         <v>92.241379310344826</v>
       </c>
@@ -3107,7 +3127,7 @@
       <c r="E21" s="3">
         <v>99.37</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="7">
         <f t="shared" si="0"/>
         <v>87.068965517241381</v>
       </c>
@@ -3119,6 +3139,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -3134,65 +3155,63 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="9" style="7"/>
-    <col min="3" max="3" width="29.125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.25" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21.875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="21.875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="14.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="15.25" style="7" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.125" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="9.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="13" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="11.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="12.375" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="15.25" style="7" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.125" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="9.375" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="20" width="12.375" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="11.375" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="12.375" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="15.625" style="7" customWidth="1"/>
-    <col min="24" max="24" width="12.25" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="17.375" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="15.875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="16384" width="9" style="7"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="9.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="13" width="12.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="20" width="12.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="11.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="12.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="15.5703125" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="I1" s="13" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="I1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13" t="s">
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
     </row>
     <row r="2" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6644,6 +6663,7 @@
     <mergeCell ref="P1:V1"/>
     <mergeCell ref="W1:AA1"/>
   </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -6659,110 +6679,108 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9" style="8"/>
-    <col min="3" max="3" width="46.25" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="14.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.25" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.875" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.875" style="8" customWidth="1"/>
-    <col min="29" max="29" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="50" max="16384" width="9" style="8"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.85546875" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="I1" s="13" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="I1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13" t="s">
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AD1" s="13" t="s">
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AD1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13" t="s">
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13" t="s">
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="14"/>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
     </row>
     <row r="2" spans="1:49" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6927,7 +6945,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3" si="0">D3-E3</f>
+        <f>D3-E3</f>
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -7202,7 +7220,7 @@
       <c r="AV4" s="5">
         <v>40</v>
       </c>
-      <c r="AW4" s="8"/>
+      <c r="AW4"/>
     </row>
     <row r="5" spans="1:49" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -8085,7 +8103,7 @@
       <c r="AV10" s="5">
         <v>0</v>
       </c>
-      <c r="AW10" s="8"/>
+      <c r="AW10"/>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -8250,7 +8268,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" ref="F12:F27" si="1">D12-E12</f>
+        <f t="shared" ref="F12:F27" si="0">D12-E12</f>
         <v>0</v>
       </c>
       <c r="G12" s="5" t="s">
@@ -8397,7 +8415,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
@@ -8544,7 +8562,7 @@
         <v>3</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="G14" s="4" t="s">
@@ -8692,7 +8710,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G15" s="5" t="s">
@@ -8839,7 +8857,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
@@ -8986,7 +9004,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
@@ -9133,7 +9151,7 @@
         <v>2</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G18" s="5" t="s">
@@ -9280,7 +9298,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G19" s="5" t="s">
@@ -9427,7 +9445,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G20" s="5" t="s">
@@ -9574,7 +9592,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G21" s="5" t="s">
@@ -9721,7 +9739,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G22" s="5" t="s">
@@ -9868,7 +9886,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G23" s="5" t="s">
@@ -10015,7 +10033,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G24" s="5" t="s">
@@ -10162,7 +10180,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G25" s="5" t="s">
@@ -10309,7 +10327,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G26" s="5" t="s">
@@ -10456,7 +10474,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G27" s="5" t="s">
@@ -12216,7 +12234,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="5">
-        <f t="shared" ref="F39:F55" si="2">D39-E39</f>
+        <f t="shared" ref="F39:F55" si="1">D39-E39</f>
         <v>0</v>
       </c>
       <c r="G39" s="5" t="s">
@@ -12363,7 +12381,7 @@
         <v>2</v>
       </c>
       <c r="F40" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G40" s="5" t="s">
@@ -12510,7 +12528,7 @@
         <v>2</v>
       </c>
       <c r="F41" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G41" s="5" t="s">
@@ -12657,7 +12675,7 @@
         <v>2</v>
       </c>
       <c r="F42" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G42" s="5" t="s">
@@ -12804,7 +12822,7 @@
         <v>2</v>
       </c>
       <c r="F43" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G43" s="5" t="s">
@@ -12951,7 +12969,7 @@
         <v>2</v>
       </c>
       <c r="F44" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G44" s="5" t="s">
@@ -13098,7 +13116,7 @@
         <v>2</v>
       </c>
       <c r="F45" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G45" s="5" t="s">
@@ -13245,7 +13263,7 @@
         <v>2</v>
       </c>
       <c r="F46" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G46" s="5" t="s">
@@ -13392,7 +13410,7 @@
         <v>2</v>
       </c>
       <c r="F47" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G47" s="5" t="s">
@@ -13539,7 +13557,7 @@
         <v>2</v>
       </c>
       <c r="F48" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G48" s="5" t="s">
@@ -13668,7 +13686,7 @@
       <c r="AV48" s="5">
         <v>4</v>
       </c>
-      <c r="AW48" s="8"/>
+      <c r="AW48"/>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
@@ -13687,7 +13705,7 @@
         <v>2</v>
       </c>
       <c r="F49" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G49" s="5" t="s">
@@ -13834,7 +13852,7 @@
         <v>2</v>
       </c>
       <c r="F50" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G50" s="5" t="s">
@@ -13981,7 +13999,7 @@
         <v>2</v>
       </c>
       <c r="F51" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G51" s="5" t="s">
@@ -14128,7 +14146,7 @@
         <v>2</v>
       </c>
       <c r="F52" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G52" s="5" t="s">
@@ -14275,7 +14293,7 @@
         <v>2</v>
       </c>
       <c r="F53" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G53" s="5" t="s">
@@ -14422,7 +14440,7 @@
         <v>2</v>
       </c>
       <c r="F54" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G54" s="5" t="s">
@@ -14569,7 +14587,7 @@
         <v>2</v>
       </c>
       <c r="F55" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G55" s="5" t="s">
@@ -14845,7 +14863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>12</v>
       </c>
@@ -14991,7 +15009,7 @@
         <v>2572</v>
       </c>
     </row>
-    <row r="58" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>8</v>
       </c>
@@ -15137,7 +15155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>12</v>
       </c>
@@ -15283,7 +15301,7 @@
         <v>2968</v>
       </c>
     </row>
-    <row r="60" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>8</v>
       </c>
@@ -15429,7 +15447,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>12</v>
       </c>
@@ -15575,7 +15593,7 @@
         <v>2540</v>
       </c>
     </row>
-    <row r="62" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>8</v>
       </c>
@@ -15721,7 +15739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>12</v>
       </c>
@@ -15867,7 +15885,7 @@
         <v>3092</v>
       </c>
     </row>
-    <row r="64" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>8</v>
       </c>
@@ -16013,7 +16031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>12</v>
       </c>
@@ -16160,10 +16178,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:AW55">
-    <sortCondition ref="A4:A55"/>
-    <sortCondition ref="C4:C55"/>
-  </sortState>
   <mergeCells count="7">
     <mergeCell ref="AR1:AV1"/>
     <mergeCell ref="D1:F1"/>
@@ -16173,6 +16187,7 @@
     <mergeCell ref="AD1:AJ1"/>
     <mergeCell ref="AK1:AQ1"/>
   </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -16180,161 +16195,159 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR10"/>
+  <dimension ref="A1:BR12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:BQ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9" style="8"/>
-    <col min="3" max="3" width="56.25" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="14.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.25" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.875" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.875" style="8" customWidth="1"/>
-    <col min="29" max="29" width="14.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.25" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.75" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.875" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.875" style="8" customWidth="1"/>
-    <col min="50" max="50" width="14.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.25" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.75" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.875" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="70" max="16384" width="9" style="8"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="56.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.85546875" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.85546875" customWidth="1"/>
+    <col min="50" max="50" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.85546875" customWidth="1" outlineLevel="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="I1" s="13" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="I1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13" t="s">
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AD1" s="13" t="s">
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AD1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13" t="s">
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13" t="s">
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="14"/>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
-      <c r="AY1" s="13" t="s">
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AY1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BB1" s="13"/>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="13"/>
-      <c r="BE1" s="13"/>
-      <c r="BF1" s="13" t="s">
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="BG1" s="13"/>
-      <c r="BH1" s="13"/>
-      <c r="BI1" s="13"/>
-      <c r="BJ1" s="13"/>
-      <c r="BK1" s="13"/>
-      <c r="BL1" s="13"/>
-      <c r="BM1" s="13" t="s">
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11"/>
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="BN1" s="14"/>
-      <c r="BO1" s="14"/>
-      <c r="BP1" s="14"/>
-      <c r="BQ1" s="14"/>
+      <c r="BN1" s="12"/>
+      <c r="BO1" s="12"/>
+      <c r="BP1" s="12"/>
+      <c r="BQ1" s="12"/>
     </row>
     <row r="2" spans="1:70" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -18220,6 +18233,424 @@
       </c>
       <c r="BQ10" s="5">
         <v>2500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="5">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5">
+        <v>4</v>
+      </c>
+      <c r="F11" s="5">
+        <v>-1</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="5">
+        <v>805</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="5">
+        <v>805</v>
+      </c>
+      <c r="K11" s="5">
+        <v>1</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+      <c r="O11" s="5">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>805</v>
+      </c>
+      <c r="R11" s="5">
+        <v>1</v>
+      </c>
+      <c r="S11" s="5">
+        <v>0</v>
+      </c>
+      <c r="T11" s="5">
+        <v>0</v>
+      </c>
+      <c r="U11" s="5">
+        <v>0</v>
+      </c>
+      <c r="V11" s="5">
+        <v>0</v>
+      </c>
+      <c r="W11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X11" s="5">
+        <v>805</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC11" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE11" s="5">
+        <v>805</v>
+      </c>
+      <c r="AF11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL11" s="5">
+        <v>805</v>
+      </c>
+      <c r="AM11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS11" s="5">
+        <v>805</v>
+      </c>
+      <c r="AT11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX11" s="5">
+        <v>805</v>
+      </c>
+      <c r="AY11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AZ11" s="5">
+        <v>805</v>
+      </c>
+      <c r="BA11" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB11" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC11" s="5">
+        <v>0.91677018633499996</v>
+      </c>
+      <c r="BD11" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE11" s="5">
+        <v>67</v>
+      </c>
+      <c r="BF11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="BG11" s="5">
+        <v>805</v>
+      </c>
+      <c r="BH11" s="5">
+        <v>0.65217391304299999</v>
+      </c>
+      <c r="BI11" s="5">
+        <v>0</v>
+      </c>
+      <c r="BJ11" s="5">
+        <v>0.26335403726700002</v>
+      </c>
+      <c r="BK11" s="5">
+        <v>1.2422360248399999E-3</v>
+      </c>
+      <c r="BL11" s="5">
+        <v>67</v>
+      </c>
+      <c r="BM11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="BN11" s="5">
+        <v>738</v>
+      </c>
+      <c r="BO11" s="5">
+        <v>0.73322981366499995</v>
+      </c>
+      <c r="BP11" s="5">
+        <v>67</v>
+      </c>
+      <c r="BQ11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5">
+        <v>3</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="5">
+        <v>805</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="5">
+        <v>811</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0.56226880394599998</v>
+      </c>
+      <c r="L12" s="5">
+        <v>7.3982737361300002E-3</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0</v>
+      </c>
+      <c r="O12" s="5">
+        <v>349</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>811</v>
+      </c>
+      <c r="R12" s="5">
+        <v>0.56226880394599998</v>
+      </c>
+      <c r="S12" s="5">
+        <v>7.3982737361300002E-3</v>
+      </c>
+      <c r="T12" s="5">
+        <v>0</v>
+      </c>
+      <c r="U12" s="5">
+        <v>0</v>
+      </c>
+      <c r="V12" s="5">
+        <v>349</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X12" s="5">
+        <v>480</v>
+      </c>
+      <c r="Y12" s="5">
+        <v>0.53468033775599999</v>
+      </c>
+      <c r="Z12" s="5">
+        <v>349</v>
+      </c>
+      <c r="AA12" s="5">
+        <v>24</v>
+      </c>
+      <c r="AB12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC12" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE12" s="5">
+        <v>1606</v>
+      </c>
+      <c r="AF12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="5">
+        <v>0.498754669988</v>
+      </c>
+      <c r="AH12" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AI12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="5">
+        <v>2</v>
+      </c>
+      <c r="AK12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL12" s="5">
+        <v>1606</v>
+      </c>
+      <c r="AM12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN12" s="5">
+        <v>0.498754669988</v>
+      </c>
+      <c r="AO12" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AP12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS12" s="5">
+        <v>4007</v>
+      </c>
+      <c r="AT12" s="5">
+        <v>0.189760538788</v>
+      </c>
+      <c r="AU12" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV12" s="5">
+        <v>3204</v>
+      </c>
+      <c r="AW12" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX12" s="5">
+        <v>805</v>
+      </c>
+      <c r="AY12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AZ12" s="5">
+        <v>1608</v>
+      </c>
+      <c r="BA12" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB12" s="5">
+        <v>0.49937810945299999</v>
+      </c>
+      <c r="BC12" s="5">
+        <v>0.49751243781100002</v>
+      </c>
+      <c r="BD12" s="5">
+        <v>6.2189054726400001E-4</v>
+      </c>
+      <c r="BE12" s="5">
+        <v>4</v>
+      </c>
+      <c r="BF12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="BG12" s="5">
+        <v>1608</v>
+      </c>
+      <c r="BH12" s="5">
+        <v>0.32151741293500002</v>
+      </c>
+      <c r="BI12" s="5">
+        <v>0.49937810945299999</v>
+      </c>
+      <c r="BJ12" s="5">
+        <v>0.17599502487599999</v>
+      </c>
+      <c r="BK12" s="5">
+        <v>6.2189054726400001E-4</v>
+      </c>
+      <c r="BL12" s="5">
+        <v>4</v>
+      </c>
+      <c r="BM12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="BN12" s="5">
+        <v>4013</v>
+      </c>
+      <c r="BO12" s="5">
+        <v>0.15148120487899999</v>
+      </c>
+      <c r="BP12" s="5">
+        <v>4</v>
+      </c>
+      <c r="BQ12" s="5">
+        <v>3212</v>
       </c>
     </row>
   </sheetData>
@@ -18228,14 +18659,16 @@
     <mergeCell ref="AY1:BE1"/>
     <mergeCell ref="BF1:BL1"/>
     <mergeCell ref="BM1:BQ1"/>
+    <mergeCell ref="AD1:AJ1"/>
+    <mergeCell ref="AK1:AQ1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="P1:V1"/>
     <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AD1:AJ1"/>
-    <mergeCell ref="AK1:AQ1"/>
   </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18243,204 +18676,202 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9" style="8"/>
-    <col min="3" max="3" width="46.25" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="70" max="70" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="72" max="72" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="74" max="74" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="75" max="76" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="77" max="77" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="78" max="78" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="79" max="79" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="80" max="80" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="81" max="81" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="82" max="83" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="84" max="84" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="85" max="85" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="86" max="86" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="88" max="88" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="89" max="89" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="90" max="90" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="91" max="91" width="9" style="8" collapsed="1"/>
-    <col min="92" max="16384" width="9" style="8"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="70" max="70" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="72" max="72" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="74" max="74" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="75" max="76" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="77" max="77" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="78" max="78" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="79" max="79" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="80" max="80" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="81" max="81" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="82" max="83" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="84" max="84" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="85" max="85" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="86" max="86" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="88" max="88" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="89" max="89" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="90" max="90" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="91" max="91" width="9" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:90" x14ac:dyDescent="0.25">
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="I1" s="13" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="I1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13" t="s">
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AD1" s="13" t="s">
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AD1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13" t="s">
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13" t="s">
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="14"/>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
-      <c r="AY1" s="13" t="s">
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AY1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BB1" s="13"/>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="13"/>
-      <c r="BE1" s="13"/>
-      <c r="BF1" s="13" t="s">
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="BG1" s="13"/>
-      <c r="BH1" s="13"/>
-      <c r="BI1" s="13"/>
-      <c r="BJ1" s="13"/>
-      <c r="BK1" s="13"/>
-      <c r="BL1" s="13"/>
-      <c r="BM1" s="13" t="s">
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11"/>
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="BN1" s="14"/>
-      <c r="BO1" s="14"/>
-      <c r="BP1" s="14"/>
-      <c r="BQ1" s="14"/>
-      <c r="BT1" s="13" t="s">
+      <c r="BN1" s="12"/>
+      <c r="BO1" s="12"/>
+      <c r="BP1" s="12"/>
+      <c r="BQ1" s="12"/>
+      <c r="BT1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="BU1" s="13"/>
-      <c r="BV1" s="13"/>
-      <c r="BW1" s="13"/>
-      <c r="BX1" s="13"/>
-      <c r="BY1" s="13"/>
-      <c r="BZ1" s="13"/>
-      <c r="CA1" s="13" t="s">
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11"/>
+      <c r="BW1" s="11"/>
+      <c r="BX1" s="11"/>
+      <c r="BY1" s="11"/>
+      <c r="BZ1" s="11"/>
+      <c r="CA1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="CB1" s="13"/>
-      <c r="CC1" s="13"/>
-      <c r="CD1" s="13"/>
-      <c r="CE1" s="13"/>
-      <c r="CF1" s="13"/>
-      <c r="CG1" s="13"/>
-      <c r="CH1" s="13" t="s">
+      <c r="CB1" s="11"/>
+      <c r="CC1" s="11"/>
+      <c r="CD1" s="11"/>
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="CI1" s="14"/>
-      <c r="CJ1" s="14"/>
-      <c r="CK1" s="14"/>
-      <c r="CL1" s="14"/>
+      <c r="CI1" s="12"/>
+      <c r="CJ1" s="12"/>
+      <c r="CK1" s="12"/>
+      <c r="CL1" s="12"/>
     </row>
     <row r="2" spans="1:90" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -19260,6 +19691,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AK1:AQ1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AD1:AJ1"/>
     <mergeCell ref="CH1:CL1"/>
     <mergeCell ref="AR1:AV1"/>
     <mergeCell ref="AY1:BE1"/>
@@ -19267,13 +19704,8 @@
     <mergeCell ref="BM1:BQ1"/>
     <mergeCell ref="BT1:BZ1"/>
     <mergeCell ref="CA1:CG1"/>
-    <mergeCell ref="AK1:AQ1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AD1:AJ1"/>
   </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -19288,242 +19720,240 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9" style="8"/>
-    <col min="3" max="3" width="46.25" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="70" max="70" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="14.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="72" max="72" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="74" max="74" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="75" max="76" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="77" max="77" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="78" max="78" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="79" max="79" width="15.25" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="80" max="80" width="14.125" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="81" max="81" width="9.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="82" max="83" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="84" max="84" width="11.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="85" max="85" width="12.375" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="86" max="86" width="15.625" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="12.25" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="88" max="88" width="17.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="89" max="89" width="14.75" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="90" max="90" width="15.875" style="8" customWidth="1" outlineLevel="2"/>
-    <col min="91" max="91" width="21.875" style="8" customWidth="1"/>
-    <col min="92" max="92" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="93" max="93" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="94" max="94" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="95" max="95" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="96" max="97" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="98" max="98" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="99" max="99" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="100" max="100" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="101" max="101" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="102" max="102" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="103" max="104" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="105" max="105" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="106" max="106" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="107" max="107" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="108" max="108" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="109" max="109" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="110" max="110" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="111" max="111" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="112" max="112" width="9" style="8" collapsed="1"/>
-    <col min="113" max="16384" width="9" style="8"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="70" max="70" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="72" max="72" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="74" max="74" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="75" max="76" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="77" max="77" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="78" max="78" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="79" max="79" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="80" max="80" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="81" max="81" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="82" max="83" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="84" max="84" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="85" max="85" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="86" max="86" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="88" max="88" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="89" max="89" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="90" max="90" width="15.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="91" max="91" width="21.85546875" customWidth="1"/>
+    <col min="92" max="92" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="93" max="93" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="94" max="94" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="95" max="95" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="96" max="97" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="98" max="98" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="99" max="99" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="100" max="100" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="101" max="101" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="102" max="102" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="103" max="104" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="105" max="105" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="106" max="106" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="107" max="107" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="108" max="108" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="109" max="109" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="110" max="110" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="111" max="111" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="112" max="112" width="9" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:113" x14ac:dyDescent="0.25">
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="I1" s="13" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="I1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13" t="s">
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AD1" s="13" t="s">
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AD1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13" t="s">
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13" t="s">
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="14"/>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
-      <c r="AY1" s="13" t="s">
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AY1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BB1" s="13"/>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="13"/>
-      <c r="BE1" s="13"/>
-      <c r="BF1" s="13" t="s">
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="BG1" s="13"/>
-      <c r="BH1" s="13"/>
-      <c r="BI1" s="13"/>
-      <c r="BJ1" s="13"/>
-      <c r="BK1" s="13"/>
-      <c r="BL1" s="13"/>
-      <c r="BM1" s="13" t="s">
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11"/>
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="BN1" s="14"/>
-      <c r="BO1" s="14"/>
-      <c r="BP1" s="14"/>
-      <c r="BQ1" s="14"/>
-      <c r="BT1" s="13" t="s">
+      <c r="BN1" s="12"/>
+      <c r="BO1" s="12"/>
+      <c r="BP1" s="12"/>
+      <c r="BQ1" s="12"/>
+      <c r="BT1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="BU1" s="13"/>
-      <c r="BV1" s="13"/>
-      <c r="BW1" s="13"/>
-      <c r="BX1" s="13"/>
-      <c r="BY1" s="13"/>
-      <c r="BZ1" s="13"/>
-      <c r="CA1" s="13" t="s">
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11"/>
+      <c r="BW1" s="11"/>
+      <c r="BX1" s="11"/>
+      <c r="BY1" s="11"/>
+      <c r="BZ1" s="11"/>
+      <c r="CA1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="CB1" s="13"/>
-      <c r="CC1" s="13"/>
-      <c r="CD1" s="13"/>
-      <c r="CE1" s="13"/>
-      <c r="CF1" s="13"/>
-      <c r="CG1" s="13"/>
-      <c r="CH1" s="13" t="s">
+      <c r="CB1" s="11"/>
+      <c r="CC1" s="11"/>
+      <c r="CD1" s="11"/>
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="CI1" s="14"/>
-      <c r="CJ1" s="14"/>
-      <c r="CK1" s="14"/>
-      <c r="CL1" s="14"/>
-      <c r="CO1" s="13" t="s">
+      <c r="CI1" s="12"/>
+      <c r="CJ1" s="12"/>
+      <c r="CK1" s="12"/>
+      <c r="CL1" s="12"/>
+      <c r="CO1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="CP1" s="13"/>
-      <c r="CQ1" s="13"/>
-      <c r="CR1" s="13"/>
-      <c r="CS1" s="13"/>
-      <c r="CT1" s="13"/>
-      <c r="CU1" s="13"/>
-      <c r="CV1" s="13" t="s">
+      <c r="CP1" s="11"/>
+      <c r="CQ1" s="11"/>
+      <c r="CR1" s="11"/>
+      <c r="CS1" s="11"/>
+      <c r="CT1" s="11"/>
+      <c r="CU1" s="11"/>
+      <c r="CV1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="CW1" s="13"/>
-      <c r="CX1" s="13"/>
-      <c r="CY1" s="13"/>
-      <c r="CZ1" s="13"/>
-      <c r="DA1" s="13"/>
-      <c r="DB1" s="13"/>
-      <c r="DC1" s="13" t="s">
+      <c r="CW1" s="11"/>
+      <c r="CX1" s="11"/>
+      <c r="CY1" s="11"/>
+      <c r="CZ1" s="11"/>
+      <c r="DA1" s="11"/>
+      <c r="DB1" s="11"/>
+      <c r="DC1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="DD1" s="14"/>
-      <c r="DE1" s="14"/>
-      <c r="DF1" s="14"/>
-      <c r="DG1" s="14"/>
+      <c r="DD1" s="12"/>
+      <c r="DE1" s="12"/>
+      <c r="DF1" s="12"/>
+      <c r="DG1" s="12"/>
     </row>
     <row r="2" spans="1:113" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -20534,6 +20964,15 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="BM1:BQ1"/>
+    <mergeCell ref="BF1:BL1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AY1:BE1"/>
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="CO1:CU1"/>
     <mergeCell ref="CV1:DB1"/>
     <mergeCell ref="DC1:DG1"/>
     <mergeCell ref="AD1:AJ1"/>
@@ -20541,16 +20980,8 @@
     <mergeCell ref="CH1:CL1"/>
     <mergeCell ref="CA1:CG1"/>
     <mergeCell ref="BT1:BZ1"/>
-    <mergeCell ref="BM1:BQ1"/>
-    <mergeCell ref="BF1:BL1"/>
-    <mergeCell ref="AY1:BE1"/>
-    <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="CO1:CU1"/>
   </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -20565,462 +20996,460 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9" style="8"/>
-    <col min="3" max="3" width="46.25" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="70" max="70" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="72" max="72" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="74" max="74" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="75" max="76" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="77" max="77" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="78" max="78" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="79" max="79" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="80" max="80" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="81" max="81" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="82" max="83" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="84" max="84" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="85" max="85" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="86" max="86" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="88" max="88" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="89" max="89" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="90" max="90" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="91" max="91" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="92" max="92" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="93" max="93" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="94" max="94" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="95" max="95" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="96" max="97" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="98" max="98" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="99" max="99" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="100" max="100" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="101" max="101" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="102" max="102" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="103" max="104" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="105" max="105" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="106" max="106" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="107" max="107" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="108" max="108" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="109" max="109" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="110" max="110" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="111" max="111" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="112" max="112" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="113" max="113" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="114" max="114" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="115" max="115" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="116" max="116" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="117" max="118" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="119" max="119" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="120" max="120" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="121" max="121" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="122" max="122" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="123" max="123" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="124" max="125" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="126" max="126" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="127" max="127" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="128" max="128" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="129" max="129" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="130" max="130" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="131" max="131" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="132" max="132" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="133" max="133" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="134" max="134" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="135" max="135" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="136" max="136" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="137" max="137" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="138" max="139" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="140" max="140" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="141" max="141" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="142" max="142" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="143" max="143" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="144" max="144" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="145" max="146" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="147" max="147" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="148" max="148" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="149" max="149" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="150" max="150" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="151" max="151" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="152" max="152" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="153" max="153" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="154" max="154" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="155" max="155" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="156" max="156" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="157" max="157" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="158" max="158" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="159" max="160" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="161" max="161" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="162" max="162" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="163" max="163" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="164" max="164" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="165" max="165" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="166" max="167" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="168" max="168" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="169" max="169" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="170" max="170" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="171" max="171" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="172" max="172" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="173" max="173" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="174" max="174" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="175" max="175" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="176" max="176" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="177" max="177" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="178" max="178" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="179" max="179" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="180" max="181" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="182" max="182" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="183" max="183" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="184" max="184" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="185" max="185" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="186" max="186" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="187" max="188" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="189" max="189" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="190" max="190" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="191" max="191" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="192" max="192" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="193" max="193" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="194" max="194" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="195" max="195" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="196" max="196" width="21.875" style="8" customWidth="1" collapsed="1"/>
-    <col min="197" max="197" width="14.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="198" max="198" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="199" max="199" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="200" max="200" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="201" max="202" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="203" max="203" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="204" max="204" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="205" max="205" width="15.25" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="206" max="206" width="14.125" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="207" max="207" width="9.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="208" max="209" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="210" max="210" width="11.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="211" max="211" width="12.375" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="212" max="212" width="15.625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="213" max="213" width="12.25" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="214" max="214" width="17.375" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="215" max="215" width="14.75" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="216" max="216" width="15.875" style="8" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="217" max="217" width="9" style="8" collapsed="1"/>
-    <col min="218" max="16384" width="9" style="8"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="70" max="70" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="72" max="72" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="74" max="74" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="75" max="76" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="77" max="77" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="78" max="78" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="79" max="79" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="80" max="80" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="81" max="81" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="82" max="83" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="84" max="84" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="85" max="85" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="86" max="86" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="88" max="88" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="89" max="89" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="90" max="90" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="91" max="91" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="92" max="92" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="93" max="93" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="94" max="94" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="95" max="95" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="96" max="97" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="98" max="98" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="99" max="99" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="100" max="100" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="101" max="101" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="102" max="102" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="103" max="104" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="105" max="105" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="106" max="106" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="107" max="107" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="108" max="108" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="109" max="109" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="110" max="110" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="111" max="111" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="112" max="112" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="113" max="113" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="114" max="114" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="115" max="115" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="116" max="116" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="117" max="118" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="119" max="119" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="120" max="120" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="121" max="121" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="122" max="122" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="123" max="123" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="124" max="125" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="126" max="126" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="127" max="127" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="128" max="128" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="129" max="129" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="130" max="130" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="131" max="131" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="132" max="132" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="133" max="133" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="134" max="134" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="135" max="135" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="136" max="136" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="137" max="137" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="138" max="139" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="140" max="140" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="141" max="141" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="142" max="142" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="143" max="143" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="144" max="144" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="145" max="146" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="147" max="147" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="148" max="148" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="149" max="149" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="150" max="150" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="151" max="151" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="152" max="152" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="153" max="153" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="154" max="154" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="155" max="155" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="156" max="156" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="157" max="157" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="158" max="158" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="159" max="160" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="161" max="161" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="162" max="162" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="163" max="163" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="164" max="164" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="165" max="165" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="166" max="167" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="168" max="168" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="169" max="169" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="170" max="170" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="171" max="171" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="172" max="172" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="173" max="173" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="174" max="174" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="175" max="175" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="176" max="176" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="177" max="177" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="178" max="178" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="179" max="179" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="180" max="181" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="182" max="182" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="183" max="183" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="184" max="184" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="185" max="185" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="186" max="186" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="187" max="188" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="189" max="189" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="190" max="190" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="191" max="191" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="192" max="192" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="193" max="193" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="194" max="194" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="195" max="195" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="196" max="196" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="197" max="197" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="198" max="198" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="199" max="199" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="200" max="200" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="201" max="202" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="203" max="203" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="204" max="204" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="205" max="205" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="206" max="206" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="207" max="207" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="208" max="209" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="210" max="210" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="211" max="211" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="212" max="212" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="213" max="213" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="214" max="214" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="215" max="215" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="216" max="216" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="217" max="217" width="9" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="I1" s="13" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="I1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13" t="s">
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AD1" s="13" t="s">
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AD1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13" t="s">
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13" t="s">
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="14"/>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
-      <c r="AY1" s="13" t="s">
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AY1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BB1" s="13"/>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="13"/>
-      <c r="BE1" s="13"/>
-      <c r="BF1" s="13" t="s">
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="BG1" s="13"/>
-      <c r="BH1" s="13"/>
-      <c r="BI1" s="13"/>
-      <c r="BJ1" s="13"/>
-      <c r="BK1" s="13"/>
-      <c r="BL1" s="13"/>
-      <c r="BM1" s="13" t="s">
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11"/>
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="BN1" s="14"/>
-      <c r="BO1" s="14"/>
-      <c r="BP1" s="14"/>
-      <c r="BQ1" s="14"/>
-      <c r="BT1" s="13" t="s">
+      <c r="BN1" s="12"/>
+      <c r="BO1" s="12"/>
+      <c r="BP1" s="12"/>
+      <c r="BQ1" s="12"/>
+      <c r="BT1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="BU1" s="13"/>
-      <c r="BV1" s="13"/>
-      <c r="BW1" s="13"/>
-      <c r="BX1" s="13"/>
-      <c r="BY1" s="13"/>
-      <c r="BZ1" s="13"/>
-      <c r="CA1" s="13" t="s">
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11"/>
+      <c r="BW1" s="11"/>
+      <c r="BX1" s="11"/>
+      <c r="BY1" s="11"/>
+      <c r="BZ1" s="11"/>
+      <c r="CA1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="CB1" s="13"/>
-      <c r="CC1" s="13"/>
-      <c r="CD1" s="13"/>
-      <c r="CE1" s="13"/>
-      <c r="CF1" s="13"/>
-      <c r="CG1" s="13"/>
-      <c r="CH1" s="13" t="s">
+      <c r="CB1" s="11"/>
+      <c r="CC1" s="11"/>
+      <c r="CD1" s="11"/>
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="CI1" s="14"/>
-      <c r="CJ1" s="14"/>
-      <c r="CK1" s="14"/>
-      <c r="CL1" s="14"/>
-      <c r="CO1" s="13" t="s">
+      <c r="CI1" s="12"/>
+      <c r="CJ1" s="12"/>
+      <c r="CK1" s="12"/>
+      <c r="CL1" s="12"/>
+      <c r="CO1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="CP1" s="13"/>
-      <c r="CQ1" s="13"/>
-      <c r="CR1" s="13"/>
-      <c r="CS1" s="13"/>
-      <c r="CT1" s="13"/>
-      <c r="CU1" s="13"/>
-      <c r="CV1" s="13" t="s">
+      <c r="CP1" s="11"/>
+      <c r="CQ1" s="11"/>
+      <c r="CR1" s="11"/>
+      <c r="CS1" s="11"/>
+      <c r="CT1" s="11"/>
+      <c r="CU1" s="11"/>
+      <c r="CV1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="CW1" s="13"/>
-      <c r="CX1" s="13"/>
-      <c r="CY1" s="13"/>
-      <c r="CZ1" s="13"/>
-      <c r="DA1" s="13"/>
-      <c r="DB1" s="13"/>
-      <c r="DC1" s="13" t="s">
+      <c r="CW1" s="11"/>
+      <c r="CX1" s="11"/>
+      <c r="CY1" s="11"/>
+      <c r="CZ1" s="11"/>
+      <c r="DA1" s="11"/>
+      <c r="DB1" s="11"/>
+      <c r="DC1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="DD1" s="14"/>
-      <c r="DE1" s="14"/>
-      <c r="DF1" s="14"/>
-      <c r="DG1" s="14"/>
-      <c r="DJ1" s="13" t="s">
+      <c r="DD1" s="12"/>
+      <c r="DE1" s="12"/>
+      <c r="DF1" s="12"/>
+      <c r="DG1" s="12"/>
+      <c r="DJ1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="DK1" s="13"/>
-      <c r="DL1" s="13"/>
-      <c r="DM1" s="13"/>
-      <c r="DN1" s="13"/>
-      <c r="DO1" s="13"/>
-      <c r="DP1" s="13"/>
-      <c r="DQ1" s="13" t="s">
+      <c r="DK1" s="11"/>
+      <c r="DL1" s="11"/>
+      <c r="DM1" s="11"/>
+      <c r="DN1" s="11"/>
+      <c r="DO1" s="11"/>
+      <c r="DP1" s="11"/>
+      <c r="DQ1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="DR1" s="13"/>
-      <c r="DS1" s="13"/>
-      <c r="DT1" s="13"/>
-      <c r="DU1" s="13"/>
-      <c r="DV1" s="13"/>
-      <c r="DW1" s="13"/>
-      <c r="DX1" s="13" t="s">
+      <c r="DR1" s="11"/>
+      <c r="DS1" s="11"/>
+      <c r="DT1" s="11"/>
+      <c r="DU1" s="11"/>
+      <c r="DV1" s="11"/>
+      <c r="DW1" s="11"/>
+      <c r="DX1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="DY1" s="14"/>
-      <c r="DZ1" s="14"/>
-      <c r="EA1" s="14"/>
-      <c r="EB1" s="14"/>
-      <c r="EE1" s="13" t="s">
+      <c r="DY1" s="12"/>
+      <c r="DZ1" s="12"/>
+      <c r="EA1" s="12"/>
+      <c r="EB1" s="12"/>
+      <c r="EE1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="EF1" s="13"/>
-      <c r="EG1" s="13"/>
-      <c r="EH1" s="13"/>
-      <c r="EI1" s="13"/>
-      <c r="EJ1" s="13"/>
-      <c r="EK1" s="13"/>
-      <c r="EL1" s="13" t="s">
+      <c r="EF1" s="11"/>
+      <c r="EG1" s="11"/>
+      <c r="EH1" s="11"/>
+      <c r="EI1" s="11"/>
+      <c r="EJ1" s="11"/>
+      <c r="EK1" s="11"/>
+      <c r="EL1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="EM1" s="13"/>
-      <c r="EN1" s="13"/>
-      <c r="EO1" s="13"/>
-      <c r="EP1" s="13"/>
-      <c r="EQ1" s="13"/>
-      <c r="ER1" s="13"/>
-      <c r="ES1" s="13" t="s">
+      <c r="EM1" s="11"/>
+      <c r="EN1" s="11"/>
+      <c r="EO1" s="11"/>
+      <c r="EP1" s="11"/>
+      <c r="EQ1" s="11"/>
+      <c r="ER1" s="11"/>
+      <c r="ES1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="ET1" s="14"/>
-      <c r="EU1" s="14"/>
-      <c r="EV1" s="14"/>
-      <c r="EW1" s="14"/>
-      <c r="EZ1" s="13" t="s">
+      <c r="ET1" s="12"/>
+      <c r="EU1" s="12"/>
+      <c r="EV1" s="12"/>
+      <c r="EW1" s="12"/>
+      <c r="EZ1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="FA1" s="13"/>
-      <c r="FB1" s="13"/>
-      <c r="FC1" s="13"/>
-      <c r="FD1" s="13"/>
-      <c r="FE1" s="13"/>
-      <c r="FF1" s="13"/>
-      <c r="FG1" s="13" t="s">
+      <c r="FA1" s="11"/>
+      <c r="FB1" s="11"/>
+      <c r="FC1" s="11"/>
+      <c r="FD1" s="11"/>
+      <c r="FE1" s="11"/>
+      <c r="FF1" s="11"/>
+      <c r="FG1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="FH1" s="13"/>
-      <c r="FI1" s="13"/>
-      <c r="FJ1" s="13"/>
-      <c r="FK1" s="13"/>
-      <c r="FL1" s="13"/>
-      <c r="FM1" s="13"/>
-      <c r="FN1" s="13" t="s">
+      <c r="FH1" s="11"/>
+      <c r="FI1" s="11"/>
+      <c r="FJ1" s="11"/>
+      <c r="FK1" s="11"/>
+      <c r="FL1" s="11"/>
+      <c r="FM1" s="11"/>
+      <c r="FN1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="FO1" s="14"/>
-      <c r="FP1" s="14"/>
-      <c r="FQ1" s="14"/>
-      <c r="FR1" s="14"/>
-      <c r="FU1" s="13" t="s">
+      <c r="FO1" s="12"/>
+      <c r="FP1" s="12"/>
+      <c r="FQ1" s="12"/>
+      <c r="FR1" s="12"/>
+      <c r="FU1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="FV1" s="13"/>
-      <c r="FW1" s="13"/>
-      <c r="FX1" s="13"/>
-      <c r="FY1" s="13"/>
-      <c r="FZ1" s="13"/>
-      <c r="GA1" s="13"/>
-      <c r="GB1" s="13" t="s">
+      <c r="FV1" s="11"/>
+      <c r="FW1" s="11"/>
+      <c r="FX1" s="11"/>
+      <c r="FY1" s="11"/>
+      <c r="FZ1" s="11"/>
+      <c r="GA1" s="11"/>
+      <c r="GB1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="GC1" s="13"/>
-      <c r="GD1" s="13"/>
-      <c r="GE1" s="13"/>
-      <c r="GF1" s="13"/>
-      <c r="GG1" s="13"/>
-      <c r="GH1" s="13"/>
-      <c r="GI1" s="13" t="s">
+      <c r="GC1" s="11"/>
+      <c r="GD1" s="11"/>
+      <c r="GE1" s="11"/>
+      <c r="GF1" s="11"/>
+      <c r="GG1" s="11"/>
+      <c r="GH1" s="11"/>
+      <c r="GI1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="GJ1" s="14"/>
-      <c r="GK1" s="14"/>
-      <c r="GL1" s="14"/>
-      <c r="GM1" s="14"/>
-      <c r="GP1" s="13" t="s">
+      <c r="GJ1" s="12"/>
+      <c r="GK1" s="12"/>
+      <c r="GL1" s="12"/>
+      <c r="GM1" s="12"/>
+      <c r="GP1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="GQ1" s="13"/>
-      <c r="GR1" s="13"/>
-      <c r="GS1" s="13"/>
-      <c r="GT1" s="13"/>
-      <c r="GU1" s="13"/>
-      <c r="GV1" s="13"/>
-      <c r="GW1" s="13" t="s">
+      <c r="GQ1" s="11"/>
+      <c r="GR1" s="11"/>
+      <c r="GS1" s="11"/>
+      <c r="GT1" s="11"/>
+      <c r="GU1" s="11"/>
+      <c r="GV1" s="11"/>
+      <c r="GW1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="GX1" s="13"/>
-      <c r="GY1" s="13"/>
-      <c r="GZ1" s="13"/>
-      <c r="HA1" s="13"/>
-      <c r="HB1" s="13"/>
-      <c r="HC1" s="13"/>
-      <c r="HD1" s="13" t="s">
+      <c r="GX1" s="11"/>
+      <c r="GY1" s="11"/>
+      <c r="GZ1" s="11"/>
+      <c r="HA1" s="11"/>
+      <c r="HB1" s="11"/>
+      <c r="HC1" s="11"/>
+      <c r="HD1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="HE1" s="14"/>
-      <c r="HF1" s="14"/>
-      <c r="HG1" s="14"/>
-      <c r="HH1" s="14"/>
+      <c r="HE1" s="12"/>
+      <c r="HF1" s="12"/>
+      <c r="HG1" s="12"/>
+      <c r="HH1" s="12"/>
     </row>
     <row r="2" spans="1:216" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -22324,13 +22753,15 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="HD1:HH1"/>
-    <mergeCell ref="FN1:FR1"/>
-    <mergeCell ref="FU1:GA1"/>
-    <mergeCell ref="GB1:GH1"/>
-    <mergeCell ref="GI1:GM1"/>
-    <mergeCell ref="GP1:GV1"/>
-    <mergeCell ref="GW1:HC1"/>
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="AY1:BE1"/>
+    <mergeCell ref="BF1:BL1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AD1:AJ1"/>
+    <mergeCell ref="AK1:AQ1"/>
     <mergeCell ref="FG1:FM1"/>
     <mergeCell ref="CH1:CL1"/>
     <mergeCell ref="CO1:CU1"/>
@@ -22343,19 +22774,18 @@
     <mergeCell ref="EL1:ER1"/>
     <mergeCell ref="ES1:EW1"/>
     <mergeCell ref="EZ1:FF1"/>
-    <mergeCell ref="CA1:CG1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AD1:AJ1"/>
-    <mergeCell ref="AK1:AQ1"/>
-    <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="AY1:BE1"/>
-    <mergeCell ref="BF1:BL1"/>
     <mergeCell ref="BM1:BQ1"/>
     <mergeCell ref="BT1:BZ1"/>
+    <mergeCell ref="CA1:CG1"/>
+    <mergeCell ref="HD1:HH1"/>
+    <mergeCell ref="FN1:FR1"/>
+    <mergeCell ref="FU1:GA1"/>
+    <mergeCell ref="GB1:GH1"/>
+    <mergeCell ref="GI1:GM1"/>
+    <mergeCell ref="GP1:GV1"/>
+    <mergeCell ref="GW1:HC1"/>
   </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Uploading a cleaned results spreadsheet.
</commit_message>
<xml_diff>
--- a/Results/Mixed Bag Solver Puzzle Results.xlsx
+++ b/Results/Mixed Bag Solver Puzzle Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="165" windowWidth="27960" windowHeight="12540" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="165" windowWidth="27960" windowHeight="12540" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cho Best Buddies" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="133">
   <si>
     <t>Solver Type</t>
   </si>
@@ -412,6 +412,15 @@
   </si>
   <si>
     <t>pomeranz_805_10 | pomeranz_805_17</t>
+  </si>
+  <si>
+    <t>pomeranz_805_5 | pomeranz_805_8 | pomeranz_805_16</t>
+  </si>
+  <si>
+    <t>pomeranz_805_4 | pomeranz_805_5 | pomeranz_805_13</t>
+  </si>
+  <si>
+    <t>pomeranz_805_2 | pomeranz_805_10 | pomeranz_805_20</t>
   </si>
 </sst>
 </file>
@@ -977,7 +986,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="36" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1019,6 +1028,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="43">
@@ -3199,8 +3210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:AV44"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -6723,7 +6734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A65" sqref="A65:XFD66"/>
     </sheetView>
   </sheetViews>
@@ -17858,10 +17869,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR12"/>
+  <dimension ref="A1:BR17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -20314,6 +20325,1051 @@
       </c>
       <c r="BQ12" s="5">
         <v>3212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>-1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <v>805</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <v>805</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q13">
+        <v>805</v>
+      </c>
+      <c r="R13">
+        <v>2.6086956521700001E-2</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0.97391304347800001</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13" t="s">
+        <v>11</v>
+      </c>
+      <c r="X13">
+        <v>805</v>
+      </c>
+      <c r="Y13">
+        <v>0.91956521739099994</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC13">
+        <v>805</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE13">
+        <v>811</v>
+      </c>
+      <c r="AF13">
+        <v>0.99260172626400001</v>
+      </c>
+      <c r="AG13">
+        <v>7.3982737361300002E-3</v>
+      </c>
+      <c r="AH13">
+        <v>0</v>
+      </c>
+      <c r="AI13">
+        <v>0</v>
+      </c>
+      <c r="AJ13">
+        <v>0</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL13">
+        <v>811</v>
+      </c>
+      <c r="AM13">
+        <v>0.99260172626400001</v>
+      </c>
+      <c r="AN13">
+        <v>7.3982737361300002E-3</v>
+      </c>
+      <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>0</v>
+      </c>
+      <c r="AQ13">
+        <v>0</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS13">
+        <v>829</v>
+      </c>
+      <c r="AT13">
+        <v>0.97014475271400002</v>
+      </c>
+      <c r="AU13">
+        <v>0</v>
+      </c>
+      <c r="AV13">
+        <v>24</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX13">
+        <v>805</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AZ13">
+        <v>805</v>
+      </c>
+      <c r="BA13">
+        <v>0</v>
+      </c>
+      <c r="BB13">
+        <v>0</v>
+      </c>
+      <c r="BC13">
+        <v>0.90931677018599999</v>
+      </c>
+      <c r="BD13">
+        <v>1.2422360248399999E-3</v>
+      </c>
+      <c r="BE13">
+        <v>72</v>
+      </c>
+      <c r="BF13" t="s">
+        <v>13</v>
+      </c>
+      <c r="BG13">
+        <v>805</v>
+      </c>
+      <c r="BH13">
+        <v>0.70683229813699999</v>
+      </c>
+      <c r="BI13">
+        <v>0</v>
+      </c>
+      <c r="BJ13">
+        <v>0.2</v>
+      </c>
+      <c r="BK13">
+        <v>3.7267080745299998E-3</v>
+      </c>
+      <c r="BL13">
+        <v>72</v>
+      </c>
+      <c r="BM13" t="s">
+        <v>14</v>
+      </c>
+      <c r="BN13">
+        <v>733</v>
+      </c>
+      <c r="BO13">
+        <v>0.75931677018599997</v>
+      </c>
+      <c r="BP13">
+        <v>72</v>
+      </c>
+      <c r="BQ13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14">
+        <v>805</v>
+      </c>
+      <c r="I14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J14">
+        <v>1582</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0.49115044247799999</v>
+      </c>
+      <c r="M14">
+        <v>0.49873577749699999</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>16</v>
+      </c>
+      <c r="P14" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q14">
+        <v>1582</v>
+      </c>
+      <c r="R14">
+        <v>1.201011378E-2</v>
+      </c>
+      <c r="S14">
+        <v>0.49115044247799999</v>
+      </c>
+      <c r="T14">
+        <v>0.48672566371699999</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>16</v>
+      </c>
+      <c r="W14" t="s">
+        <v>53</v>
+      </c>
+      <c r="X14">
+        <v>3897</v>
+      </c>
+      <c r="Y14">
+        <v>0.184065934066</v>
+      </c>
+      <c r="Z14">
+        <v>16</v>
+      </c>
+      <c r="AA14">
+        <v>3108</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC14">
+        <v>805</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE14">
+        <v>828</v>
+      </c>
+      <c r="AF14">
+        <v>0.95289855072499996</v>
+      </c>
+      <c r="AG14">
+        <v>2.7777777777800002E-2</v>
+      </c>
+      <c r="AH14">
+        <v>1.93236714976E-2</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL14">
+        <v>828</v>
+      </c>
+      <c r="AM14">
+        <v>0.95289855072499996</v>
+      </c>
+      <c r="AN14">
+        <v>2.7777777777800002E-2</v>
+      </c>
+      <c r="AO14">
+        <v>1.93236714976E-2</v>
+      </c>
+      <c r="AP14">
+        <v>0</v>
+      </c>
+      <c r="AQ14">
+        <v>0</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS14">
+        <v>897</v>
+      </c>
+      <c r="AT14">
+        <v>0.88628762541799999</v>
+      </c>
+      <c r="AU14">
+        <v>0</v>
+      </c>
+      <c r="AV14">
+        <v>92</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX14">
+        <v>805</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AZ14">
+        <v>1594</v>
+      </c>
+      <c r="BA14">
+        <v>0</v>
+      </c>
+      <c r="BB14">
+        <v>0.49498117942300002</v>
+      </c>
+      <c r="BC14">
+        <v>0.487452948557</v>
+      </c>
+      <c r="BD14">
+        <v>0</v>
+      </c>
+      <c r="BE14">
+        <v>28</v>
+      </c>
+      <c r="BF14" t="s">
+        <v>52</v>
+      </c>
+      <c r="BG14">
+        <v>1594</v>
+      </c>
+      <c r="BH14">
+        <v>0</v>
+      </c>
+      <c r="BI14">
+        <v>0.49498117942300002</v>
+      </c>
+      <c r="BJ14">
+        <v>0.487452948557</v>
+      </c>
+      <c r="BK14">
+        <v>0</v>
+      </c>
+      <c r="BL14">
+        <v>28</v>
+      </c>
+      <c r="BM14" t="s">
+        <v>53</v>
+      </c>
+      <c r="BN14">
+        <v>3933</v>
+      </c>
+      <c r="BO14">
+        <v>0.15709416813900001</v>
+      </c>
+      <c r="BP14">
+        <v>28</v>
+      </c>
+      <c r="BQ14">
+        <v>3156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="18">
+        <v>2</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="18">
+        <v>3</v>
+      </c>
+      <c r="E15" s="18">
+        <v>4</v>
+      </c>
+      <c r="F15" s="18">
+        <v>-1</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="18">
+        <v>805</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="J15" s="18">
+        <v>808</v>
+      </c>
+      <c r="K15" s="18">
+        <v>0</v>
+      </c>
+      <c r="L15" s="18">
+        <v>3.7128712871299999E-3</v>
+      </c>
+      <c r="M15" s="18">
+        <v>0.99504950495</v>
+      </c>
+      <c r="N15" s="18">
+        <v>0</v>
+      </c>
+      <c r="O15" s="18">
+        <v>1</v>
+      </c>
+      <c r="P15" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q15" s="18">
+        <v>808</v>
+      </c>
+      <c r="R15" s="18">
+        <v>0.412128712871</v>
+      </c>
+      <c r="S15" s="18">
+        <v>3.7128712871299999E-3</v>
+      </c>
+      <c r="T15" s="18">
+        <v>0.57920792079200001</v>
+      </c>
+      <c r="U15" s="18">
+        <v>3.7128712871299999E-3</v>
+      </c>
+      <c r="V15" s="18">
+        <v>1</v>
+      </c>
+      <c r="W15" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="X15" s="18">
+        <v>816</v>
+      </c>
+      <c r="Y15" s="18">
+        <v>0.70287637698899996</v>
+      </c>
+      <c r="Z15" s="18">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="18">
+        <v>12</v>
+      </c>
+      <c r="AB15" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC15" s="18">
+        <v>805</v>
+      </c>
+      <c r="AD15" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE15" s="18">
+        <v>805</v>
+      </c>
+      <c r="AF15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="18">
+        <v>0.99503105590100005</v>
+      </c>
+      <c r="AI15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="18">
+        <v>4</v>
+      </c>
+      <c r="AK15" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL15" s="18">
+        <v>805</v>
+      </c>
+      <c r="AM15" s="18">
+        <v>0.83229813664600005</v>
+      </c>
+      <c r="AN15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO15" s="18">
+        <v>0.162732919255</v>
+      </c>
+      <c r="AP15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="18">
+        <v>4</v>
+      </c>
+      <c r="AR15" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS15" s="18">
+        <v>801</v>
+      </c>
+      <c r="AT15" s="18">
+        <v>0.90745341614899999</v>
+      </c>
+      <c r="AU15" s="18">
+        <v>4</v>
+      </c>
+      <c r="AV15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AW15" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX15" s="18">
+        <v>805</v>
+      </c>
+      <c r="AY15" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="AZ15" s="18">
+        <v>807</v>
+      </c>
+      <c r="BA15" s="18">
+        <v>0</v>
+      </c>
+      <c r="BB15" s="18">
+        <v>2.4783147459699999E-3</v>
+      </c>
+      <c r="BC15" s="18">
+        <v>0.88847583643100003</v>
+      </c>
+      <c r="BD15" s="18">
+        <v>0</v>
+      </c>
+      <c r="BE15" s="18">
+        <v>88</v>
+      </c>
+      <c r="BF15" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="BG15" s="18">
+        <v>807</v>
+      </c>
+      <c r="BH15" s="18">
+        <v>0.85006195786899996</v>
+      </c>
+      <c r="BI15" s="18">
+        <v>2.4783147459699999E-3</v>
+      </c>
+      <c r="BJ15" s="18">
+        <v>3.84138785626E-2</v>
+      </c>
+      <c r="BK15" s="18">
+        <v>0</v>
+      </c>
+      <c r="BL15" s="18">
+        <v>88</v>
+      </c>
+      <c r="BM15" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="BN15" s="18">
+        <v>725</v>
+      </c>
+      <c r="BO15" s="18">
+        <v>0.85485854858499999</v>
+      </c>
+      <c r="BP15" s="18">
+        <v>88</v>
+      </c>
+      <c r="BQ15" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="19">
+        <v>2</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="19">
+        <v>3</v>
+      </c>
+      <c r="E16" s="19">
+        <v>4</v>
+      </c>
+      <c r="F16" s="19">
+        <v>-1</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="19">
+        <v>805</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" s="19">
+        <v>805</v>
+      </c>
+      <c r="K16" s="19">
+        <v>0</v>
+      </c>
+      <c r="L16" s="19">
+        <v>0</v>
+      </c>
+      <c r="M16" s="19">
+        <v>0.94409937888200002</v>
+      </c>
+      <c r="N16" s="19">
+        <v>0</v>
+      </c>
+      <c r="O16" s="19">
+        <v>45</v>
+      </c>
+      <c r="P16" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q16" s="19">
+        <v>805</v>
+      </c>
+      <c r="R16" s="19">
+        <v>0.85714285714299998</v>
+      </c>
+      <c r="S16" s="19">
+        <v>0</v>
+      </c>
+      <c r="T16" s="19">
+        <v>8.6956521739099998E-2</v>
+      </c>
+      <c r="U16" s="19">
+        <v>0</v>
+      </c>
+      <c r="V16" s="19">
+        <v>45</v>
+      </c>
+      <c r="W16" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="X16" s="19">
+        <v>760</v>
+      </c>
+      <c r="Y16" s="19">
+        <v>0.86739130434800005</v>
+      </c>
+      <c r="Z16" s="19">
+        <v>45</v>
+      </c>
+      <c r="AA16" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC16" s="19">
+        <v>805</v>
+      </c>
+      <c r="AD16" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE16" s="19">
+        <v>805</v>
+      </c>
+      <c r="AF16" s="19">
+        <v>1</v>
+      </c>
+      <c r="AG16" s="19">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="19">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="19">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="19">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL16" s="19">
+        <v>805</v>
+      </c>
+      <c r="AM16" s="19">
+        <v>1</v>
+      </c>
+      <c r="AN16" s="19">
+        <v>0</v>
+      </c>
+      <c r="AO16" s="19">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="19">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="19">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS16" s="19">
+        <v>805</v>
+      </c>
+      <c r="AT16" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU16" s="19">
+        <v>0</v>
+      </c>
+      <c r="AV16" s="19">
+        <v>0</v>
+      </c>
+      <c r="AW16" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX16" s="19">
+        <v>805</v>
+      </c>
+      <c r="AY16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="AZ16" s="19">
+        <v>829</v>
+      </c>
+      <c r="BA16" s="19">
+        <v>0</v>
+      </c>
+      <c r="BB16" s="19">
+        <v>2.8950542822700001E-2</v>
+      </c>
+      <c r="BC16" s="19">
+        <v>0.73703256936100003</v>
+      </c>
+      <c r="BD16" s="19">
+        <v>0</v>
+      </c>
+      <c r="BE16" s="19">
+        <v>194</v>
+      </c>
+      <c r="BF16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="BG16" s="19">
+        <v>829</v>
+      </c>
+      <c r="BH16" s="19">
+        <v>0.73703256936100003</v>
+      </c>
+      <c r="BI16" s="19">
+        <v>2.8950542822700001E-2</v>
+      </c>
+      <c r="BJ16" s="19">
+        <v>0</v>
+      </c>
+      <c r="BK16" s="19">
+        <v>0</v>
+      </c>
+      <c r="BL16" s="19">
+        <v>194</v>
+      </c>
+      <c r="BM16" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="BN16" s="19">
+        <v>707</v>
+      </c>
+      <c r="BO16" s="19">
+        <v>0.66259711431699997</v>
+      </c>
+      <c r="BP16" s="19">
+        <v>194</v>
+      </c>
+      <c r="BQ16" s="19">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="19">
+        <v>2</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="19">
+        <v>3</v>
+      </c>
+      <c r="E17" s="19">
+        <v>3</v>
+      </c>
+      <c r="F17" s="19">
+        <v>0</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="19">
+        <v>805</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" s="19">
+        <v>2173</v>
+      </c>
+      <c r="K17" s="19">
+        <v>0</v>
+      </c>
+      <c r="L17" s="19">
+        <v>0.62954440865200001</v>
+      </c>
+      <c r="M17" s="19">
+        <v>0.354348826507</v>
+      </c>
+      <c r="N17" s="19">
+        <v>0</v>
+      </c>
+      <c r="O17" s="19">
+        <v>35</v>
+      </c>
+      <c r="P17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q17" s="19">
+        <v>2173</v>
+      </c>
+      <c r="R17" s="19">
+        <v>0.31753336401299997</v>
+      </c>
+      <c r="S17" s="19">
+        <v>0.62954440865200001</v>
+      </c>
+      <c r="T17" s="19">
+        <v>3.6815462494200001E-2</v>
+      </c>
+      <c r="U17" s="19">
+        <v>0</v>
+      </c>
+      <c r="V17" s="19">
+        <v>35</v>
+      </c>
+      <c r="W17" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="X17" s="19">
+        <v>6242</v>
+      </c>
+      <c r="Y17" s="19">
+        <v>0.110602198502</v>
+      </c>
+      <c r="Z17" s="19">
+        <v>35</v>
+      </c>
+      <c r="AA17" s="19">
+        <v>5472</v>
+      </c>
+      <c r="AB17" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC17" s="19">
+        <v>805</v>
+      </c>
+      <c r="AD17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE17" s="19">
+        <v>2138</v>
+      </c>
+      <c r="AF17" s="19">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="19">
+        <v>0.62347988774600005</v>
+      </c>
+      <c r="AH17" s="19">
+        <v>0.37652011225400001</v>
+      </c>
+      <c r="AI17" s="19">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="19">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL17" s="19">
+        <v>2138</v>
+      </c>
+      <c r="AM17" s="19">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="19">
+        <v>0.62347988774600005</v>
+      </c>
+      <c r="AO17" s="19">
+        <v>0.37652011225400001</v>
+      </c>
+      <c r="AP17" s="19">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="19">
+        <v>0</v>
+      </c>
+      <c r="AR17" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS17" s="19">
+        <v>6137</v>
+      </c>
+      <c r="AT17" s="19">
+        <v>0.13072348052800001</v>
+      </c>
+      <c r="AU17" s="19">
+        <v>0</v>
+      </c>
+      <c r="AV17" s="19">
+        <v>5332</v>
+      </c>
+      <c r="AW17" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX17" s="19">
+        <v>805</v>
+      </c>
+      <c r="AY17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AZ17" s="19">
+        <v>2380</v>
+      </c>
+      <c r="BA17" s="19">
+        <v>0</v>
+      </c>
+      <c r="BB17" s="19">
+        <v>0.66176470588199998</v>
+      </c>
+      <c r="BC17" s="19">
+        <v>0.236554621849</v>
+      </c>
+      <c r="BD17" s="19">
+        <v>0</v>
+      </c>
+      <c r="BE17" s="19">
+        <v>242</v>
+      </c>
+      <c r="BF17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="BG17" s="19">
+        <v>2380</v>
+      </c>
+      <c r="BH17" s="19">
+        <v>0</v>
+      </c>
+      <c r="BI17" s="19">
+        <v>0.66176470588199998</v>
+      </c>
+      <c r="BJ17" s="19">
+        <v>0.236554621849</v>
+      </c>
+      <c r="BK17" s="19">
+        <v>0</v>
+      </c>
+      <c r="BL17" s="19">
+        <v>242</v>
+      </c>
+      <c r="BM17" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="BN17" s="19">
+        <v>286</v>
+      </c>
+      <c r="BO17" s="19">
+        <v>0.18088071348900001</v>
+      </c>
+      <c r="BP17" s="19">
+        <v>611</v>
+      </c>
+      <c r="BQ17" s="19">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploading more two puzzle solved results.
</commit_message>
<xml_diff>
--- a/Results/Mixed Bag Solver Puzzle Results.xlsx
+++ b/Results/Mixed Bag Solver Puzzle Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="2745" windowWidth="27960" windowHeight="12540" activeTab="5"/>
+    <workbookView xWindow="2010" yWindow="2745" windowWidth="27960" windowHeight="12540" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cho Best Buddies" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2404" uniqueCount="149">
   <si>
     <t>Solver Type</t>
   </si>
@@ -442,6 +442,33 @@
   </si>
   <si>
     <t>pomeranz_805_4 | mcgill_540_5 | mcgill_540_13</t>
+  </si>
+  <si>
+    <t>pomeranz_805_9 | pomeranz_805_13</t>
+  </si>
+  <si>
+    <t>pomeranz_805_11 | pomeranz_805_17</t>
+  </si>
+  <si>
+    <t>pomeranz_805_4 | pomeranz_805_17</t>
+  </si>
+  <si>
+    <t>pomeranz_805_13 | pomeranz_805_17</t>
+  </si>
+  <si>
+    <t>pomeranz_805_4 | pomeranz_805_10</t>
+  </si>
+  <si>
+    <t>pomeranz_805_10 | pomeranz_805_19</t>
+  </si>
+  <si>
+    <t>pomeranz_805_3 | pomeranz_805_6</t>
+  </si>
+  <si>
+    <t>pomeranz_805_11 | pomeranz_805_18</t>
+  </si>
+  <si>
+    <t>pomeranz_805_8 | pomeranz_805_12</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1047,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="36" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1075,6 +1102,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -6776,10 +6804,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW88"/>
+  <dimension ref="A1:AW110"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -19072,7 +19100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:49" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>8</v>
       </c>
@@ -19658,6 +19686,3240 @@
         <v>4</v>
       </c>
       <c r="AW88" s="20"/>
+    </row>
+    <row r="89" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" s="5">
+        <v>2</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D89" s="5">
+        <v>2</v>
+      </c>
+      <c r="E89" s="5">
+        <v>2</v>
+      </c>
+      <c r="F89" s="5">
+        <v>0</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H89" s="5">
+        <v>805</v>
+      </c>
+      <c r="I89" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J89" s="5">
+        <v>805</v>
+      </c>
+      <c r="K89" s="5">
+        <v>0</v>
+      </c>
+      <c r="L89" s="5">
+        <v>0</v>
+      </c>
+      <c r="M89" s="5">
+        <v>1</v>
+      </c>
+      <c r="N89" s="5">
+        <v>0</v>
+      </c>
+      <c r="O89" s="5">
+        <v>0</v>
+      </c>
+      <c r="P89" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q89" s="5">
+        <v>805</v>
+      </c>
+      <c r="R89" s="5">
+        <v>0.79751552795000002</v>
+      </c>
+      <c r="S89" s="5">
+        <v>0</v>
+      </c>
+      <c r="T89" s="5">
+        <v>0.20124223602499999</v>
+      </c>
+      <c r="U89" s="5">
+        <v>1.2422360248399999E-3</v>
+      </c>
+      <c r="V89" s="5">
+        <v>0</v>
+      </c>
+      <c r="W89" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X89" s="5">
+        <v>805</v>
+      </c>
+      <c r="Y89" s="5">
+        <v>0.874223602484</v>
+      </c>
+      <c r="Z89" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA89" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB89" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC89" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD89" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE89" s="5">
+        <v>805</v>
+      </c>
+      <c r="AF89" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG89" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH89" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI89" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ89" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK89" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL89" s="5">
+        <v>805</v>
+      </c>
+      <c r="AM89" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN89" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO89" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP89" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ89" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR89" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS89" s="5">
+        <v>805</v>
+      </c>
+      <c r="AT89" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU89" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV89" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW89" s="24"/>
+    </row>
+    <row r="90" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" s="5">
+        <v>2</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D90" s="5">
+        <v>2</v>
+      </c>
+      <c r="E90" s="5">
+        <v>2</v>
+      </c>
+      <c r="F90" s="5">
+        <v>0</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H90" s="5">
+        <v>805</v>
+      </c>
+      <c r="I90" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J90" s="5">
+        <v>1204</v>
+      </c>
+      <c r="K90" s="5">
+        <v>0</v>
+      </c>
+      <c r="L90" s="5">
+        <v>0.331395348837</v>
+      </c>
+      <c r="M90" s="5">
+        <v>0.35631229235900003</v>
+      </c>
+      <c r="N90" s="5">
+        <v>0</v>
+      </c>
+      <c r="O90" s="5">
+        <v>376</v>
+      </c>
+      <c r="P90" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q90" s="5">
+        <v>1211</v>
+      </c>
+      <c r="R90" s="5">
+        <v>0.30305532617699998</v>
+      </c>
+      <c r="S90" s="5">
+        <v>0.33526011560699998</v>
+      </c>
+      <c r="T90" s="5">
+        <v>7.4318744838999997E-3</v>
+      </c>
+      <c r="U90" s="5">
+        <v>0</v>
+      </c>
+      <c r="V90" s="5">
+        <v>429</v>
+      </c>
+      <c r="W90" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X90" s="5">
+        <v>2000</v>
+      </c>
+      <c r="Y90" s="5">
+        <v>0.146562371346</v>
+      </c>
+      <c r="Z90" s="5">
+        <v>429</v>
+      </c>
+      <c r="AA90" s="5">
+        <v>1624</v>
+      </c>
+      <c r="AB90" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC90" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD90" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE90" s="5">
+        <v>1181</v>
+      </c>
+      <c r="AF90" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG90" s="5">
+        <v>0.31837425910200001</v>
+      </c>
+      <c r="AH90" s="5">
+        <v>0.34377646062700001</v>
+      </c>
+      <c r="AI90" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ90" s="5">
+        <v>399</v>
+      </c>
+      <c r="AK90" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL90" s="5">
+        <v>1181</v>
+      </c>
+      <c r="AM90" s="5">
+        <v>0.34377646062700001</v>
+      </c>
+      <c r="AN90" s="5">
+        <v>0.31837425910200001</v>
+      </c>
+      <c r="AO90" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP90" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ90" s="5">
+        <v>399</v>
+      </c>
+      <c r="AR90" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS90" s="5">
+        <v>1910</v>
+      </c>
+      <c r="AT90" s="5">
+        <v>0.16933737548700001</v>
+      </c>
+      <c r="AU90" s="5">
+        <v>399</v>
+      </c>
+      <c r="AV90" s="5">
+        <v>1504</v>
+      </c>
+      <c r="AW90" s="24"/>
+    </row>
+    <row r="91" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" s="5">
+        <v>2</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D91" s="5">
+        <v>2</v>
+      </c>
+      <c r="E91" s="5">
+        <v>2</v>
+      </c>
+      <c r="F91" s="5">
+        <v>0</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H91" s="5">
+        <v>805</v>
+      </c>
+      <c r="I91" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J91" s="5">
+        <v>805</v>
+      </c>
+      <c r="K91" s="5">
+        <v>4.9689440993800002E-3</v>
+      </c>
+      <c r="L91" s="5">
+        <v>0</v>
+      </c>
+      <c r="M91" s="5">
+        <v>0.96645962732900004</v>
+      </c>
+      <c r="N91" s="5">
+        <v>1.2422360248399999E-3</v>
+      </c>
+      <c r="O91" s="5">
+        <v>22</v>
+      </c>
+      <c r="P91" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q91" s="5">
+        <v>805</v>
+      </c>
+      <c r="R91" s="5">
+        <v>0.74409937888199995</v>
+      </c>
+      <c r="S91" s="5">
+        <v>0</v>
+      </c>
+      <c r="T91" s="5">
+        <v>0.22857142857099999</v>
+      </c>
+      <c r="U91" s="5">
+        <v>0</v>
+      </c>
+      <c r="V91" s="5">
+        <v>22</v>
+      </c>
+      <c r="W91" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X91" s="5">
+        <v>783</v>
+      </c>
+      <c r="Y91" s="5">
+        <v>0.77981366459599999</v>
+      </c>
+      <c r="Z91" s="5">
+        <v>22</v>
+      </c>
+      <c r="AA91" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB91" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC91" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD91" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE91" s="5">
+        <v>827</v>
+      </c>
+      <c r="AF91" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG91" s="5">
+        <v>2.6602176541699999E-2</v>
+      </c>
+      <c r="AH91" s="5">
+        <v>0.97339782345799997</v>
+      </c>
+      <c r="AI91" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ91" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK91" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL91" s="5">
+        <v>827</v>
+      </c>
+      <c r="AM91" s="5">
+        <v>0.97339782345799997</v>
+      </c>
+      <c r="AN91" s="5">
+        <v>2.6602176541699999E-2</v>
+      </c>
+      <c r="AO91" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP91" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ91" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR91" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS91" s="5">
+        <v>893</v>
+      </c>
+      <c r="AT91" s="5">
+        <v>0.89529675251999996</v>
+      </c>
+      <c r="AU91" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV91" s="5">
+        <v>88</v>
+      </c>
+      <c r="AW91" s="24"/>
+    </row>
+    <row r="92" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B92" s="5">
+        <v>2</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D92" s="5">
+        <v>2</v>
+      </c>
+      <c r="E92" s="5">
+        <v>2</v>
+      </c>
+      <c r="F92" s="5">
+        <v>0</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H92" s="5">
+        <v>805</v>
+      </c>
+      <c r="I92" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J92" s="5">
+        <v>1610</v>
+      </c>
+      <c r="K92" s="5">
+        <v>0</v>
+      </c>
+      <c r="L92" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="M92" s="5">
+        <v>0.394409937888</v>
+      </c>
+      <c r="N92" s="5">
+        <v>0</v>
+      </c>
+      <c r="O92" s="5">
+        <v>170</v>
+      </c>
+      <c r="P92" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q92" s="5">
+        <v>805</v>
+      </c>
+      <c r="R92" s="5">
+        <v>2.4844720496900001E-3</v>
+      </c>
+      <c r="S92" s="5">
+        <v>0</v>
+      </c>
+      <c r="T92" s="5">
+        <v>0.20869565217399999</v>
+      </c>
+      <c r="U92" s="5">
+        <v>0</v>
+      </c>
+      <c r="V92" s="5">
+        <v>635</v>
+      </c>
+      <c r="W92" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X92" s="5">
+        <v>3855</v>
+      </c>
+      <c r="Y92" s="5">
+        <v>0.13155279503100001</v>
+      </c>
+      <c r="Z92" s="5">
+        <v>170</v>
+      </c>
+      <c r="AA92" s="5">
+        <v>3220</v>
+      </c>
+      <c r="AB92" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC92" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD92" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE92" s="5">
+        <v>1440</v>
+      </c>
+      <c r="AF92" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG92" s="5">
+        <v>0.440972222222</v>
+      </c>
+      <c r="AH92" s="5">
+        <v>0.55902777777799995</v>
+      </c>
+      <c r="AI92" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ92" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK92" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL92" s="5">
+        <v>1440</v>
+      </c>
+      <c r="AM92" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN92" s="5">
+        <v>0.440972222222</v>
+      </c>
+      <c r="AO92" s="5">
+        <v>0.55902777777799995</v>
+      </c>
+      <c r="AP92" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ92" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR92" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS92" s="5">
+        <v>3345</v>
+      </c>
+      <c r="AT92" s="5">
+        <v>0.22683109118100001</v>
+      </c>
+      <c r="AU92" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV92" s="5">
+        <v>2540</v>
+      </c>
+      <c r="AW92" s="24"/>
+    </row>
+    <row r="93" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93" s="5">
+        <v>2</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D93" s="5">
+        <v>2</v>
+      </c>
+      <c r="E93" s="5">
+        <v>2</v>
+      </c>
+      <c r="F93" s="5">
+        <v>0</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H93" s="5">
+        <v>805</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J93" s="5">
+        <v>807</v>
+      </c>
+      <c r="K93" s="5">
+        <v>0</v>
+      </c>
+      <c r="L93" s="5">
+        <v>2.4783147459699999E-3</v>
+      </c>
+      <c r="M93" s="5">
+        <v>0.99752168525399998</v>
+      </c>
+      <c r="N93" s="5">
+        <v>0</v>
+      </c>
+      <c r="O93" s="5">
+        <v>0</v>
+      </c>
+      <c r="P93" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q93" s="5">
+        <v>807</v>
+      </c>
+      <c r="R93" s="5">
+        <v>0.93184634448600001</v>
+      </c>
+      <c r="S93" s="5">
+        <v>2.4783147459699999E-3</v>
+      </c>
+      <c r="T93" s="5">
+        <v>6.4436183395299995E-2</v>
+      </c>
+      <c r="U93" s="5">
+        <v>1.2391573729900001E-3</v>
+      </c>
+      <c r="V93" s="5">
+        <v>0</v>
+      </c>
+      <c r="W93" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X93" s="5">
+        <v>813</v>
+      </c>
+      <c r="Y93" s="5">
+        <v>0.95172201722000005</v>
+      </c>
+      <c r="Z93" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA93" s="5">
+        <v>8</v>
+      </c>
+      <c r="AB93" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC93" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD93" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE93" s="5">
+        <v>805</v>
+      </c>
+      <c r="AF93" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG93" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH93" s="5">
+        <v>0.99751552794999998</v>
+      </c>
+      <c r="AI93" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ93" s="5">
+        <v>2</v>
+      </c>
+      <c r="AK93" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL93" s="5">
+        <v>805</v>
+      </c>
+      <c r="AM93" s="5">
+        <v>0.79751552795000002</v>
+      </c>
+      <c r="AN93" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO93" s="5">
+        <v>0.198757763975</v>
+      </c>
+      <c r="AP93" s="5">
+        <v>1.2422360248399999E-3</v>
+      </c>
+      <c r="AQ93" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR93" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS93" s="5">
+        <v>803</v>
+      </c>
+      <c r="AT93" s="5">
+        <v>0.86956521739100001</v>
+      </c>
+      <c r="AU93" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV93" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW93" s="24"/>
+    </row>
+    <row r="94" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" s="5">
+        <v>2</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D94" s="5">
+        <v>2</v>
+      </c>
+      <c r="E94" s="5">
+        <v>2</v>
+      </c>
+      <c r="F94" s="5">
+        <v>0</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H94" s="5">
+        <v>805</v>
+      </c>
+      <c r="I94" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J94" s="5">
+        <v>811</v>
+      </c>
+      <c r="K94" s="5">
+        <v>0</v>
+      </c>
+      <c r="L94" s="5">
+        <v>7.3982737361300002E-3</v>
+      </c>
+      <c r="M94" s="5">
+        <v>0.82737361282400002</v>
+      </c>
+      <c r="N94" s="5">
+        <v>1.2330456226899999E-3</v>
+      </c>
+      <c r="O94" s="5">
+        <v>133</v>
+      </c>
+      <c r="P94" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q94" s="5">
+        <v>811</v>
+      </c>
+      <c r="R94" s="5">
+        <v>0.766954377312</v>
+      </c>
+      <c r="S94" s="5">
+        <v>7.3982737361300002E-3</v>
+      </c>
+      <c r="T94" s="5">
+        <v>6.0419235511699997E-2</v>
+      </c>
+      <c r="U94" s="5">
+        <v>1.2330456226899999E-3</v>
+      </c>
+      <c r="V94" s="5">
+        <v>133</v>
+      </c>
+      <c r="W94" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X94" s="5">
+        <v>696</v>
+      </c>
+      <c r="Y94" s="5">
+        <v>0.76417370325699996</v>
+      </c>
+      <c r="Z94" s="5">
+        <v>133</v>
+      </c>
+      <c r="AA94" s="5">
+        <v>24</v>
+      </c>
+      <c r="AB94" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC94" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD94" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE94" s="5">
+        <v>938</v>
+      </c>
+      <c r="AF94" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG94" s="5">
+        <v>0.14179104477599999</v>
+      </c>
+      <c r="AH94" s="5">
+        <v>0.85181236673799998</v>
+      </c>
+      <c r="AI94" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ94" s="5">
+        <v>6</v>
+      </c>
+      <c r="AK94" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL94" s="5">
+        <v>938</v>
+      </c>
+      <c r="AM94" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN94" s="5">
+        <v>0.14179104477599999</v>
+      </c>
+      <c r="AO94" s="5">
+        <v>0.85181236673799998</v>
+      </c>
+      <c r="AP94" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ94" s="5">
+        <v>6</v>
+      </c>
+      <c r="AR94" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS94" s="5">
+        <v>1331</v>
+      </c>
+      <c r="AT94" s="5">
+        <v>0.48597606581899999</v>
+      </c>
+      <c r="AU94" s="5">
+        <v>6</v>
+      </c>
+      <c r="AV94" s="5">
+        <v>532</v>
+      </c>
+      <c r="AW94" s="24"/>
+    </row>
+    <row r="95" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95" s="5">
+        <v>2</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D95" s="5">
+        <v>2</v>
+      </c>
+      <c r="E95" s="5">
+        <v>2</v>
+      </c>
+      <c r="F95" s="5">
+        <v>0</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H95" s="5">
+        <v>805</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J95" s="5">
+        <v>805</v>
+      </c>
+      <c r="K95" s="5">
+        <v>0.98633540372700002</v>
+      </c>
+      <c r="L95" s="5">
+        <v>0</v>
+      </c>
+      <c r="M95" s="5">
+        <v>9.9378881987600004E-3</v>
+      </c>
+      <c r="N95" s="5">
+        <v>0</v>
+      </c>
+      <c r="O95" s="5">
+        <v>3</v>
+      </c>
+      <c r="P95" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q95" s="5">
+        <v>805</v>
+      </c>
+      <c r="R95" s="5">
+        <v>0.98633540372700002</v>
+      </c>
+      <c r="S95" s="5">
+        <v>0</v>
+      </c>
+      <c r="T95" s="5">
+        <v>9.9378881987600004E-3</v>
+      </c>
+      <c r="U95" s="5">
+        <v>0</v>
+      </c>
+      <c r="V95" s="5">
+        <v>3</v>
+      </c>
+      <c r="W95" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X95" s="5">
+        <v>802</v>
+      </c>
+      <c r="Y95" s="5">
+        <v>0.97919254658400001</v>
+      </c>
+      <c r="Z95" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA95" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB95" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC95" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD95" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE95" s="5">
+        <v>808</v>
+      </c>
+      <c r="AF95" s="5">
+        <v>0.99381188118800001</v>
+      </c>
+      <c r="AG95" s="5">
+        <v>3.7128712871299999E-3</v>
+      </c>
+      <c r="AH95" s="5">
+        <v>2.4752475247499998E-3</v>
+      </c>
+      <c r="AI95" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ95" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK95" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL95" s="5">
+        <v>808</v>
+      </c>
+      <c r="AM95" s="5">
+        <v>0.99381188118800001</v>
+      </c>
+      <c r="AN95" s="5">
+        <v>3.7128712871299999E-3</v>
+      </c>
+      <c r="AO95" s="5">
+        <v>2.4752475247499998E-3</v>
+      </c>
+      <c r="AP95" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ95" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR95" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS95" s="5">
+        <v>817</v>
+      </c>
+      <c r="AT95" s="5">
+        <v>0.97949816401500001</v>
+      </c>
+      <c r="AU95" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV95" s="5">
+        <v>12</v>
+      </c>
+      <c r="AW95" s="24"/>
+    </row>
+    <row r="96" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96" s="5">
+        <v>2</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D96" s="5">
+        <v>2</v>
+      </c>
+      <c r="E96" s="5">
+        <v>2</v>
+      </c>
+      <c r="F96" s="5">
+        <v>0</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H96" s="5">
+        <v>805</v>
+      </c>
+      <c r="I96" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J96" s="5">
+        <v>1586</v>
+      </c>
+      <c r="K96" s="5">
+        <v>0.48297604035300001</v>
+      </c>
+      <c r="L96" s="5">
+        <v>0.49243379571200002</v>
+      </c>
+      <c r="M96" s="5">
+        <v>2.2698612862499998E-2</v>
+      </c>
+      <c r="N96" s="5">
+        <v>0</v>
+      </c>
+      <c r="O96" s="5">
+        <v>3</v>
+      </c>
+      <c r="P96" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q96" s="5">
+        <v>1586</v>
+      </c>
+      <c r="R96" s="5">
+        <v>0.48297604035300001</v>
+      </c>
+      <c r="S96" s="5">
+        <v>0.49243379571200002</v>
+      </c>
+      <c r="T96" s="5">
+        <v>2.2698612862499998E-2</v>
+      </c>
+      <c r="U96" s="5">
+        <v>0</v>
+      </c>
+      <c r="V96" s="5">
+        <v>3</v>
+      </c>
+      <c r="W96" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X96" s="5">
+        <v>3926</v>
+      </c>
+      <c r="Y96" s="5">
+        <v>0.19445151438</v>
+      </c>
+      <c r="Z96" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA96" s="5">
+        <v>3124</v>
+      </c>
+      <c r="AB96" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC96" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD96" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE96" s="5">
+        <v>1607</v>
+      </c>
+      <c r="AF96" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG96" s="5">
+        <v>0.49906658369599999</v>
+      </c>
+      <c r="AH96" s="5">
+        <v>0.48599875544499999</v>
+      </c>
+      <c r="AI96" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ96" s="5">
+        <v>24</v>
+      </c>
+      <c r="AK96" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL96" s="5">
+        <v>1607</v>
+      </c>
+      <c r="AM96" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN96" s="5">
+        <v>0.49906658369599999</v>
+      </c>
+      <c r="AO96" s="5">
+        <v>0.48599875544499999</v>
+      </c>
+      <c r="AP96" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ96" s="5">
+        <v>24</v>
+      </c>
+      <c r="AR96" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS96" s="5">
+        <v>3989</v>
+      </c>
+      <c r="AT96" s="5">
+        <v>0.18894841764299999</v>
+      </c>
+      <c r="AU96" s="5">
+        <v>24</v>
+      </c>
+      <c r="AV96" s="5">
+        <v>3208</v>
+      </c>
+      <c r="AW96" s="24"/>
+    </row>
+    <row r="97" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97" s="5">
+        <v>2</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D97" s="5">
+        <v>2</v>
+      </c>
+      <c r="E97" s="5">
+        <v>2</v>
+      </c>
+      <c r="F97" s="5">
+        <v>0</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H97" s="5">
+        <v>805</v>
+      </c>
+      <c r="I97" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J97" s="5">
+        <v>805</v>
+      </c>
+      <c r="K97" s="5">
+        <v>0</v>
+      </c>
+      <c r="L97" s="5">
+        <v>0</v>
+      </c>
+      <c r="M97" s="5">
+        <v>0.99751552794999998</v>
+      </c>
+      <c r="N97" s="5">
+        <v>2.4844720496900001E-3</v>
+      </c>
+      <c r="O97" s="5">
+        <v>0</v>
+      </c>
+      <c r="P97" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q97" s="5">
+        <v>805</v>
+      </c>
+      <c r="R97" s="5">
+        <v>0.44472049689400001</v>
+      </c>
+      <c r="S97" s="5">
+        <v>0</v>
+      </c>
+      <c r="T97" s="5">
+        <v>0.55527950310600005</v>
+      </c>
+      <c r="U97" s="5">
+        <v>0</v>
+      </c>
+      <c r="V97" s="5">
+        <v>0</v>
+      </c>
+      <c r="W97" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X97" s="5">
+        <v>805</v>
+      </c>
+      <c r="Y97" s="5">
+        <v>0.73664596273299998</v>
+      </c>
+      <c r="Z97" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA97" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB97" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC97" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD97" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE97" s="5">
+        <v>805</v>
+      </c>
+      <c r="AF97" s="5">
+        <v>0.99751552794999998</v>
+      </c>
+      <c r="AG97" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH97" s="5">
+        <v>2.4844720496900001E-3</v>
+      </c>
+      <c r="AI97" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ97" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK97" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL97" s="5">
+        <v>805</v>
+      </c>
+      <c r="AM97" s="5">
+        <v>0.99751552794999998</v>
+      </c>
+      <c r="AN97" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO97" s="5">
+        <v>2.4844720496900001E-3</v>
+      </c>
+      <c r="AP97" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ97" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR97" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS97" s="5">
+        <v>805</v>
+      </c>
+      <c r="AT97" s="5">
+        <v>0.99503105590100005</v>
+      </c>
+      <c r="AU97" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV97" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW97" s="24"/>
+    </row>
+    <row r="98" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" s="5">
+        <v>2</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D98" s="5">
+        <v>2</v>
+      </c>
+      <c r="E98" s="5">
+        <v>2</v>
+      </c>
+      <c r="F98" s="5">
+        <v>0</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H98" s="5">
+        <v>805</v>
+      </c>
+      <c r="I98" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J98" s="5">
+        <v>1586</v>
+      </c>
+      <c r="K98" s="5">
+        <v>0</v>
+      </c>
+      <c r="L98" s="5">
+        <v>0.49243379571200002</v>
+      </c>
+      <c r="M98" s="5">
+        <v>0.50756620428800003</v>
+      </c>
+      <c r="N98" s="5">
+        <v>0</v>
+      </c>
+      <c r="O98" s="5">
+        <v>0</v>
+      </c>
+      <c r="P98" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q98" s="5">
+        <v>1586</v>
+      </c>
+      <c r="R98" s="5">
+        <v>0</v>
+      </c>
+      <c r="S98" s="5">
+        <v>0.49243379571200002</v>
+      </c>
+      <c r="T98" s="5">
+        <v>0.50756620428800003</v>
+      </c>
+      <c r="U98" s="5">
+        <v>0</v>
+      </c>
+      <c r="V98" s="5">
+        <v>0</v>
+      </c>
+      <c r="W98" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X98" s="5">
+        <v>3929</v>
+      </c>
+      <c r="Y98" s="5">
+        <v>0.14240264698399999</v>
+      </c>
+      <c r="Z98" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA98" s="5">
+        <v>3124</v>
+      </c>
+      <c r="AB98" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC98" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD98" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE98" s="5">
+        <v>1610</v>
+      </c>
+      <c r="AF98" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG98" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AH98" s="5">
+        <v>0.48509316770200001</v>
+      </c>
+      <c r="AI98" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ98" s="5">
+        <v>24</v>
+      </c>
+      <c r="AK98" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL98" s="5">
+        <v>1610</v>
+      </c>
+      <c r="AM98" s="5">
+        <v>0.48447204968899998</v>
+      </c>
+      <c r="AN98" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AO98" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP98" s="5">
+        <v>6.2111801242199999E-4</v>
+      </c>
+      <c r="AQ98" s="5">
+        <v>24</v>
+      </c>
+      <c r="AR98" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS98" s="5">
+        <v>4001</v>
+      </c>
+      <c r="AT98" s="5">
+        <v>0.19180124223600001</v>
+      </c>
+      <c r="AU98" s="5">
+        <v>24</v>
+      </c>
+      <c r="AV98" s="5">
+        <v>3220</v>
+      </c>
+      <c r="AW98" s="24"/>
+    </row>
+    <row r="99" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" s="5">
+        <v>2</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D99" s="5">
+        <v>2</v>
+      </c>
+      <c r="E99" s="5">
+        <v>2</v>
+      </c>
+      <c r="F99" s="5">
+        <v>0</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H99" s="5">
+        <v>805</v>
+      </c>
+      <c r="I99" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J99" s="5">
+        <v>805</v>
+      </c>
+      <c r="K99" s="5">
+        <v>1</v>
+      </c>
+      <c r="L99" s="5">
+        <v>0</v>
+      </c>
+      <c r="M99" s="5">
+        <v>0</v>
+      </c>
+      <c r="N99" s="5">
+        <v>0</v>
+      </c>
+      <c r="O99" s="5">
+        <v>0</v>
+      </c>
+      <c r="P99" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q99" s="5">
+        <v>805</v>
+      </c>
+      <c r="R99" s="5">
+        <v>1</v>
+      </c>
+      <c r="S99" s="5">
+        <v>0</v>
+      </c>
+      <c r="T99" s="5">
+        <v>0</v>
+      </c>
+      <c r="U99" s="5">
+        <v>0</v>
+      </c>
+      <c r="V99" s="5">
+        <v>0</v>
+      </c>
+      <c r="W99" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X99" s="5">
+        <v>805</v>
+      </c>
+      <c r="Y99" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z99" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA99" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB99" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC99" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD99" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE99" s="5">
+        <v>805</v>
+      </c>
+      <c r="AF99" s="5">
+        <v>0.99751552794999998</v>
+      </c>
+      <c r="AG99" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH99" s="5">
+        <v>2.4844720496900001E-3</v>
+      </c>
+      <c r="AI99" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ99" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK99" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL99" s="5">
+        <v>805</v>
+      </c>
+      <c r="AM99" s="5">
+        <v>0.99751552794999998</v>
+      </c>
+      <c r="AN99" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO99" s="5">
+        <v>2.4844720496900001E-3</v>
+      </c>
+      <c r="AP99" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ99" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR99" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS99" s="5">
+        <v>805</v>
+      </c>
+      <c r="AT99" s="5">
+        <v>0.99503105590100005</v>
+      </c>
+      <c r="AU99" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV99" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW99" s="24"/>
+    </row>
+    <row r="100" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B100" s="5">
+        <v>2</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D100" s="5">
+        <v>2</v>
+      </c>
+      <c r="E100" s="5">
+        <v>2</v>
+      </c>
+      <c r="F100" s="5">
+        <v>0</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H100" s="5">
+        <v>805</v>
+      </c>
+      <c r="I100" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J100" s="5">
+        <v>1610</v>
+      </c>
+      <c r="K100" s="5">
+        <v>0</v>
+      </c>
+      <c r="L100" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="M100" s="5">
+        <v>0.408695652174</v>
+      </c>
+      <c r="N100" s="5">
+        <v>0</v>
+      </c>
+      <c r="O100" s="5">
+        <v>147</v>
+      </c>
+      <c r="P100" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q100" s="5">
+        <v>805</v>
+      </c>
+      <c r="R100" s="5">
+        <v>0.18136645962699999</v>
+      </c>
+      <c r="S100" s="5">
+        <v>0</v>
+      </c>
+      <c r="T100" s="5">
+        <v>1.2422360248399999E-3</v>
+      </c>
+      <c r="U100" s="5">
+        <v>0</v>
+      </c>
+      <c r="V100" s="5">
+        <v>658</v>
+      </c>
+      <c r="W100" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X100" s="5">
+        <v>147</v>
+      </c>
+      <c r="Y100" s="5">
+        <v>0.17236024844699999</v>
+      </c>
+      <c r="Z100" s="5">
+        <v>658</v>
+      </c>
+      <c r="AA100" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB100" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC100" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD100" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE100" s="5">
+        <v>1463</v>
+      </c>
+      <c r="AF100" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG100" s="5">
+        <v>0.44976076555</v>
+      </c>
+      <c r="AH100" s="5">
+        <v>0.55023923445</v>
+      </c>
+      <c r="AI100" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ100" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK100" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL100" s="5">
+        <v>1463</v>
+      </c>
+      <c r="AM100" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN100" s="5">
+        <v>0.44976076555</v>
+      </c>
+      <c r="AO100" s="5">
+        <v>0.55023923445</v>
+      </c>
+      <c r="AP100" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ100" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR100" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS100" s="5">
+        <v>3437</v>
+      </c>
+      <c r="AT100" s="5">
+        <v>0.231379109689</v>
+      </c>
+      <c r="AU100" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV100" s="5">
+        <v>2632</v>
+      </c>
+      <c r="AW100" s="24"/>
+    </row>
+    <row r="101" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B101" s="5">
+        <v>2</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D101" s="5">
+        <v>2</v>
+      </c>
+      <c r="E101" s="5">
+        <v>3</v>
+      </c>
+      <c r="F101" s="5">
+        <v>-1</v>
+      </c>
+      <c r="G101" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H101" s="5">
+        <v>805</v>
+      </c>
+      <c r="I101" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J101" s="5">
+        <v>805</v>
+      </c>
+      <c r="K101" s="5">
+        <v>0</v>
+      </c>
+      <c r="L101" s="5">
+        <v>0</v>
+      </c>
+      <c r="M101" s="5">
+        <v>0.94658385093200004</v>
+      </c>
+      <c r="N101" s="5">
+        <v>2.4844720496900001E-3</v>
+      </c>
+      <c r="O101" s="5">
+        <v>41</v>
+      </c>
+      <c r="P101" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q101" s="5">
+        <v>805</v>
+      </c>
+      <c r="R101" s="5">
+        <v>0.44472049689400001</v>
+      </c>
+      <c r="S101" s="5">
+        <v>0</v>
+      </c>
+      <c r="T101" s="5">
+        <v>0.50434782608700002</v>
+      </c>
+      <c r="U101" s="5">
+        <v>0</v>
+      </c>
+      <c r="V101" s="5">
+        <v>41</v>
+      </c>
+      <c r="W101" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X101" s="5">
+        <v>764</v>
+      </c>
+      <c r="Y101" s="5">
+        <v>0.69254658385099999</v>
+      </c>
+      <c r="Z101" s="5">
+        <v>41</v>
+      </c>
+      <c r="AA101" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB101" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC101" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD101" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE101" s="5">
+        <v>805</v>
+      </c>
+      <c r="AF101" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG101" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH101" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI101" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ101" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK101" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL101" s="5">
+        <v>805</v>
+      </c>
+      <c r="AM101" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN101" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO101" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP101" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ101" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR101" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS101" s="5">
+        <v>805</v>
+      </c>
+      <c r="AT101" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU101" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV101" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW101" s="24"/>
+    </row>
+    <row r="102" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B102" s="5">
+        <v>2</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D102" s="5">
+        <v>2</v>
+      </c>
+      <c r="E102" s="5">
+        <v>2</v>
+      </c>
+      <c r="F102" s="5">
+        <v>0</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H102" s="5">
+        <v>805</v>
+      </c>
+      <c r="I102" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J102" s="5">
+        <v>805</v>
+      </c>
+      <c r="K102" s="5">
+        <v>0</v>
+      </c>
+      <c r="L102" s="5">
+        <v>0</v>
+      </c>
+      <c r="M102" s="5">
+        <v>0.68322981366500002</v>
+      </c>
+      <c r="N102" s="5">
+        <v>0</v>
+      </c>
+      <c r="O102" s="5">
+        <v>255</v>
+      </c>
+      <c r="P102" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q102" s="5">
+        <v>805</v>
+      </c>
+      <c r="R102" s="5">
+        <v>0.30062111801199998</v>
+      </c>
+      <c r="S102" s="5">
+        <v>0</v>
+      </c>
+      <c r="T102" s="5">
+        <v>0.38012422360199999</v>
+      </c>
+      <c r="U102" s="5">
+        <v>2.4844720496900001E-3</v>
+      </c>
+      <c r="V102" s="5">
+        <v>255</v>
+      </c>
+      <c r="W102" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X102" s="5">
+        <v>550</v>
+      </c>
+      <c r="Y102" s="5">
+        <v>0.43664596273299999</v>
+      </c>
+      <c r="Z102" s="5">
+        <v>255</v>
+      </c>
+      <c r="AA102" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB102" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC102" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD102" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE102" s="5">
+        <v>1060</v>
+      </c>
+      <c r="AF102" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG102" s="5">
+        <v>0.24056603773599999</v>
+      </c>
+      <c r="AH102" s="5">
+        <v>0.75849056603800002</v>
+      </c>
+      <c r="AI102" s="5">
+        <v>9.4339622641500002E-4</v>
+      </c>
+      <c r="AJ102" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK102" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL102" s="5">
+        <v>1060</v>
+      </c>
+      <c r="AM102" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN102" s="5">
+        <v>0.24056603773599999</v>
+      </c>
+      <c r="AO102" s="5">
+        <v>0.75849056603800002</v>
+      </c>
+      <c r="AP102" s="5">
+        <v>9.4339622641500002E-4</v>
+      </c>
+      <c r="AQ102" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR102" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS102" s="5">
+        <v>1825</v>
+      </c>
+      <c r="AT102" s="5">
+        <v>0.41739726027399998</v>
+      </c>
+      <c r="AU102" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV102" s="5">
+        <v>1020</v>
+      </c>
+      <c r="AW102" s="24"/>
+    </row>
+    <row r="103" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103" s="5">
+        <v>2</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D103" s="5">
+        <v>2</v>
+      </c>
+      <c r="E103" s="5">
+        <v>2</v>
+      </c>
+      <c r="F103" s="5">
+        <v>0</v>
+      </c>
+      <c r="G103" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H103" s="5">
+        <v>805</v>
+      </c>
+      <c r="I103" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J103" s="5">
+        <v>809</v>
+      </c>
+      <c r="K103" s="5">
+        <v>0.995055624227</v>
+      </c>
+      <c r="L103" s="5">
+        <v>4.9443757725600003E-3</v>
+      </c>
+      <c r="M103" s="5">
+        <v>0</v>
+      </c>
+      <c r="N103" s="5">
+        <v>0</v>
+      </c>
+      <c r="O103" s="5">
+        <v>0</v>
+      </c>
+      <c r="P103" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q103" s="5">
+        <v>809</v>
+      </c>
+      <c r="R103" s="5">
+        <v>0.995055624227</v>
+      </c>
+      <c r="S103" s="5">
+        <v>4.9443757725600003E-3</v>
+      </c>
+      <c r="T103" s="5">
+        <v>0</v>
+      </c>
+      <c r="U103" s="5">
+        <v>0</v>
+      </c>
+      <c r="V103" s="5">
+        <v>0</v>
+      </c>
+      <c r="W103" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X103" s="5">
+        <v>821</v>
+      </c>
+      <c r="Y103" s="5">
+        <v>0.97929354445799999</v>
+      </c>
+      <c r="Z103" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA103" s="5">
+        <v>16</v>
+      </c>
+      <c r="AB103" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC103" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD103" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE103" s="5">
+        <v>805</v>
+      </c>
+      <c r="AF103" s="5">
+        <v>0.99503105590100005</v>
+      </c>
+      <c r="AG103" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH103" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI103" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ103" s="5">
+        <v>4</v>
+      </c>
+      <c r="AK103" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL103" s="5">
+        <v>805</v>
+      </c>
+      <c r="AM103" s="5">
+        <v>0.99503105590100005</v>
+      </c>
+      <c r="AN103" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO103" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP103" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ103" s="5">
+        <v>4</v>
+      </c>
+      <c r="AR103" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS103" s="5">
+        <v>801</v>
+      </c>
+      <c r="AT103" s="5">
+        <v>0.99347826087000002</v>
+      </c>
+      <c r="AU103" s="5">
+        <v>4</v>
+      </c>
+      <c r="AV103" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW103" s="24"/>
+    </row>
+    <row r="104" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B104" s="5">
+        <v>2</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D104" s="5">
+        <v>2</v>
+      </c>
+      <c r="E104" s="5">
+        <v>2</v>
+      </c>
+      <c r="F104" s="5">
+        <v>0</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H104" s="5">
+        <v>805</v>
+      </c>
+      <c r="I104" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J104" s="5">
+        <v>1509</v>
+      </c>
+      <c r="K104" s="5">
+        <v>0</v>
+      </c>
+      <c r="L104" s="5">
+        <v>0.46653412856199999</v>
+      </c>
+      <c r="M104" s="5">
+        <v>0.53346587143799995</v>
+      </c>
+      <c r="N104" s="5">
+        <v>0</v>
+      </c>
+      <c r="O104" s="5">
+        <v>0</v>
+      </c>
+      <c r="P104" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q104" s="5">
+        <v>1509</v>
+      </c>
+      <c r="R104" s="5">
+        <v>0</v>
+      </c>
+      <c r="S104" s="5">
+        <v>0.46653412856199999</v>
+      </c>
+      <c r="T104" s="5">
+        <v>0.53346587143799995</v>
+      </c>
+      <c r="U104" s="5">
+        <v>0</v>
+      </c>
+      <c r="V104" s="5">
+        <v>0</v>
+      </c>
+      <c r="W104" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X104" s="5">
+        <v>3621</v>
+      </c>
+      <c r="Y104" s="5">
+        <v>0.22148577741</v>
+      </c>
+      <c r="Z104" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA104" s="5">
+        <v>2816</v>
+      </c>
+      <c r="AB104" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC104" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD104" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE104" s="5">
+        <v>1610</v>
+      </c>
+      <c r="AF104" s="5">
+        <v>0.43229813664599998</v>
+      </c>
+      <c r="AG104" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AH104" s="5">
+        <v>4.9689440993800002E-3</v>
+      </c>
+      <c r="AI104" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ104" s="5">
+        <v>101</v>
+      </c>
+      <c r="AK104" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL104" s="5">
+        <v>1610</v>
+      </c>
+      <c r="AM104" s="5">
+        <v>0.43229813664599998</v>
+      </c>
+      <c r="AN104" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AO104" s="5">
+        <v>4.9689440993800002E-3</v>
+      </c>
+      <c r="AP104" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ104" s="5">
+        <v>101</v>
+      </c>
+      <c r="AR104" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS104" s="5">
+        <v>3924</v>
+      </c>
+      <c r="AT104" s="5">
+        <v>0.170372670807</v>
+      </c>
+      <c r="AU104" s="5">
+        <v>101</v>
+      </c>
+      <c r="AV104" s="5">
+        <v>3220</v>
+      </c>
+      <c r="AW104" s="24"/>
+    </row>
+    <row r="105" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105" s="5">
+        <v>2</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D105" s="5">
+        <v>2</v>
+      </c>
+      <c r="E105" s="5">
+        <v>2</v>
+      </c>
+      <c r="F105" s="5">
+        <v>0</v>
+      </c>
+      <c r="G105" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H105" s="5">
+        <v>805</v>
+      </c>
+      <c r="I105" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="5">
+        <v>810</v>
+      </c>
+      <c r="K105" s="5">
+        <v>0</v>
+      </c>
+      <c r="L105" s="5">
+        <v>6.1728395061700003E-3</v>
+      </c>
+      <c r="M105" s="5">
+        <v>0.87777777777800003</v>
+      </c>
+      <c r="N105" s="5">
+        <v>0</v>
+      </c>
+      <c r="O105" s="5">
+        <v>94</v>
+      </c>
+      <c r="P105" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q105" s="5">
+        <v>1605</v>
+      </c>
+      <c r="R105" s="5">
+        <v>6.2305295950200001E-4</v>
+      </c>
+      <c r="S105" s="5">
+        <v>0.49844236760100002</v>
+      </c>
+      <c r="T105" s="5">
+        <v>5.7320872274100002E-2</v>
+      </c>
+      <c r="U105" s="5">
+        <v>6.2305295950200001E-4</v>
+      </c>
+      <c r="V105" s="5">
+        <v>711</v>
+      </c>
+      <c r="W105" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X105" s="5">
+        <v>731</v>
+      </c>
+      <c r="Y105" s="5">
+        <v>0.67545454545500005</v>
+      </c>
+      <c r="Z105" s="5">
+        <v>94</v>
+      </c>
+      <c r="AA105" s="5">
+        <v>20</v>
+      </c>
+      <c r="AB105" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC105" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD105" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE105" s="5">
+        <v>899</v>
+      </c>
+      <c r="AF105" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG105" s="5">
+        <v>0.10456062291400001</v>
+      </c>
+      <c r="AH105" s="5">
+        <v>0.88987764182399998</v>
+      </c>
+      <c r="AI105" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ105" s="5">
+        <v>5</v>
+      </c>
+      <c r="AK105" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL105" s="5">
+        <v>899</v>
+      </c>
+      <c r="AM105" s="5">
+        <v>0.864293659622</v>
+      </c>
+      <c r="AN105" s="5">
+        <v>0.10456062291400001</v>
+      </c>
+      <c r="AO105" s="5">
+        <v>2.5583982202400001E-2</v>
+      </c>
+      <c r="AP105" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ105" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR105" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS105" s="5">
+        <v>1176</v>
+      </c>
+      <c r="AT105" s="5">
+        <v>0.65749364945</v>
+      </c>
+      <c r="AU105" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV105" s="5">
+        <v>376</v>
+      </c>
+      <c r="AW105" s="24"/>
+    </row>
+    <row r="106" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B106" s="5">
+        <v>2</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D106" s="5">
+        <v>2</v>
+      </c>
+      <c r="E106" s="5">
+        <v>2</v>
+      </c>
+      <c r="F106" s="5">
+        <v>0</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H106" s="5">
+        <v>805</v>
+      </c>
+      <c r="I106" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J106" s="5">
+        <v>805</v>
+      </c>
+      <c r="K106" s="5">
+        <v>0</v>
+      </c>
+      <c r="L106" s="5">
+        <v>0</v>
+      </c>
+      <c r="M106" s="5">
+        <v>0.57763975155299996</v>
+      </c>
+      <c r="N106" s="5">
+        <v>1.2422360248399999E-3</v>
+      </c>
+      <c r="O106" s="5">
+        <v>339</v>
+      </c>
+      <c r="P106" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q106" s="5">
+        <v>805</v>
+      </c>
+      <c r="R106" s="5">
+        <v>7.4534161490700003E-3</v>
+      </c>
+      <c r="S106" s="5">
+        <v>0</v>
+      </c>
+      <c r="T106" s="5">
+        <v>0.57018633540399999</v>
+      </c>
+      <c r="U106" s="5">
+        <v>1.2422360248399999E-3</v>
+      </c>
+      <c r="V106" s="5">
+        <v>339</v>
+      </c>
+      <c r="W106" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X106" s="5">
+        <v>466</v>
+      </c>
+      <c r="Y106" s="5">
+        <v>0.42919254658400002</v>
+      </c>
+      <c r="Z106" s="5">
+        <v>339</v>
+      </c>
+      <c r="AA106" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB106" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC106" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD106" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE106" s="5">
+        <v>1144</v>
+      </c>
+      <c r="AF106" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG106" s="5">
+        <v>0.29632867132899998</v>
+      </c>
+      <c r="AH106" s="5">
+        <v>0.70367132867100002</v>
+      </c>
+      <c r="AI106" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ106" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK106" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL106" s="5">
+        <v>1144</v>
+      </c>
+      <c r="AM106" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN106" s="5">
+        <v>0.29632867132899998</v>
+      </c>
+      <c r="AO106" s="5">
+        <v>0.70367132867100002</v>
+      </c>
+      <c r="AP106" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ106" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR106" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS106" s="5">
+        <v>2161</v>
+      </c>
+      <c r="AT106" s="5">
+        <v>0.33364183248500001</v>
+      </c>
+      <c r="AU106" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV106" s="5">
+        <v>1356</v>
+      </c>
+      <c r="AW106" s="24"/>
+    </row>
+    <row r="107" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B107" s="5">
+        <v>2</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D107" s="5">
+        <v>2</v>
+      </c>
+      <c r="E107" s="5">
+        <v>2</v>
+      </c>
+      <c r="F107" s="5">
+        <v>0</v>
+      </c>
+      <c r="G107" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H107" s="5">
+        <v>805</v>
+      </c>
+      <c r="I107" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="5">
+        <v>826</v>
+      </c>
+      <c r="K107" s="5">
+        <v>0</v>
+      </c>
+      <c r="L107" s="5">
+        <v>2.5423728813599999E-2</v>
+      </c>
+      <c r="M107" s="5">
+        <v>0.97215496367999998</v>
+      </c>
+      <c r="N107" s="5">
+        <v>0</v>
+      </c>
+      <c r="O107" s="5">
+        <v>2</v>
+      </c>
+      <c r="P107" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q107" s="5">
+        <v>826</v>
+      </c>
+      <c r="R107" s="5">
+        <v>0.96004842614999997</v>
+      </c>
+      <c r="S107" s="5">
+        <v>2.5423728813599999E-2</v>
+      </c>
+      <c r="T107" s="5">
+        <v>1.2106537530300001E-2</v>
+      </c>
+      <c r="U107" s="5">
+        <v>0</v>
+      </c>
+      <c r="V107" s="5">
+        <v>2</v>
+      </c>
+      <c r="W107" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X107" s="5">
+        <v>887</v>
+      </c>
+      <c r="Y107" s="5">
+        <v>0.87767154105699996</v>
+      </c>
+      <c r="Z107" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA107" s="5">
+        <v>84</v>
+      </c>
+      <c r="AB107" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC107" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD107" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE107" s="5">
+        <v>807</v>
+      </c>
+      <c r="AF107" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG107" s="5">
+        <v>2.4783147459699999E-3</v>
+      </c>
+      <c r="AH107" s="5">
+        <v>0.97149938042100004</v>
+      </c>
+      <c r="AI107" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ107" s="5">
+        <v>21</v>
+      </c>
+      <c r="AK107" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL107" s="5">
+        <v>807</v>
+      </c>
+      <c r="AM107" s="5">
+        <v>0.87980173482000001</v>
+      </c>
+      <c r="AN107" s="5">
+        <v>2.4783147459699999E-3</v>
+      </c>
+      <c r="AO107" s="5">
+        <v>9.0458488227999997E-2</v>
+      </c>
+      <c r="AP107" s="5">
+        <v>1.2391573729900001E-3</v>
+      </c>
+      <c r="AQ107" s="5">
+        <v>21</v>
+      </c>
+      <c r="AR107" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS107" s="5">
+        <v>792</v>
+      </c>
+      <c r="AT107" s="5">
+        <v>0.85301353013500003</v>
+      </c>
+      <c r="AU107" s="5">
+        <v>21</v>
+      </c>
+      <c r="AV107" s="5">
+        <v>8</v>
+      </c>
+      <c r="AW107" s="24"/>
+    </row>
+    <row r="108" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B108" s="5">
+        <v>2</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D108" s="5">
+        <v>2</v>
+      </c>
+      <c r="E108" s="5">
+        <v>2</v>
+      </c>
+      <c r="F108" s="5">
+        <v>0</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H108" s="5">
+        <v>805</v>
+      </c>
+      <c r="I108" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="5">
+        <v>808</v>
+      </c>
+      <c r="K108" s="5">
+        <v>0</v>
+      </c>
+      <c r="L108" s="5">
+        <v>3.7128712871299999E-3</v>
+      </c>
+      <c r="M108" s="5">
+        <v>0.99257425742600003</v>
+      </c>
+      <c r="N108" s="5">
+        <v>0</v>
+      </c>
+      <c r="O108" s="5">
+        <v>3</v>
+      </c>
+      <c r="P108" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q108" s="5">
+        <v>808</v>
+      </c>
+      <c r="R108" s="5">
+        <v>0.982673267327</v>
+      </c>
+      <c r="S108" s="5">
+        <v>3.7128712871299999E-3</v>
+      </c>
+      <c r="T108" s="5">
+        <v>9.90099009901E-3</v>
+      </c>
+      <c r="U108" s="5">
+        <v>0</v>
+      </c>
+      <c r="V108" s="5">
+        <v>3</v>
+      </c>
+      <c r="W108" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X108" s="5">
+        <v>814</v>
+      </c>
+      <c r="Y108" s="5">
+        <v>0.96450428396599996</v>
+      </c>
+      <c r="Z108" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA108" s="5">
+        <v>12</v>
+      </c>
+      <c r="AB108" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC108" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD108" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE108" s="5">
+        <v>808</v>
+      </c>
+      <c r="AF108" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG108" s="5">
+        <v>3.7128712871299999E-3</v>
+      </c>
+      <c r="AH108" s="5">
+        <v>0.99257425742600003</v>
+      </c>
+      <c r="AI108" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ108" s="5">
+        <v>3</v>
+      </c>
+      <c r="AK108" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL108" s="5">
+        <v>808</v>
+      </c>
+      <c r="AM108" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN108" s="5">
+        <v>3.7128712871299999E-3</v>
+      </c>
+      <c r="AO108" s="5">
+        <v>0.99257425742600003</v>
+      </c>
+      <c r="AP108" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ108" s="5">
+        <v>3</v>
+      </c>
+      <c r="AR108" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS108" s="5">
+        <v>814</v>
+      </c>
+      <c r="AT108" s="5">
+        <v>0.84547123622999998</v>
+      </c>
+      <c r="AU108" s="5">
+        <v>3</v>
+      </c>
+      <c r="AV108" s="5">
+        <v>12</v>
+      </c>
+      <c r="AW108" s="24"/>
+    </row>
+    <row r="109" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B109" s="5">
+        <v>2</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D109" s="5">
+        <v>2</v>
+      </c>
+      <c r="E109" s="5">
+        <v>3</v>
+      </c>
+      <c r="F109" s="5">
+        <v>-1</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H109" s="5">
+        <v>805</v>
+      </c>
+      <c r="I109" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="5">
+        <v>806</v>
+      </c>
+      <c r="K109" s="5">
+        <v>0.99875930521099998</v>
+      </c>
+      <c r="L109" s="5">
+        <v>1.24069478908E-3</v>
+      </c>
+      <c r="M109" s="5">
+        <v>0</v>
+      </c>
+      <c r="N109" s="5">
+        <v>0</v>
+      </c>
+      <c r="O109" s="5">
+        <v>0</v>
+      </c>
+      <c r="P109" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q109" s="5">
+        <v>806</v>
+      </c>
+      <c r="R109" s="5">
+        <v>0.99875930521099998</v>
+      </c>
+      <c r="S109" s="5">
+        <v>1.24069478908E-3</v>
+      </c>
+      <c r="T109" s="5">
+        <v>0</v>
+      </c>
+      <c r="U109" s="5">
+        <v>0</v>
+      </c>
+      <c r="V109" s="5">
+        <v>0</v>
+      </c>
+      <c r="W109" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X109" s="5">
+        <v>809</v>
+      </c>
+      <c r="Y109" s="5">
+        <v>0.99474660074200005</v>
+      </c>
+      <c r="Z109" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA109" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB109" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC109" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD109" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE109" s="5">
+        <v>805</v>
+      </c>
+      <c r="AF109" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG109" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH109" s="5">
+        <v>0.58385093167699997</v>
+      </c>
+      <c r="AI109" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ109" s="5">
+        <v>335</v>
+      </c>
+      <c r="AK109" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL109" s="5">
+        <v>805</v>
+      </c>
+      <c r="AM109" s="5">
+        <v>3.7267080745299998E-3</v>
+      </c>
+      <c r="AN109" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO109" s="5">
+        <v>0.580124223602</v>
+      </c>
+      <c r="AP109" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ109" s="5">
+        <v>335</v>
+      </c>
+      <c r="AR109" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS109" s="5">
+        <v>470</v>
+      </c>
+      <c r="AT109" s="5">
+        <v>0.39875776397500001</v>
+      </c>
+      <c r="AU109" s="5">
+        <v>335</v>
+      </c>
+      <c r="AV109" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW109" s="24"/>
+    </row>
+    <row r="110" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B110" s="5">
+        <v>2</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D110" s="5">
+        <v>2</v>
+      </c>
+      <c r="E110" s="5">
+        <v>2</v>
+      </c>
+      <c r="F110" s="5">
+        <v>0</v>
+      </c>
+      <c r="G110" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H110" s="5">
+        <v>805</v>
+      </c>
+      <c r="I110" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="5">
+        <v>1467</v>
+      </c>
+      <c r="K110" s="5">
+        <v>0</v>
+      </c>
+      <c r="L110" s="5">
+        <v>0.451261077028</v>
+      </c>
+      <c r="M110" s="5">
+        <v>0.44580777096099999</v>
+      </c>
+      <c r="N110" s="5">
+        <v>0</v>
+      </c>
+      <c r="O110" s="5">
+        <v>151</v>
+      </c>
+      <c r="P110" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q110" s="5">
+        <v>1467</v>
+      </c>
+      <c r="R110" s="5">
+        <v>0.44580777096099999</v>
+      </c>
+      <c r="S110" s="5">
+        <v>0.451261077028</v>
+      </c>
+      <c r="T110" s="5">
+        <v>0</v>
+      </c>
+      <c r="U110" s="5">
+        <v>0</v>
+      </c>
+      <c r="V110" s="5">
+        <v>151</v>
+      </c>
+      <c r="W110" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X110" s="5">
+        <v>3302</v>
+      </c>
+      <c r="Y110" s="5">
+        <v>0.18411526209099999</v>
+      </c>
+      <c r="Z110" s="5">
+        <v>151</v>
+      </c>
+      <c r="AA110" s="5">
+        <v>2648</v>
+      </c>
+      <c r="AB110" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC110" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD110" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE110" s="5">
+        <v>1459</v>
+      </c>
+      <c r="AF110" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG110" s="5">
+        <v>0.44825222755299998</v>
+      </c>
+      <c r="AH110" s="5">
+        <v>0.45373543522999998</v>
+      </c>
+      <c r="AI110" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ110" s="5">
+        <v>143</v>
+      </c>
+      <c r="AK110" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL110" s="5">
+        <v>956</v>
+      </c>
+      <c r="AM110" s="5">
+        <v>3.1380753138099998E-3</v>
+      </c>
+      <c r="AN110" s="5">
+        <v>0.15794979079499999</v>
+      </c>
+      <c r="AO110" s="5">
+        <v>0.14644351464399999</v>
+      </c>
+      <c r="AP110" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ110" s="5">
+        <v>662</v>
+      </c>
+      <c r="AR110" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS110" s="5">
+        <v>3278</v>
+      </c>
+      <c r="AT110" s="5">
+        <v>0.12942122186499999</v>
+      </c>
+      <c r="AU110" s="5">
+        <v>143</v>
+      </c>
+      <c r="AV110" s="5">
+        <v>2616</v>
+      </c>
+      <c r="AW110" s="24"/>
     </row>
   </sheetData>
   <sortState ref="A3:AW102">
@@ -19682,8 +22944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -23406,16 +26668,16 @@
     <sortCondition ref="C3:C17"/>
   </sortState>
   <mergeCells count="10">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AR1:AV1"/>
     <mergeCell ref="AY1:BE1"/>
     <mergeCell ref="BF1:BL1"/>
     <mergeCell ref="BM1:BQ1"/>
     <mergeCell ref="AD1:AJ1"/>
     <mergeCell ref="AK1:AQ1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AR1:AV1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25530,12 +28792,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AK1:AQ1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AD1:AJ1"/>
     <mergeCell ref="CH1:CL1"/>
     <mergeCell ref="AR1:AV1"/>
     <mergeCell ref="AY1:BE1"/>
@@ -25543,6 +28799,12 @@
     <mergeCell ref="BM1:BQ1"/>
     <mergeCell ref="BT1:BZ1"/>
     <mergeCell ref="CA1:CG1"/>
+    <mergeCell ref="AK1:AQ1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AD1:AJ1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26803,12 +30065,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AY1:BE1"/>
-    <mergeCell ref="AR1:AV1"/>
     <mergeCell ref="CO1:CU1"/>
     <mergeCell ref="CV1:DB1"/>
     <mergeCell ref="DC1:DG1"/>
@@ -26819,6 +30075,12 @@
     <mergeCell ref="BT1:BZ1"/>
     <mergeCell ref="BM1:BQ1"/>
     <mergeCell ref="BF1:BL1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AY1:BE1"/>
+    <mergeCell ref="AR1:AV1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28592,6 +31854,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="BT1:BZ1"/>
+    <mergeCell ref="CA1:CG1"/>
+    <mergeCell ref="HD1:HH1"/>
+    <mergeCell ref="FN1:FR1"/>
+    <mergeCell ref="FU1:GA1"/>
+    <mergeCell ref="GB1:GH1"/>
+    <mergeCell ref="GI1:GM1"/>
+    <mergeCell ref="GP1:GV1"/>
+    <mergeCell ref="GW1:HC1"/>
+    <mergeCell ref="FG1:FM1"/>
+    <mergeCell ref="CH1:CL1"/>
+    <mergeCell ref="CO1:CU1"/>
+    <mergeCell ref="CV1:DB1"/>
+    <mergeCell ref="DC1:DG1"/>
+    <mergeCell ref="DJ1:DP1"/>
     <mergeCell ref="EZ1:FF1"/>
     <mergeCell ref="AR1:AV1"/>
     <mergeCell ref="AY1:BE1"/>
@@ -28608,21 +31885,6 @@
     <mergeCell ref="EL1:ER1"/>
     <mergeCell ref="ES1:EW1"/>
     <mergeCell ref="BM1:BQ1"/>
-    <mergeCell ref="BT1:BZ1"/>
-    <mergeCell ref="CA1:CG1"/>
-    <mergeCell ref="HD1:HH1"/>
-    <mergeCell ref="FN1:FR1"/>
-    <mergeCell ref="FU1:GA1"/>
-    <mergeCell ref="GB1:GH1"/>
-    <mergeCell ref="GI1:GM1"/>
-    <mergeCell ref="GP1:GV1"/>
-    <mergeCell ref="GW1:HC1"/>
-    <mergeCell ref="FG1:FM1"/>
-    <mergeCell ref="CH1:CL1"/>
-    <mergeCell ref="CO1:CU1"/>
-    <mergeCell ref="CV1:DB1"/>
-    <mergeCell ref="DC1:DG1"/>
-    <mergeCell ref="DJ1:DP1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uploading a second five puzzle result.
</commit_message>
<xml_diff>
--- a/Results/Mixed Bag Solver Puzzle Results.xlsx
+++ b/Results/Mixed Bag Solver Puzzle Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="2805" windowWidth="27960" windowHeight="12480" activeTab="6"/>
+    <workbookView xWindow="2010" yWindow="2805" windowWidth="27960" windowHeight="12480" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Cho Best Buddies" sheetId="7" r:id="rId1"/>
@@ -17,12 +17,13 @@
     <sheet name="Five Puzzles" sheetId="12" r:id="rId8"/>
     <sheet name="Ten Puzzles" sheetId="13" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2760" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2804" uniqueCount="163">
   <si>
     <t>Solver Type</t>
   </si>
@@ -508,6 +509,9 @@
   </si>
   <si>
     <t>pomeranz_805_12 | pomeranz_805_14 | pomeranz_805_18</t>
+  </si>
+  <si>
+    <t>pomeranz_805_1 | pomeranz_805_2 | pomeranz_805_8 | pomeranz_805_9 | pomeranz_805_10</t>
   </si>
 </sst>
 </file>
@@ -1484,14 +1488,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.375" customWidth="1"/>
+    <col min="2" max="2" width="10.375" customWidth="1"/>
+    <col min="3" max="3" width="13.75" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.25" customWidth="1"/>
+    <col min="7" max="7" width="18.125" customWidth="1"/>
+    <col min="8" max="8" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2095,14 +2099,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.375" customWidth="1"/>
+    <col min="2" max="2" width="10.375" customWidth="1"/>
+    <col min="3" max="3" width="13.75" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.25" customWidth="1"/>
+    <col min="7" max="7" width="18.125" customWidth="1"/>
+    <col min="8" max="8" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2705,18 +2709,18 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="13.875" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="5" max="6" width="18.75" customWidth="1"/>
+    <col min="7" max="7" width="20.625" customWidth="1"/>
+    <col min="8" max="8" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>81</v>
       </c>
@@ -3318,30 +3322,30 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="14.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="9.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="13" width="12.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="11.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="9.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="20" width="12.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="11.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="12.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="15.5703125" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="17.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="15.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="29.125" customWidth="1"/>
+    <col min="4" max="4" width="12.875" customWidth="1"/>
+    <col min="5" max="5" width="13.25" customWidth="1"/>
+    <col min="6" max="6" width="21.875" customWidth="1"/>
+    <col min="7" max="7" width="21.875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="15.25" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="9.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="13" width="12.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="12.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="15.25" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.125" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.375" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="20" width="12.375" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="11.375" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="12.375" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="15.625" customWidth="1"/>
+    <col min="24" max="24" width="12.25" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="17.375" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.875" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -6842,50 +6846,50 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="46.25" customWidth="1"/>
+    <col min="4" max="4" width="12.875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.28515625" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.85546875" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.85546875" customWidth="1"/>
-    <col min="29" max="29" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.375" customWidth="1"/>
+    <col min="7" max="7" width="21.875" customWidth="1"/>
+    <col min="8" max="8" width="14.375" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.25" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.125" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.375" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.375" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.25" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.125" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.375" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.375" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.625" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.25" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.375" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.875" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.875" customWidth="1"/>
+    <col min="29" max="29" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.25">
@@ -23293,68 +23297,68 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="56.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="56.25" customWidth="1"/>
+    <col min="4" max="4" width="12.875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.28515625" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.85546875" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.85546875" customWidth="1"/>
-    <col min="29" max="29" width="14.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.140625" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.140625" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.28515625" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.85546875" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.85546875" customWidth="1"/>
-    <col min="50" max="50" width="14.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.140625" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.140625" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.28515625" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="6" width="25.375" customWidth="1"/>
+    <col min="7" max="7" width="21.875" customWidth="1"/>
+    <col min="8" max="8" width="14.375" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.25" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.125" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.375" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.375" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.25" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.125" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.375" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.375" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.625" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.25" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.375" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.875" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.875" customWidth="1"/>
+    <col min="29" max="29" width="14.375" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.25" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.125" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.375" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.375" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.25" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.125" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.375" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.375" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.625" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.25" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.375" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.75" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.875" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.875" customWidth="1"/>
+    <col min="50" max="50" width="14.375" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.25" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.125" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.375" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.375" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.25" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.125" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.375" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.375" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.625" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.25" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.375" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.75" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.875" customWidth="1" outlineLevel="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:70" x14ac:dyDescent="0.25">
@@ -30182,93 +30186,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" activeCellId="1" sqref="A15:XFD15 A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
     <col min="3" max="3" width="67" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="70" max="70" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="72" max="72" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="74" max="74" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="75" max="76" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="77" max="77" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="78" max="78" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="79" max="79" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="80" max="80" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="81" max="81" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="82" max="83" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="84" max="84" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="85" max="85" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="86" max="86" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="88" max="88" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="89" max="89" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="90" max="90" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="6" width="25.375" customWidth="1"/>
+    <col min="7" max="7" width="21.875" customWidth="1"/>
+    <col min="8" max="8" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="70" max="70" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="72" max="72" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="74" max="74" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="75" max="76" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="77" max="77" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="78" max="78" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="79" max="79" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="80" max="80" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="81" max="81" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="82" max="83" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="84" max="84" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="85" max="85" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="86" max="86" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="88" max="88" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="89" max="89" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="90" max="90" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="91" max="91" width="9" collapsed="1"/>
   </cols>
   <sheetData>
@@ -34210,114 +34214,114 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DI4"/>
+  <dimension ref="A1:DI6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="87.75" customWidth="1"/>
+    <col min="4" max="4" width="12.875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="70" max="70" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="14.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="72" max="72" width="15.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="14.140625" customWidth="1" outlineLevel="2"/>
-    <col min="74" max="74" width="9.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="75" max="76" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="77" max="77" width="11.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="78" max="78" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="79" max="79" width="15.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="80" max="80" width="14.140625" customWidth="1" outlineLevel="2"/>
-    <col min="81" max="81" width="9.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="82" max="83" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="84" max="84" width="11.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="85" max="85" width="12.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="86" max="86" width="15.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="12.28515625" customWidth="1" outlineLevel="2"/>
-    <col min="88" max="88" width="17.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="89" max="89" width="14.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="90" max="90" width="15.85546875" customWidth="1" outlineLevel="2"/>
-    <col min="91" max="91" width="21.85546875" customWidth="1"/>
-    <col min="92" max="92" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="93" max="93" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="94" max="94" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="95" max="95" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="96" max="97" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="98" max="98" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="99" max="99" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="100" max="100" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="101" max="101" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="102" max="102" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="103" max="104" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="105" max="105" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="106" max="106" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="107" max="107" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="108" max="108" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="109" max="109" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="110" max="110" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="111" max="111" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="6" width="25.375" customWidth="1"/>
+    <col min="7" max="7" width="21.875" customWidth="1"/>
+    <col min="8" max="8" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="70" max="70" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="14.375" customWidth="1" outlineLevel="2"/>
+    <col min="72" max="72" width="15.25" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="14.125" customWidth="1" outlineLevel="2"/>
+    <col min="74" max="74" width="9.375" customWidth="1" outlineLevel="2"/>
+    <col min="75" max="76" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="77" max="77" width="11.375" customWidth="1" outlineLevel="2"/>
+    <col min="78" max="78" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="79" max="79" width="15.25" customWidth="1" outlineLevel="1"/>
+    <col min="80" max="80" width="14.125" customWidth="1" outlineLevel="2"/>
+    <col min="81" max="81" width="9.375" customWidth="1" outlineLevel="2"/>
+    <col min="82" max="83" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="84" max="84" width="11.375" customWidth="1" outlineLevel="2"/>
+    <col min="85" max="85" width="12.375" customWidth="1" outlineLevel="2"/>
+    <col min="86" max="86" width="15.625" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="12.25" customWidth="1" outlineLevel="2"/>
+    <col min="88" max="88" width="17.375" customWidth="1" outlineLevel="1"/>
+    <col min="89" max="89" width="14.75" customWidth="1" outlineLevel="2"/>
+    <col min="90" max="90" width="15.875" customWidth="1" outlineLevel="2"/>
+    <col min="91" max="91" width="21.875" customWidth="1"/>
+    <col min="92" max="92" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="93" max="93" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="94" max="94" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="95" max="95" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="96" max="97" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="98" max="98" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="99" max="99" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="100" max="100" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="101" max="101" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="102" max="102" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="103" max="104" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="105" max="105" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="106" max="106" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="107" max="107" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="108" max="108" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="109" max="109" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="110" max="110" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="111" max="111" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="112" max="112" width="9" collapsed="1"/>
   </cols>
   <sheetData>
@@ -35459,6 +35463,680 @@
       </c>
       <c r="DH4" s="6"/>
       <c r="DI4" s="6"/>
+    </row>
+    <row r="5" spans="1:113" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="5">
+        <v>805</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="5">
+        <v>811</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>7.3982737361300002E-3</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0.93958076448799999</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5">
+        <v>43</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>811</v>
+      </c>
+      <c r="R5" s="5">
+        <v>0.72996300863100005</v>
+      </c>
+      <c r="S5" s="5">
+        <v>7.3982737361300002E-3</v>
+      </c>
+      <c r="T5" s="5">
+        <v>0.20961775585699999</v>
+      </c>
+      <c r="U5" s="5">
+        <v>0</v>
+      </c>
+      <c r="V5" s="5">
+        <v>43</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X5" s="5">
+        <v>786</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>0.75030156815399995</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>43</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>24</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC5" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE5" s="5">
+        <v>841</v>
+      </c>
+      <c r="AF5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="5">
+        <v>4.2806183115300003E-2</v>
+      </c>
+      <c r="AH5" s="5">
+        <v>0.92508917954799996</v>
+      </c>
+      <c r="AI5" s="5">
+        <v>1.1890606420899999E-3</v>
+      </c>
+      <c r="AJ5" s="5">
+        <v>26</v>
+      </c>
+      <c r="AK5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL5" s="5">
+        <v>841</v>
+      </c>
+      <c r="AM5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="5">
+        <v>4.2806183115300003E-2</v>
+      </c>
+      <c r="AO5" s="5">
+        <v>0.92508917954799996</v>
+      </c>
+      <c r="AP5" s="5">
+        <v>1.1890606420899999E-3</v>
+      </c>
+      <c r="AQ5" s="5">
+        <v>26</v>
+      </c>
+      <c r="AR5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS5" s="5">
+        <v>923</v>
+      </c>
+      <c r="AT5" s="5">
+        <v>0.72655426764999997</v>
+      </c>
+      <c r="AU5" s="5">
+        <v>26</v>
+      </c>
+      <c r="AV5" s="5">
+        <v>144</v>
+      </c>
+      <c r="AW5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX5" s="5">
+        <v>805</v>
+      </c>
+      <c r="AY5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AZ5" s="5">
+        <v>814</v>
+      </c>
+      <c r="BA5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="5">
+        <v>1.1056511056500001E-2</v>
+      </c>
+      <c r="BC5" s="5">
+        <v>0.98894348894299999</v>
+      </c>
+      <c r="BD5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="BG5" s="5">
+        <v>814</v>
+      </c>
+      <c r="BH5" s="5">
+        <v>0.98894348894299999</v>
+      </c>
+      <c r="BI5" s="5">
+        <v>1.1056511056500001E-2</v>
+      </c>
+      <c r="BJ5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BK5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BL5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="BN5" s="5">
+        <v>841</v>
+      </c>
+      <c r="BO5" s="5">
+        <v>0.95451843043999995</v>
+      </c>
+      <c r="BP5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BQ5" s="5">
+        <v>36</v>
+      </c>
+      <c r="BR5" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="BS5" s="5">
+        <v>805</v>
+      </c>
+      <c r="BT5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="BU5" s="5">
+        <v>807</v>
+      </c>
+      <c r="BV5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BW5" s="5">
+        <v>2.4783147459699999E-3</v>
+      </c>
+      <c r="BX5" s="5">
+        <v>0.99504337050799996</v>
+      </c>
+      <c r="BY5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BZ5" s="5">
+        <v>2</v>
+      </c>
+      <c r="CA5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB5" s="5">
+        <v>807</v>
+      </c>
+      <c r="CC5" s="5">
+        <v>0.79553903345700006</v>
+      </c>
+      <c r="CD5" s="5">
+        <v>2.4783147459699999E-3</v>
+      </c>
+      <c r="CE5" s="5">
+        <v>0.198265179678</v>
+      </c>
+      <c r="CF5" s="5">
+        <v>1.2391573729900001E-3</v>
+      </c>
+      <c r="CG5" s="5">
+        <v>2</v>
+      </c>
+      <c r="CH5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="CI5" s="5">
+        <v>811</v>
+      </c>
+      <c r="CJ5" s="5">
+        <v>0.86961869618700005</v>
+      </c>
+      <c r="CK5" s="5">
+        <v>2</v>
+      </c>
+      <c r="CL5" s="5">
+        <v>8</v>
+      </c>
+      <c r="CM5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="CN5" s="5">
+        <v>805</v>
+      </c>
+      <c r="CO5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="CP5" s="5">
+        <v>823</v>
+      </c>
+      <c r="CQ5" s="5">
+        <v>0</v>
+      </c>
+      <c r="CR5" s="5">
+        <v>2.1871202916200001E-2</v>
+      </c>
+      <c r="CS5" s="5">
+        <v>0.97812879708400002</v>
+      </c>
+      <c r="CT5" s="5">
+        <v>0</v>
+      </c>
+      <c r="CU5" s="5">
+        <v>0</v>
+      </c>
+      <c r="CV5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="CW5" s="5">
+        <v>823</v>
+      </c>
+      <c r="CX5" s="5">
+        <v>0.97812879708400002</v>
+      </c>
+      <c r="CY5" s="5">
+        <v>2.1871202916200001E-2</v>
+      </c>
+      <c r="CZ5" s="5">
+        <v>0</v>
+      </c>
+      <c r="DA5" s="5">
+        <v>0</v>
+      </c>
+      <c r="DB5" s="5">
+        <v>0</v>
+      </c>
+      <c r="DC5" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="DD5" s="5">
+        <v>877</v>
+      </c>
+      <c r="DE5" s="5">
+        <v>0.91277080957800005</v>
+      </c>
+      <c r="DF5" s="5">
+        <v>0</v>
+      </c>
+      <c r="DG5" s="5">
+        <v>72</v>
+      </c>
+      <c r="DH5" s="6"/>
+      <c r="DI5" s="6"/>
+    </row>
+    <row r="6" spans="1:113" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="5">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="5">
+        <v>805</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="5">
+        <v>808</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>3.7128712871299999E-3</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0.67450495049500003</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5">
+        <v>260</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>808</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0.48886138613899999</v>
+      </c>
+      <c r="S6" s="5">
+        <v>3.7128712871299999E-3</v>
+      </c>
+      <c r="T6" s="5">
+        <v>0.18564356435599999</v>
+      </c>
+      <c r="U6" s="5">
+        <v>0</v>
+      </c>
+      <c r="V6" s="5">
+        <v>260</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X6" s="5">
+        <v>557</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>0.50642594859199996</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>260</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>12</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>805</v>
+      </c>
+      <c r="AD6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>1794</v>
+      </c>
+      <c r="AF6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="5">
+        <v>0.55128205128200003</v>
+      </c>
+      <c r="AH6" s="5">
+        <v>0.43255295429200002</v>
+      </c>
+      <c r="AI6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="5">
+        <v>29</v>
+      </c>
+      <c r="AK6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL6" s="5">
+        <v>1794</v>
+      </c>
+      <c r="AM6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="5">
+        <v>0.55128205128200003</v>
+      </c>
+      <c r="AO6" s="5">
+        <v>0.43255295429200002</v>
+      </c>
+      <c r="AP6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="5">
+        <v>29</v>
+      </c>
+      <c r="AR6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS6" s="5">
+        <v>4732</v>
+      </c>
+      <c r="AT6" s="5">
+        <v>0.13820625918900001</v>
+      </c>
+      <c r="AU6" s="5">
+        <v>29</v>
+      </c>
+      <c r="AV6" s="5">
+        <v>3956</v>
+      </c>
+      <c r="AW6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX6" s="5">
+        <v>805</v>
+      </c>
+      <c r="AY6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AZ6" s="5">
+        <v>1609</v>
+      </c>
+      <c r="BA6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="5">
+        <v>0.49968924797999997</v>
+      </c>
+      <c r="BC6" s="5">
+        <v>0.50031075201999997</v>
+      </c>
+      <c r="BD6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BF6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="BG6" s="5">
+        <v>1609</v>
+      </c>
+      <c r="BH6" s="5">
+        <v>0.50031075201999997</v>
+      </c>
+      <c r="BI6" s="5">
+        <v>0.49968924797999997</v>
+      </c>
+      <c r="BJ6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BK6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BL6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="BN6" s="5">
+        <v>4021</v>
+      </c>
+      <c r="BO6" s="5">
+        <v>0.198706789356</v>
+      </c>
+      <c r="BP6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BQ6" s="5">
+        <v>3216</v>
+      </c>
+      <c r="BR6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="BS6" s="5">
+        <v>805</v>
+      </c>
+      <c r="BT6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="BU6" s="5">
+        <v>1611</v>
+      </c>
+      <c r="BV6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BW6" s="5">
+        <v>0.50031036623199998</v>
+      </c>
+      <c r="BX6" s="5">
+        <v>0.49844816883900001</v>
+      </c>
+      <c r="BY6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BZ6" s="5">
+        <v>2</v>
+      </c>
+      <c r="CA6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="CB6" s="5">
+        <v>1611</v>
+      </c>
+      <c r="CC6" s="5">
+        <v>0</v>
+      </c>
+      <c r="CD6" s="5">
+        <v>0.50031036623199998</v>
+      </c>
+      <c r="CE6" s="5">
+        <v>0.49844816883900001</v>
+      </c>
+      <c r="CF6" s="5">
+        <v>0</v>
+      </c>
+      <c r="CG6" s="5">
+        <v>2</v>
+      </c>
+      <c r="CH6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="CI6" s="5">
+        <v>4027</v>
+      </c>
+      <c r="CJ6" s="5">
+        <v>0.17386448250200001</v>
+      </c>
+      <c r="CK6" s="5">
+        <v>2</v>
+      </c>
+      <c r="CL6" s="5">
+        <v>3224</v>
+      </c>
+      <c r="CM6" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="CN6" s="5">
+        <v>805</v>
+      </c>
+      <c r="CO6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CP6" s="5">
+        <v>1766</v>
+      </c>
+      <c r="CQ6" s="5">
+        <v>0</v>
+      </c>
+      <c r="CR6" s="5">
+        <v>0.54416761041899997</v>
+      </c>
+      <c r="CS6" s="5">
+        <v>0.455266138165</v>
+      </c>
+      <c r="CT6" s="5">
+        <v>0</v>
+      </c>
+      <c r="CU6" s="5">
+        <v>1</v>
+      </c>
+      <c r="CV6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CW6" s="5">
+        <v>1766</v>
+      </c>
+      <c r="CX6" s="5">
+        <v>0</v>
+      </c>
+      <c r="CY6" s="5">
+        <v>0.54416761041899997</v>
+      </c>
+      <c r="CZ6" s="5">
+        <v>0.455266138165</v>
+      </c>
+      <c r="DA6" s="5">
+        <v>0</v>
+      </c>
+      <c r="DB6" s="5">
+        <v>1</v>
+      </c>
+      <c r="DC6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="DD6" s="5">
+        <v>4648</v>
+      </c>
+      <c r="DE6" s="5">
+        <v>0.16713271671300001</v>
+      </c>
+      <c r="DF6" s="5">
+        <v>1</v>
+      </c>
+      <c r="DG6" s="5">
+        <v>3844</v>
+      </c>
+      <c r="DH6" s="6"/>
+      <c r="DI6" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -35494,201 +36172,201 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="46.25" customWidth="1"/>
+    <col min="4" max="4" width="12.875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="70" max="70" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="72" max="72" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="74" max="74" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="75" max="76" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="77" max="77" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="78" max="78" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="79" max="79" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="80" max="80" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="81" max="81" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="82" max="83" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="84" max="84" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="85" max="85" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="86" max="86" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="88" max="88" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="89" max="89" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="90" max="90" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="91" max="91" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="92" max="92" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="93" max="93" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="94" max="94" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="95" max="95" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="96" max="97" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="98" max="98" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="99" max="99" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="100" max="100" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="101" max="101" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="102" max="102" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="103" max="104" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="105" max="105" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="106" max="106" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="107" max="107" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="108" max="108" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="109" max="109" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="110" max="110" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="111" max="111" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="112" max="112" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="113" max="113" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="114" max="114" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="115" max="115" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="116" max="116" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="117" max="118" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="119" max="119" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="120" max="120" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="121" max="121" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="122" max="122" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="123" max="123" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="124" max="125" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="126" max="126" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="127" max="127" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="128" max="128" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="129" max="129" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="130" max="130" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="131" max="131" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="132" max="132" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="133" max="133" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="134" max="134" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="135" max="135" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="136" max="136" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="137" max="137" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="138" max="139" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="140" max="140" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="141" max="141" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="142" max="142" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="143" max="143" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="144" max="144" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="145" max="146" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="147" max="147" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="148" max="148" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="149" max="149" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="150" max="150" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="151" max="151" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="152" max="152" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="153" max="153" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="154" max="154" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="155" max="155" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="156" max="156" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="157" max="157" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="158" max="158" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="159" max="160" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="161" max="161" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="162" max="162" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="163" max="163" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="164" max="164" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="165" max="165" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="166" max="167" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="168" max="168" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="169" max="169" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="170" max="170" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="171" max="171" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="172" max="172" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="173" max="173" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="174" max="174" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="175" max="175" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="176" max="176" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="177" max="177" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="178" max="178" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="179" max="179" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="180" max="181" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="182" max="182" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="183" max="183" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="184" max="184" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="185" max="185" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="186" max="186" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="187" max="188" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="189" max="189" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="190" max="190" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="191" max="191" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="192" max="192" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="193" max="193" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="194" max="194" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="195" max="195" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="196" max="196" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="197" max="197" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="198" max="198" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="199" max="199" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="200" max="200" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="201" max="202" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="203" max="203" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="204" max="204" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="205" max="205" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="206" max="206" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="207" max="207" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="208" max="209" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="210" max="210" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="211" max="211" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="212" max="212" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="213" max="213" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="214" max="214" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="215" max="215" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="216" max="216" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="6" width="25.375" customWidth="1"/>
+    <col min="7" max="7" width="21.875" customWidth="1"/>
+    <col min="8" max="8" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="70" max="70" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="72" max="72" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="74" max="74" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="75" max="76" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="77" max="77" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="78" max="78" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="79" max="79" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="80" max="80" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="81" max="81" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="82" max="83" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="84" max="84" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="85" max="85" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="86" max="86" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="88" max="88" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="89" max="89" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="90" max="90" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="91" max="91" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="92" max="92" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="93" max="93" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="94" max="94" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="95" max="95" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="96" max="97" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="98" max="98" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="99" max="99" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="100" max="100" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="101" max="101" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="102" max="102" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="103" max="104" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="105" max="105" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="106" max="106" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="107" max="107" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="108" max="108" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="109" max="109" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="110" max="110" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="111" max="111" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="112" max="112" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="113" max="113" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="114" max="114" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="115" max="115" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="116" max="116" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="117" max="118" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="119" max="119" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="120" max="120" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="121" max="121" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="122" max="122" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="123" max="123" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="124" max="125" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="126" max="126" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="127" max="127" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="128" max="128" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="129" max="129" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="130" max="130" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="131" max="131" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="132" max="132" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="133" max="133" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="134" max="134" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="135" max="135" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="136" max="136" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="137" max="137" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="138" max="139" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="140" max="140" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="141" max="141" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="142" max="142" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="143" max="143" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="144" max="144" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="145" max="146" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="147" max="147" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="148" max="148" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="149" max="149" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="150" max="150" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="151" max="151" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="152" max="152" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="153" max="153" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="154" max="154" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="155" max="155" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="156" max="156" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="157" max="157" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="158" max="158" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="159" max="160" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="161" max="161" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="162" max="162" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="163" max="163" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="164" max="164" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="165" max="165" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="166" max="167" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="168" max="168" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="169" max="169" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="170" max="170" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="171" max="171" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="172" max="172" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="173" max="173" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="174" max="174" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="175" max="175" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="176" max="176" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="177" max="177" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="178" max="178" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="179" max="179" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="180" max="181" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="182" max="182" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="183" max="183" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="184" max="184" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="185" max="185" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="186" max="186" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="187" max="188" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="189" max="189" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="190" max="190" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="191" max="191" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="192" max="192" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="193" max="193" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="194" max="194" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="195" max="195" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="196" max="196" width="21.875" customWidth="1" collapsed="1"/>
+    <col min="197" max="197" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="198" max="198" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="199" max="199" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="200" max="200" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="201" max="202" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="203" max="203" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="204" max="204" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="205" max="205" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="206" max="206" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="207" max="207" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="208" max="209" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="210" max="210" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="211" max="211" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="212" max="212" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="213" max="213" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="214" max="214" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="215" max="215" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="216" max="216" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="217" max="217" width="9" collapsed="1"/>
   </cols>
   <sheetData>
@@ -37258,6 +37936,9 @@
     <mergeCell ref="DC1:DG1"/>
     <mergeCell ref="DJ1:DP1"/>
     <mergeCell ref="EZ1:FF1"/>
+    <mergeCell ref="ES1:EW1"/>
+    <mergeCell ref="EE1:EK1"/>
+    <mergeCell ref="EL1:ER1"/>
     <mergeCell ref="HD1:HH1"/>
     <mergeCell ref="FN1:FR1"/>
     <mergeCell ref="FU1:GA1"/>
@@ -37265,7 +37946,6 @@
     <mergeCell ref="GI1:GM1"/>
     <mergeCell ref="GP1:GV1"/>
     <mergeCell ref="GW1:HC1"/>
-    <mergeCell ref="ES1:EW1"/>
     <mergeCell ref="AR1:AV1"/>
     <mergeCell ref="AY1:BE1"/>
     <mergeCell ref="BF1:BL1"/>
@@ -37280,8 +37960,6 @@
     <mergeCell ref="BM1:BQ1"/>
     <mergeCell ref="DQ1:DW1"/>
     <mergeCell ref="DX1:EB1"/>
-    <mergeCell ref="EE1:EK1"/>
-    <mergeCell ref="EL1:ER1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uploading the Mixed-Bag Solver results for the 5 paper example in the paper.
</commit_message>
<xml_diff>
--- a/Results/Mixed Bag Solver Puzzle Results.xlsx
+++ b/Results/Mixed Bag Solver Puzzle Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="2805" windowWidth="27960" windowHeight="12480" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="2010" yWindow="2805" windowWidth="27960" windowHeight="12480" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Cho Best Buddies" sheetId="7" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Four Puzzles" sheetId="14" r:id="rId8"/>
     <sheet name="Five Puzzles" sheetId="12" r:id="rId9"/>
     <sheet name="Ten Puzzles" sheetId="13" r:id="rId10"/>
+    <sheet name="Paper Results" sheetId="17" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3255" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3284" uniqueCount="189">
   <si>
     <t>Solver Type</t>
   </si>
@@ -572,6 +573,24 @@
   </si>
   <si>
     <t># Puzzles</t>
+  </si>
+  <si>
+    <t>pomeranz_805_19 | mcgill_540_7 | pomeranz_805_14 | 3300_1 | pomeranz_805_10</t>
+  </si>
+  <si>
+    <t>Paper Results</t>
+  </si>
+  <si>
+    <t>EDAS</t>
+  </si>
+  <si>
+    <t>Average Score</t>
+  </si>
+  <si>
+    <t># Input Pieces</t>
+  </si>
+  <si>
+    <t># Solved Pieces</t>
   </si>
 </sst>
 </file>
@@ -1155,7 +1174,7 @@
     <xf numFmtId="0" fontId="4" fillId="36" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1197,6 +1216,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="43" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1206,26 +1247,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="43" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1580,14 +1606,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.375" customWidth="1"/>
-    <col min="2" max="2" width="10.375" customWidth="1"/>
-    <col min="3" max="3" width="13.75" customWidth="1"/>
-    <col min="4" max="4" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="17.25" customWidth="1"/>
-    <col min="7" max="7" width="18.125" customWidth="1"/>
-    <col min="8" max="8" width="17.375" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2185,465 +2211,465 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HH7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AW2"/>
+    <sheetView topLeftCell="AW1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="3" max="3" width="46.25" customWidth="1"/>
-    <col min="4" max="4" width="12.875" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="25.375" customWidth="1"/>
-    <col min="7" max="7" width="21.875" customWidth="1"/>
-    <col min="8" max="8" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="70" max="70" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="72" max="72" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="74" max="74" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="75" max="76" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="77" max="77" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="78" max="78" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="79" max="79" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="80" max="80" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="81" max="81" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="82" max="83" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="84" max="84" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="85" max="85" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="86" max="86" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="88" max="88" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="89" max="89" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="90" max="90" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="91" max="91" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="92" max="92" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="93" max="93" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="94" max="94" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="95" max="95" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="96" max="97" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="98" max="98" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="99" max="99" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="100" max="100" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="101" max="101" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="102" max="102" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="103" max="104" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="105" max="105" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="106" max="106" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="107" max="107" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="108" max="108" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="109" max="109" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="110" max="110" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="111" max="111" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="112" max="112" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="113" max="113" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="114" max="114" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="115" max="115" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="116" max="116" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="117" max="118" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="119" max="119" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="120" max="120" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="121" max="121" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="122" max="122" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="123" max="123" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="124" max="125" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="126" max="126" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="127" max="127" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="128" max="128" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="129" max="129" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="130" max="130" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="131" max="131" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="132" max="132" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="133" max="133" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="134" max="134" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="135" max="135" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="136" max="136" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="137" max="137" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="138" max="139" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="140" max="140" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="141" max="141" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="142" max="142" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="143" max="143" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="144" max="144" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="145" max="146" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="147" max="147" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="148" max="148" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="149" max="149" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="150" max="150" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="151" max="151" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="152" max="152" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="153" max="153" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="154" max="154" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="155" max="155" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="156" max="156" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="157" max="157" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="158" max="158" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="159" max="160" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="161" max="161" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="162" max="162" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="163" max="163" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="164" max="164" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="165" max="165" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="166" max="167" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="168" max="168" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="169" max="169" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="170" max="170" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="171" max="171" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="172" max="172" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="173" max="173" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="174" max="174" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="175" max="175" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="176" max="176" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="177" max="177" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="178" max="178" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="179" max="179" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="180" max="181" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="182" max="182" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="183" max="183" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="184" max="184" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="185" max="185" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="186" max="186" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="187" max="188" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="189" max="189" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="190" max="190" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="191" max="191" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="192" max="192" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="193" max="193" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="194" max="194" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="195" max="195" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="196" max="196" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="197" max="197" width="14.375" customWidth="1" outlineLevel="2"/>
-    <col min="198" max="198" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="199" max="199" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="200" max="200" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="201" max="202" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="203" max="203" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="204" max="204" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="205" max="205" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="206" max="206" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="207" max="207" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="208" max="209" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="210" max="210" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="211" max="211" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="212" max="212" width="15.625" customWidth="1" outlineLevel="1"/>
-    <col min="213" max="213" width="12.25" customWidth="1" outlineLevel="2"/>
-    <col min="214" max="214" width="17.375" customWidth="1" outlineLevel="1"/>
-    <col min="215" max="215" width="14.75" customWidth="1" outlineLevel="2"/>
-    <col min="216" max="216" width="15.875" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="70" max="70" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="72" max="72" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="74" max="74" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="75" max="76" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="77" max="77" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="78" max="78" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="79" max="79" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="80" max="80" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="81" max="81" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="82" max="83" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="84" max="84" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="85" max="85" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="86" max="86" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="88" max="88" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="89" max="89" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="90" max="90" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="91" max="91" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="92" max="92" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="93" max="93" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="94" max="94" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="95" max="95" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="96" max="97" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="98" max="98" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="99" max="99" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="100" max="100" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="101" max="101" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="102" max="102" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="103" max="104" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="105" max="105" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="106" max="106" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="107" max="107" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="108" max="108" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="109" max="109" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="110" max="110" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="111" max="111" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="112" max="112" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="113" max="113" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="114" max="114" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="115" max="115" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="116" max="116" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="117" max="118" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="119" max="119" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="120" max="120" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="121" max="121" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="122" max="122" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="123" max="123" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="124" max="125" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="126" max="126" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="127" max="127" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="128" max="128" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="129" max="129" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="130" max="130" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="131" max="131" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="132" max="132" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="133" max="133" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="134" max="134" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="135" max="135" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="136" max="136" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="137" max="137" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="138" max="139" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="140" max="140" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="141" max="141" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="142" max="142" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="143" max="143" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="144" max="144" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="145" max="146" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="147" max="147" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="148" max="148" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="149" max="149" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="150" max="150" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="151" max="151" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="152" max="152" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="153" max="153" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="154" max="154" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="155" max="155" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="156" max="156" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="157" max="157" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="158" max="158" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="159" max="160" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="161" max="161" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="162" max="162" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="163" max="163" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="164" max="164" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="165" max="165" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="166" max="167" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="168" max="168" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="169" max="169" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="170" max="170" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="171" max="171" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="172" max="172" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="173" max="173" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="174" max="174" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="175" max="175" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="176" max="176" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="177" max="177" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="178" max="178" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="179" max="179" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="180" max="181" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="182" max="182" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="183" max="183" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="184" max="184" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="185" max="185" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="186" max="186" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="187" max="188" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="189" max="189" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="190" max="190" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="191" max="191" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="192" max="192" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="193" max="193" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="194" max="194" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="195" max="195" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="196" max="196" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="197" max="197" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="198" max="198" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="199" max="199" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="200" max="200" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="201" max="202" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="203" max="203" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="204" max="204" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="205" max="205" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="206" max="206" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="207" max="207" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="208" max="209" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="210" max="210" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="211" max="211" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="212" max="212" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="213" max="213" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="214" max="214" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="215" max="215" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="216" max="216" width="15.85546875" customWidth="1" outlineLevel="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:216" x14ac:dyDescent="0.25">
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="I1" s="22" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="I1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22" t="s">
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22" t="s">
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AD1" s="22" t="s">
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AD1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="22"/>
-      <c r="AG1" s="22"/>
-      <c r="AH1" s="22"/>
-      <c r="AI1" s="22"/>
-      <c r="AJ1" s="22"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="22"/>
-      <c r="AQ1" s="22"/>
-      <c r="AR1" s="22" t="s">
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="23"/>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="23"/>
-      <c r="AV1" s="23"/>
-      <c r="AY1" s="22" t="s">
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
+      <c r="AY1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="22"/>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22" t="s">
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="30"/>
+      <c r="BF1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="BG1" s="22"/>
-      <c r="BH1" s="22"/>
-      <c r="BI1" s="22"/>
-      <c r="BJ1" s="22"/>
-      <c r="BK1" s="22"/>
-      <c r="BL1" s="22"/>
-      <c r="BM1" s="22" t="s">
+      <c r="BG1" s="30"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="BN1" s="23"/>
-      <c r="BO1" s="23"/>
-      <c r="BP1" s="23"/>
-      <c r="BQ1" s="23"/>
-      <c r="BT1" s="22" t="s">
+      <c r="BN1" s="31"/>
+      <c r="BO1" s="31"/>
+      <c r="BP1" s="31"/>
+      <c r="BQ1" s="31"/>
+      <c r="BT1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="BU1" s="22"/>
-      <c r="BV1" s="22"/>
-      <c r="BW1" s="22"/>
-      <c r="BX1" s="22"/>
-      <c r="BY1" s="22"/>
-      <c r="BZ1" s="22"/>
-      <c r="CA1" s="22" t="s">
+      <c r="BU1" s="30"/>
+      <c r="BV1" s="30"/>
+      <c r="BW1" s="30"/>
+      <c r="BX1" s="30"/>
+      <c r="BY1" s="30"/>
+      <c r="BZ1" s="30"/>
+      <c r="CA1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="CB1" s="22"/>
-      <c r="CC1" s="22"/>
-      <c r="CD1" s="22"/>
-      <c r="CE1" s="22"/>
-      <c r="CF1" s="22"/>
-      <c r="CG1" s="22"/>
-      <c r="CH1" s="22" t="s">
+      <c r="CB1" s="30"/>
+      <c r="CC1" s="30"/>
+      <c r="CD1" s="30"/>
+      <c r="CE1" s="30"/>
+      <c r="CF1" s="30"/>
+      <c r="CG1" s="30"/>
+      <c r="CH1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="CI1" s="23"/>
-      <c r="CJ1" s="23"/>
-      <c r="CK1" s="23"/>
-      <c r="CL1" s="23"/>
-      <c r="CO1" s="22" t="s">
+      <c r="CI1" s="31"/>
+      <c r="CJ1" s="31"/>
+      <c r="CK1" s="31"/>
+      <c r="CL1" s="31"/>
+      <c r="CO1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="CP1" s="22"/>
-      <c r="CQ1" s="22"/>
-      <c r="CR1" s="22"/>
-      <c r="CS1" s="22"/>
-      <c r="CT1" s="22"/>
-      <c r="CU1" s="22"/>
-      <c r="CV1" s="22" t="s">
+      <c r="CP1" s="30"/>
+      <c r="CQ1" s="30"/>
+      <c r="CR1" s="30"/>
+      <c r="CS1" s="30"/>
+      <c r="CT1" s="30"/>
+      <c r="CU1" s="30"/>
+      <c r="CV1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="CW1" s="22"/>
-      <c r="CX1" s="22"/>
-      <c r="CY1" s="22"/>
-      <c r="CZ1" s="22"/>
-      <c r="DA1" s="22"/>
-      <c r="DB1" s="22"/>
-      <c r="DC1" s="22" t="s">
+      <c r="CW1" s="30"/>
+      <c r="CX1" s="30"/>
+      <c r="CY1" s="30"/>
+      <c r="CZ1" s="30"/>
+      <c r="DA1" s="30"/>
+      <c r="DB1" s="30"/>
+      <c r="DC1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="DD1" s="23"/>
-      <c r="DE1" s="23"/>
-      <c r="DF1" s="23"/>
-      <c r="DG1" s="23"/>
-      <c r="DJ1" s="22" t="s">
+      <c r="DD1" s="31"/>
+      <c r="DE1" s="31"/>
+      <c r="DF1" s="31"/>
+      <c r="DG1" s="31"/>
+      <c r="DJ1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="DK1" s="22"/>
-      <c r="DL1" s="22"/>
-      <c r="DM1" s="22"/>
-      <c r="DN1" s="22"/>
-      <c r="DO1" s="22"/>
-      <c r="DP1" s="22"/>
-      <c r="DQ1" s="22" t="s">
+      <c r="DK1" s="30"/>
+      <c r="DL1" s="30"/>
+      <c r="DM1" s="30"/>
+      <c r="DN1" s="30"/>
+      <c r="DO1" s="30"/>
+      <c r="DP1" s="30"/>
+      <c r="DQ1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="DR1" s="22"/>
-      <c r="DS1" s="22"/>
-      <c r="DT1" s="22"/>
-      <c r="DU1" s="22"/>
-      <c r="DV1" s="22"/>
-      <c r="DW1" s="22"/>
-      <c r="DX1" s="22" t="s">
+      <c r="DR1" s="30"/>
+      <c r="DS1" s="30"/>
+      <c r="DT1" s="30"/>
+      <c r="DU1" s="30"/>
+      <c r="DV1" s="30"/>
+      <c r="DW1" s="30"/>
+      <c r="DX1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="DY1" s="23"/>
-      <c r="DZ1" s="23"/>
-      <c r="EA1" s="23"/>
-      <c r="EB1" s="23"/>
-      <c r="EE1" s="22" t="s">
+      <c r="DY1" s="31"/>
+      <c r="DZ1" s="31"/>
+      <c r="EA1" s="31"/>
+      <c r="EB1" s="31"/>
+      <c r="EE1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="EF1" s="22"/>
-      <c r="EG1" s="22"/>
-      <c r="EH1" s="22"/>
-      <c r="EI1" s="22"/>
-      <c r="EJ1" s="22"/>
-      <c r="EK1" s="22"/>
-      <c r="EL1" s="22" t="s">
+      <c r="EF1" s="30"/>
+      <c r="EG1" s="30"/>
+      <c r="EH1" s="30"/>
+      <c r="EI1" s="30"/>
+      <c r="EJ1" s="30"/>
+      <c r="EK1" s="30"/>
+      <c r="EL1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="EM1" s="22"/>
-      <c r="EN1" s="22"/>
-      <c r="EO1" s="22"/>
-      <c r="EP1" s="22"/>
-      <c r="EQ1" s="22"/>
-      <c r="ER1" s="22"/>
-      <c r="ES1" s="22" t="s">
+      <c r="EM1" s="30"/>
+      <c r="EN1" s="30"/>
+      <c r="EO1" s="30"/>
+      <c r="EP1" s="30"/>
+      <c r="EQ1" s="30"/>
+      <c r="ER1" s="30"/>
+      <c r="ES1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="ET1" s="23"/>
-      <c r="EU1" s="23"/>
-      <c r="EV1" s="23"/>
-      <c r="EW1" s="23"/>
-      <c r="EZ1" s="22" t="s">
+      <c r="ET1" s="31"/>
+      <c r="EU1" s="31"/>
+      <c r="EV1" s="31"/>
+      <c r="EW1" s="31"/>
+      <c r="EZ1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="FA1" s="22"/>
-      <c r="FB1" s="22"/>
-      <c r="FC1" s="22"/>
-      <c r="FD1" s="22"/>
-      <c r="FE1" s="22"/>
-      <c r="FF1" s="22"/>
-      <c r="FG1" s="22" t="s">
+      <c r="FA1" s="30"/>
+      <c r="FB1" s="30"/>
+      <c r="FC1" s="30"/>
+      <c r="FD1" s="30"/>
+      <c r="FE1" s="30"/>
+      <c r="FF1" s="30"/>
+      <c r="FG1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="FH1" s="22"/>
-      <c r="FI1" s="22"/>
-      <c r="FJ1" s="22"/>
-      <c r="FK1" s="22"/>
-      <c r="FL1" s="22"/>
-      <c r="FM1" s="22"/>
-      <c r="FN1" s="22" t="s">
+      <c r="FH1" s="30"/>
+      <c r="FI1" s="30"/>
+      <c r="FJ1" s="30"/>
+      <c r="FK1" s="30"/>
+      <c r="FL1" s="30"/>
+      <c r="FM1" s="30"/>
+      <c r="FN1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="FO1" s="23"/>
-      <c r="FP1" s="23"/>
-      <c r="FQ1" s="23"/>
-      <c r="FR1" s="23"/>
-      <c r="FU1" s="22" t="s">
+      <c r="FO1" s="31"/>
+      <c r="FP1" s="31"/>
+      <c r="FQ1" s="31"/>
+      <c r="FR1" s="31"/>
+      <c r="FU1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="FV1" s="22"/>
-      <c r="FW1" s="22"/>
-      <c r="FX1" s="22"/>
-      <c r="FY1" s="22"/>
-      <c r="FZ1" s="22"/>
-      <c r="GA1" s="22"/>
-      <c r="GB1" s="22" t="s">
+      <c r="FV1" s="30"/>
+      <c r="FW1" s="30"/>
+      <c r="FX1" s="30"/>
+      <c r="FY1" s="30"/>
+      <c r="FZ1" s="30"/>
+      <c r="GA1" s="30"/>
+      <c r="GB1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="GC1" s="22"/>
-      <c r="GD1" s="22"/>
-      <c r="GE1" s="22"/>
-      <c r="GF1" s="22"/>
-      <c r="GG1" s="22"/>
-      <c r="GH1" s="22"/>
-      <c r="GI1" s="22" t="s">
+      <c r="GC1" s="30"/>
+      <c r="GD1" s="30"/>
+      <c r="GE1" s="30"/>
+      <c r="GF1" s="30"/>
+      <c r="GG1" s="30"/>
+      <c r="GH1" s="30"/>
+      <c r="GI1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="GJ1" s="23"/>
-      <c r="GK1" s="23"/>
-      <c r="GL1" s="23"/>
-      <c r="GM1" s="23"/>
-      <c r="GP1" s="22" t="s">
+      <c r="GJ1" s="31"/>
+      <c r="GK1" s="31"/>
+      <c r="GL1" s="31"/>
+      <c r="GM1" s="31"/>
+      <c r="GP1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="GQ1" s="22"/>
-      <c r="GR1" s="22"/>
-      <c r="GS1" s="22"/>
-      <c r="GT1" s="22"/>
-      <c r="GU1" s="22"/>
-      <c r="GV1" s="22"/>
-      <c r="GW1" s="22" t="s">
+      <c r="GQ1" s="30"/>
+      <c r="GR1" s="30"/>
+      <c r="GS1" s="30"/>
+      <c r="GT1" s="30"/>
+      <c r="GU1" s="30"/>
+      <c r="GV1" s="30"/>
+      <c r="GW1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="GX1" s="22"/>
-      <c r="GY1" s="22"/>
-      <c r="GZ1" s="22"/>
-      <c r="HA1" s="22"/>
-      <c r="HB1" s="22"/>
-      <c r="HC1" s="22"/>
-      <c r="HD1" s="22" t="s">
+      <c r="GX1" s="30"/>
+      <c r="GY1" s="30"/>
+      <c r="GZ1" s="30"/>
+      <c r="HA1" s="30"/>
+      <c r="HB1" s="30"/>
+      <c r="HC1" s="30"/>
+      <c r="HD1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="HE1" s="23"/>
-      <c r="HF1" s="23"/>
-      <c r="HG1" s="23"/>
-      <c r="HH1" s="23"/>
+      <c r="HE1" s="31"/>
+      <c r="HF1" s="31"/>
+      <c r="HG1" s="31"/>
+      <c r="HH1" s="31"/>
     </row>
     <row r="2" spans="1:216" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4600,27 +4626,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="BT1:BZ1"/>
-    <mergeCell ref="CA1:CG1"/>
-    <mergeCell ref="BM1:BQ1"/>
-    <mergeCell ref="DQ1:DW1"/>
-    <mergeCell ref="DX1:EB1"/>
-    <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="AY1:BE1"/>
-    <mergeCell ref="BF1:BL1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AD1:AJ1"/>
-    <mergeCell ref="AK1:AQ1"/>
-    <mergeCell ref="HD1:HH1"/>
-    <mergeCell ref="FN1:FR1"/>
-    <mergeCell ref="FU1:GA1"/>
-    <mergeCell ref="GB1:GH1"/>
-    <mergeCell ref="GI1:GM1"/>
-    <mergeCell ref="GP1:GV1"/>
-    <mergeCell ref="GW1:HC1"/>
     <mergeCell ref="FG1:FM1"/>
     <mergeCell ref="CH1:CL1"/>
     <mergeCell ref="CO1:CU1"/>
@@ -4631,9 +4636,211 @@
     <mergeCell ref="ES1:EW1"/>
     <mergeCell ref="EE1:EK1"/>
     <mergeCell ref="EL1:ER1"/>
+    <mergeCell ref="HD1:HH1"/>
+    <mergeCell ref="FN1:FR1"/>
+    <mergeCell ref="FU1:GA1"/>
+    <mergeCell ref="GB1:GH1"/>
+    <mergeCell ref="GI1:GM1"/>
+    <mergeCell ref="GP1:GV1"/>
+    <mergeCell ref="GW1:HC1"/>
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="AY1:BE1"/>
+    <mergeCell ref="BF1:BL1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AD1:AJ1"/>
+    <mergeCell ref="AK1:AQ1"/>
+    <mergeCell ref="BT1:BZ1"/>
+    <mergeCell ref="CA1:CG1"/>
+    <mergeCell ref="BM1:BQ1"/>
+    <mergeCell ref="DQ1:DW1"/>
+    <mergeCell ref="DX1:EB1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$H$14,0,21*(ROW(A3)-ROW(A$3)))</f>
+        <v>805</v>
+      </c>
+      <c r="B3" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$J$14,0,21*(ROW(B3)-ROW(B$3)))</f>
+        <v>805</v>
+      </c>
+      <c r="C3" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$K$14,0,21*(ROW(C3)-ROW(C$3)))</f>
+        <v>0.99006211180100001</v>
+      </c>
+      <c r="D3" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$R$14,0,21*(ROW(D3)-ROW(D$3)))</f>
+        <v>0.99006211180100001</v>
+      </c>
+      <c r="E3" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$Y$14,0,21*(ROW(E3)-ROW(E$3)))</f>
+        <v>0.98819875776400001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$H$14,0,21*(ROW(A4)-ROW(A$3)))</f>
+        <v>540</v>
+      </c>
+      <c r="B4" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$J$14,0,21*(ROW(B4)-ROW(B$3)))</f>
+        <v>540</v>
+      </c>
+      <c r="C4" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$K$14,0,21*(ROW(C4)-ROW(C$3)))</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$R$14,0,21*(ROW(D4)-ROW(D$3)))</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$Y$14,0,21*(ROW(E4)-ROW(E$3)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$H$14,0,21*(ROW(A5)-ROW(A$3)))</f>
+        <v>805</v>
+      </c>
+      <c r="B5" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$J$14,0,21*(ROW(B5)-ROW(B$3)))</f>
+        <v>813</v>
+      </c>
+      <c r="C5" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$K$14,0,21*(ROW(C5)-ROW(C$3)))</f>
+        <v>0.99015990159900003</v>
+      </c>
+      <c r="D5" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$R$14,0,21*(ROW(D5)-ROW(D$3)))</f>
+        <v>0.99015990159900003</v>
+      </c>
+      <c r="E5" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$Y$14,0,21*(ROW(E5)-ROW(E$3)))</f>
+        <v>0.96057347670299997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$H$14,0,21*(ROW(A6)-ROW(A$3)))</f>
+        <v>3300</v>
+      </c>
+      <c r="B6" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$J$14,0,21*(ROW(B6)-ROW(B$3)))</f>
+        <v>3300</v>
+      </c>
+      <c r="C6" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$K$14,0,21*(ROW(C6)-ROW(C$3)))</f>
+        <v>0.99878787878800002</v>
+      </c>
+      <c r="D6" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$R$14,0,21*(ROW(D6)-ROW(D$3)))</f>
+        <v>0.99878787878800002</v>
+      </c>
+      <c r="E6" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$Y$14,0,21*(ROW(E6)-ROW(E$3)))</f>
+        <v>0.99833333333300001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$H$14,0,21*(ROW(A7)-ROW(A$3)))</f>
+        <v>805</v>
+      </c>
+      <c r="B7" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$J$14,0,21*(ROW(B7)-ROW(B$3)))</f>
+        <v>805</v>
+      </c>
+      <c r="C7" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$K$14,0,21*(ROW(C7)-ROW(C$3)))</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$R$14,0,21*(ROW(D7)-ROW(D$3)))</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="12">
+        <f ca="1">OFFSET('Five Puzzles'!$Y$14,0,21*(ROW(E7)-ROW(E$3)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" s="34"/>
+      <c r="C10" s="11">
+        <f ca="1">($A$3*C3+$A$4*C4+$A$5*C5+$A$6*C6+$A$7*C7)/($A$3+$A$4+$A$5+$A$6+$A$7)</f>
+        <v>0.99681514321141484</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" ref="D10:E10" ca="1" si="0">($A$3*D3+$A$4*D4+$A$5*D5+$A$6*D6+$A$7*D7)/($A$3+$A$4+$A$5+$A$6+$A$7)</f>
+        <v>0.99681514321141484</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.99252784152595286</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:B10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4647,14 +4854,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.375" customWidth="1"/>
-    <col min="2" max="2" width="10.375" customWidth="1"/>
-    <col min="3" max="3" width="13.75" customWidth="1"/>
-    <col min="4" max="4" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="17.25" customWidth="1"/>
-    <col min="7" max="7" width="18.125" customWidth="1"/>
-    <col min="8" max="8" width="17.375" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5257,15 +5464,15 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" customWidth="1"/>
-    <col min="2" max="2" width="13.875" customWidth="1"/>
-    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="6" width="18.75" customWidth="1"/>
-    <col min="7" max="7" width="20.625" customWidth="1"/>
-    <col min="8" max="8" width="19.625" customWidth="1"/>
+    <col min="5" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5864,8 +6071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5874,31 +6081,31 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="4" width="9" style="19"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="8" max="8" width="13.75" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="26" t="s">
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
+      <c r="A2" s="26"/>
       <c r="B2" s="2" t="s">
         <v>177</v>
       </c>
@@ -5931,39 +6138,39 @@
       <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="23">
         <f>AVERAGE('Two Puzzles'!$R$3:$R$43, 'Two Puzzles'!$AM$3:$AM$43, 'Two Puzzles'!$BH$3:$BH$43, 'Two Puzzles'!$CC$3:$CC$43, 'Two Puzzles'!$CX$3:$CX$43)</f>
         <v>0.84983451377929853</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="23">
         <f>AVERAGE('Two Puzzles'!$R$3:$R$57, 'Two Puzzles'!$AM$3:$AM$57, 'Two Puzzles'!$BH$3:$BH$57, 'Two Puzzles'!$CC$3:$CC$57, 'Two Puzzles'!$CX$3:$CX$57)</f>
         <v>0.75715864924547338</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="23">
         <f>AVERAGE('Two Puzzles'!$R$58:$R$112, 'Two Puzzles'!$AM$58:$AM$112, 'Two Puzzles'!$BH$58:$BH$112, 'Two Puzzles'!$CC$58:$CC$112, 'Two Puzzles'!$CX$58:$CX$112)</f>
         <v>0.32123237820141054</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="23">
         <f>AVERAGE('Two Puzzles'!$Y$3:$Y$43, 'Two Puzzles'!$AT$3:$AT$43, 'Two Puzzles'!$BO$3:$BO$43, 'Two Puzzles'!$CJ$3:$CJ$43, 'Two Puzzles'!$DE$3:$DE$43)</f>
         <v>0.93280464401321939</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="23">
         <f>AVERAGE('Two Puzzles'!$Y$3:$Y$57, 'Two Puzzles'!$AT$3:$AT$57, 'Two Puzzles'!$BO$3:$BO$57, 'Two Puzzles'!$CJ$3:$CJ$57, 'Two Puzzles'!$DE$3:$DE$57)</f>
         <v>0.87447248674616351</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="23">
         <f>AVERAGE('Two Puzzles'!$Y$58:$Y$112, 'Two Puzzles'!$AT$58:$AT$112, 'Two Puzzles'!$BO$58:$BO$112, 'Two Puzzles'!$CJ$58:$CJ$112, 'Two Puzzles'!$DE$58:$DE$112)</f>
         <v>0.4620062760458547</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="24">
         <f>(COUNTIF('Two Puzzles'!$K$3:$K$43,1) +COUNTIF( 'Two Puzzles'!$AF$3:$AF$43, 1)+COUNTIF('Two Puzzles'!$BA$3:$BA$43, 1) +COUNTIF('Two Puzzles'!$BV$3:$BV$43, 1)+COUNTIF('Two Puzzles'!$CQ$3:$CQ$43,1))/COUNT('Two Puzzles'!$K$3:$K$43, 'Two Puzzles'!$AF$3:$AF$43, 'Two Puzzles'!$BA$3:$BA$43, 'Two Puzzles'!$BV$3:$BV$43, 'Two Puzzles'!$CQ$3:$CQ$43)</f>
         <v>0.29268292682926828</v>
       </c>
-      <c r="I3" s="31">
+      <c r="I3" s="24">
         <f>(COUNTIF('Two Puzzles'!$K$3:$K$57,1) +COUNTIF( 'Two Puzzles'!$AF$3:$AF$57, 1)+COUNTIF('Two Puzzles'!$BA$3:$BA$57, 1) +COUNTIF('Two Puzzles'!$BV$3:$BV$57, 1)+COUNTIF('Two Puzzles'!$CQ$3:$CQ$57,1))/COUNT('Two Puzzles'!$K$3:$K$57, 'Two Puzzles'!$AF$3:$AF$57, 'Two Puzzles'!$BA$3:$BA$57, 'Two Puzzles'!$BV$3:$BV$57, 'Two Puzzles'!$CQ$3:$CQ$57)</f>
         <v>0.23636363636363636</v>
       </c>
-      <c r="J3" s="31">
+      <c r="J3" s="24">
         <f>(COUNTIF('Two Puzzles'!$K$58:$K$112,1) +COUNTIF( 'Two Puzzles'!$AF$58:$AF$112, 1)+COUNTIF('Two Puzzles'!$BA$58:$BA$112, 1) +COUNTIF('Two Puzzles'!$BV$58:$BV$112, 1)+COUNTIF('Two Puzzles'!$CQ$58:$CQ$112,1))/COUNT('Two Puzzles'!$K$58:$K$112, 'Two Puzzles'!$AF$58:$AF$112, 'Two Puzzles'!$BA$58:$BA$112, 'Two Puzzles'!$BV$58:$BV$112, 'Two Puzzles'!$CQ$58:$CQ$112)</f>
         <v>5.4545454545454543E-2</v>
       </c>
@@ -5972,39 +6179,39 @@
       <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="23">
         <f>AVERAGE('Three Puzzles'!$R$3:$R$11, 'Three Puzzles'!$AM$3:$AM$11, 'Three Puzzles'!$BH$3:$BH$11, 'Three Puzzles'!$CC$3:$CC$11, 'Three Puzzles'!$CX$3:$CX$11)</f>
         <v>0.95358277750203702</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="23">
         <f>AVERAGE('Three Puzzles'!$R$3:$R$25, 'Three Puzzles'!$AM$3:$AM$25, 'Three Puzzles'!$BH$3:$BH$25, 'Three Puzzles'!$CC$3:$CC$25, 'Three Puzzles'!$CX$3:$CX$25)</f>
         <v>0.79982154840293596</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="23">
         <f>AVERAGE('Three Puzzles'!$R$26:$R$48, 'Three Puzzles'!$AM$26:$AM$48, 'Three Puzzles'!$BH$26:$BH$48, 'Three Puzzles'!$CC$26:$CC$48, 'Three Puzzles'!$CX$26:$CX$48)</f>
         <v>0.20287870511251105</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="23">
         <f>AVERAGE('Three Puzzles'!$Y$3:$Y$11, 'Three Puzzles'!$AT$3:$AT$11, 'Three Puzzles'!$BO$3:$BO$11, 'Three Puzzles'!$CJ$3:$CJ$11, 'Three Puzzles'!$DE$3:$DE$11)</f>
         <v>0.95505137468459245</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="23">
         <f>AVERAGE('Three Puzzles'!$Y$3:$Y$25, 'Three Puzzles'!$AT$3:$AT$25, 'Three Puzzles'!$BO$3:$BO$25, 'Three Puzzles'!$CJ$3:$CJ$25, 'Three Puzzles'!$DE$3:$DE$25)</f>
         <v>0.86883242049646381</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="23">
         <f>AVERAGE('Three Puzzles'!$Y$26:$Y$48, 'Three Puzzles'!$AT$26:$AT$48, 'Three Puzzles'!$BO$26:$BO$48, 'Three Puzzles'!$CJ$26:$CJ$48, 'Three Puzzles'!$DE$26:$DE$48)</f>
         <v>0.36424235623478401</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="24">
         <f>(COUNTIF('Three Puzzles'!$K$3:$K$11,1) +COUNTIF( 'Three Puzzles'!$AF$3:$AF$11, 1)+COUNTIF('Three Puzzles'!$BA$3:$BA$11, 1) +COUNTIF('Three Puzzles'!$BV$3:$BV$11, 1)+COUNTIF('Three Puzzles'!$CQ$3:$CQ$11,1))/COUNT('Three Puzzles'!$K$3:$K$11, 'Three Puzzles'!$AF$3:$AF$11, 'Three Puzzles'!$BA$3:$BA$11, 'Three Puzzles'!$BV$3:$BV$11, 'Three Puzzles'!$CQ$3:$CQ$11)</f>
         <v>0.18518518518518517</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="24">
         <f>(COUNTIF('Three Puzzles'!$K$3:$K$25,1) +COUNTIF( 'Three Puzzles'!$AF$3:$AF$25, 1)+COUNTIF('Three Puzzles'!$BA$3:$BA$25, 1) +COUNTIF('Three Puzzles'!$BV$3:$BV$25, 1)+COUNTIF('Three Puzzles'!$CQ$3:$CQ$25,1))/COUNT('Three Puzzles'!$K$3:$K$25, 'Three Puzzles'!$AF$3:$AF$25, 'Three Puzzles'!$BA$3:$BA$25, 'Three Puzzles'!$BV$3:$BV$25, 'Three Puzzles'!$CQ$3:$CQ$25)</f>
         <v>0.18840579710144928</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J4" s="24">
         <f>(COUNTIF('Three Puzzles'!$K$26:$K$48,1) +COUNTIF( 'Three Puzzles'!$AF$26:$AF$48, 1)+COUNTIF('Three Puzzles'!$BA$26:$BA$48, 1) +COUNTIF('Three Puzzles'!$BV$26:$BV$48, 1)+COUNTIF('Three Puzzles'!$CQ$26:$CQ$48,1))/COUNT('Three Puzzles'!$K$26:$K$48, 'Three Puzzles'!$AF$26:$AF$48, 'Three Puzzles'!$BA$26:$BA$48, 'Three Puzzles'!$BV$26:$BV$48, 'Three Puzzles'!$CQ$26:$CQ$48)</f>
         <v>1.4492753623188406E-2</v>
       </c>
@@ -6013,39 +6220,39 @@
       <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="23">
         <f>AVERAGE('Four Puzzles'!$R$3:$R$6, 'Four Puzzles'!$AM$3:$AM$6, 'Four Puzzles'!$BH$3:$BH$6, 'Four Puzzles'!$CC$3:$CC$6, 'Four Puzzles'!$CX$3:$CX$6)</f>
         <v>0.88067985433268758</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="23">
         <f>AVERAGE('Four Puzzles'!$R$3:$R$10, 'Four Puzzles'!$AM$3:$AM$10, 'Four Puzzles'!$BH$3:$BH$10, 'Four Puzzles'!$CC$3:$CC$10, 'Four Puzzles'!$CX$3:$CX$10)</f>
         <v>0.77798660315657175</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="23">
         <f>AVERAGE('Four Puzzles'!$R$11:$R$18, 'Four Puzzles'!$AM$11:$AM$18, 'Four Puzzles'!$BH$11:$BH$18, 'Four Puzzles'!$CC$11:$CC$18, 'Four Puzzles'!$CX$11:$CX$18)</f>
         <v>0.10885747128991347</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="23">
         <f>AVERAGE('Four Puzzles'!$Y$3:$Y$6, 'Four Puzzles'!$AT$3:$AT$6, 'Four Puzzles'!$BO$3:$BO$6, 'Four Puzzles'!$CJ$3:$CJ$6, 'Four Puzzles'!$DE$3:$DE$6)</f>
         <v>0.91998650898237488</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="23">
         <f>AVERAGE('Four Puzzles'!$Y$3:$Y$10, 'Four Puzzles'!$AT$3:$AT$10, 'Four Puzzles'!$BO$3:$BO$10, 'Four Puzzles'!$CJ$3:$CJ$10, 'Four Puzzles'!$DE$3:$DE$10)</f>
         <v>0.86218281249084383</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="23">
         <f>AVERAGE('Four Puzzles'!$Y$11:$Y$18, 'Four Puzzles'!$AT$11:$AT$18, 'Four Puzzles'!$BO$11:$BO$18, 'Four Puzzles'!$CJ$11:$CJ$18, 'Four Puzzles'!$DE$11:$DE$18)</f>
         <v>0.25999581130692812</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="24">
         <f>(COUNTIF('Four Puzzles'!$K$3:$K$6,1) +COUNTIF( 'Four Puzzles'!$AF$3:$AF$6, 1)+COUNTIF('Four Puzzles'!$BA$3:$BA$6, 1) +COUNTIF('Four Puzzles'!$BV$3:$BV$6, 1)+COUNTIF('Four Puzzles'!$CQ$3:$CQ$6,1))/COUNT('Four Puzzles'!$K$3:$K$6, 'Four Puzzles'!$AF$3:$AF$6, 'Four Puzzles'!$BA$3:$BA$6, 'Four Puzzles'!$BV$3:$BV$6, 'Four Puzzles'!$CQ$3:$CQ$6)</f>
         <v>0.25</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="24">
         <f>(COUNTIF('Four Puzzles'!$K$3:$K$10,1) +COUNTIF( 'Four Puzzles'!$AF$3:$AF$10, 1)+COUNTIF('Four Puzzles'!$BA$3:$BA$10, 1) +COUNTIF('Four Puzzles'!$BV$3:$BV$10, 1)+COUNTIF('Four Puzzles'!$CQ$3:$CQ$10,1))/COUNT('Four Puzzles'!$K$3:$K$10, 'Four Puzzles'!$AF$3:$AF$10, 'Four Puzzles'!$BA$3:$BA$10, 'Four Puzzles'!$BV$3:$BV$10, 'Four Puzzles'!$CQ$3:$CQ$10)</f>
         <v>0.15625</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="24">
         <f>(COUNTIF('Four Puzzles'!$K$11:$K$18,1) +COUNTIF( 'Four Puzzles'!$AF$11:$AF$18, 1)+COUNTIF('Four Puzzles'!$BA$11:$BA$18, 1) +COUNTIF('Four Puzzles'!$BV$11:$BV$18, 1)+COUNTIF('Four Puzzles'!$CQ$11:$CQ$18,1))/COUNT('Four Puzzles'!$K$11:$K$18, 'Four Puzzles'!$AF$11:$AF$18, 'Four Puzzles'!$BA$11:$BA$18, 'Four Puzzles'!$BV$11:$BV$18, 'Four Puzzles'!$CQ$11:$CQ$18)</f>
         <v>0</v>
       </c>
@@ -6054,39 +6261,39 @@
       <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="23">
         <f>AVERAGE('Five Puzzles'!$R$3:$R$5, 'Five Puzzles'!$AM$3:$AM$5, 'Five Puzzles'!$BH$3:$BH$5, 'Five Puzzles'!$CC$3:$CC$5, 'Five Puzzles'!$CX$3:$CX$5)</f>
         <v>0.79279610734273331</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="23">
         <f>AVERAGE('Five Puzzles'!$R$3:$R$7, 'Five Puzzles'!$AM$3:$AM$7, 'Five Puzzles'!$BH$3:$BH$7, 'Five Puzzles'!$CC$3:$CC$7, 'Five Puzzles'!$CX$3:$CX$7)</f>
         <v>0.82781459903156007</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="23">
         <f>AVERAGE('Five Puzzles'!$R$8:$R$12, 'Five Puzzles'!$AM$8:$AM$12, 'Five Puzzles'!$BH$8:$BH$12, 'Five Puzzles'!$CC$8:$CC$12, 'Five Puzzles'!$CX$8:$CX$12)</f>
         <v>9.8659922927702939E-2</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="23">
         <f>AVERAGE('Five Puzzles'!$Y$3:$Y$5, 'Five Puzzles'!$AT$3:$AT$5, 'Five Puzzles'!$BO$3:$BO$5, 'Five Puzzles'!$CJ$3:$CJ$5, 'Five Puzzles'!$DE$3:$DE$5)</f>
         <v>0.86845374030340006</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="23">
         <f>AVERAGE('Five Puzzles'!$Y$3:$Y$7, 'Five Puzzles'!$AT$3:$AT$7, 'Five Puzzles'!$BO$3:$BO$7, 'Five Puzzles'!$CJ$3:$CJ$7, 'Five Puzzles'!$DE$3:$DE$7)</f>
         <v>0.87665176177028015</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="23">
         <f>AVERAGE('Five Puzzles'!$Y$8:$Y$12, 'Five Puzzles'!$AT$8:$AT$12, 'Five Puzzles'!$BO$8:$BO$12, 'Five Puzzles'!$CJ$8:$CJ$12, 'Five Puzzles'!$DE$8:$DE$12)</f>
         <v>0.20433746637170003</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="24">
         <f>(COUNTIF('Five Puzzles'!$K$3:$K$5,1) +COUNTIF( 'Five Puzzles'!$AF$3:$AF$5, 1)+COUNTIF('Five Puzzles'!$BA$3:$BA$5, 1) +COUNTIF('Five Puzzles'!$BV$3:$BV$5, 1)+COUNTIF('Five Puzzles'!$CQ$3:$CQ$5,1))/COUNT('Five Puzzles'!$K$3:$K$5, 'Five Puzzles'!$AF$3:$AF$5, 'Five Puzzles'!$BA$3:$BA$5, 'Five Puzzles'!$BV$3:$BV$5, 'Five Puzzles'!$CQ$3:$CQ$5)</f>
         <v>0.2</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I6" s="24">
         <f>(COUNTIF('Five Puzzles'!$K$3:$K$7,1) +COUNTIF( 'Five Puzzles'!$AF$3:$AF$7, 1)+COUNTIF('Five Puzzles'!$BA$3:$BA$7, 1) +COUNTIF('Five Puzzles'!$BV$3:$BV$7, 1)+COUNTIF('Five Puzzles'!$CQ$3:$CQ$7,1))/COUNT('Five Puzzles'!$K$3:$K$7, 'Five Puzzles'!$AF$3:$AF$7, 'Five Puzzles'!$BA$3:$BA$7, 'Five Puzzles'!$BV$3:$BV$7, 'Five Puzzles'!$CQ$3:$CQ$7)</f>
         <v>0.24</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="24">
         <f>(COUNTIF('Five Puzzles'!$K$8:$K$12,1) +COUNTIF( 'Five Puzzles'!$AF$8:$AF$12, 1)+COUNTIF('Five Puzzles'!$BA$8:$BA$12, 1) +COUNTIF('Five Puzzles'!$BV$8:$BV$12, 1)+COUNTIF('Five Puzzles'!$CQ$8:$CQ$12,1))/COUNT('Five Puzzles'!$K$8:$K$12, 'Five Puzzles'!$AF$8:$AF$12, 'Five Puzzles'!$BA$8:$BA$12, 'Five Puzzles'!$BV$8:$BV$12, 'Five Puzzles'!$CQ$8:$CQ$12)</f>
         <v>0</v>
       </c>
@@ -6113,63 +6320,63 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="3" max="3" width="29.125" customWidth="1"/>
-    <col min="4" max="4" width="12.875" customWidth="1"/>
-    <col min="5" max="5" width="13.25" customWidth="1"/>
-    <col min="6" max="6" width="21.875" customWidth="1"/>
-    <col min="7" max="7" width="21.875" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="14.375" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="15.25" customWidth="1"/>
-    <col min="10" max="10" width="14.125" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="9.375" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="13" width="12.375" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="11.375" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="12.375" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="15.25" customWidth="1"/>
-    <col min="17" max="17" width="14.125" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="9.375" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="20" width="12.375" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="11.375" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="12.375" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="15.625" customWidth="1"/>
-    <col min="24" max="24" width="12.25" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="17.375" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="15.875" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="13" width="12.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="20" width="12.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="11.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="12.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="15.5703125" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="I1" s="22" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="I1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22" t="s">
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22" t="s">
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
     </row>
     <row r="2" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -9637,108 +9844,108 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="3" max="3" width="46.25" customWidth="1"/>
-    <col min="4" max="4" width="12.875" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="25.375" customWidth="1"/>
-    <col min="7" max="7" width="21.875" customWidth="1"/>
-    <col min="8" max="8" width="14.375" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.625" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.25" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.375" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.875" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.875" customWidth="1"/>
-    <col min="29" max="29" width="14.375" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.625" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.25" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.375" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.75" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.875" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.875" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.85546875" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="I1" s="22" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="I1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22" t="s">
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22" t="s">
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AD1" s="22" t="s">
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AD1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="22"/>
-      <c r="AG1" s="22"/>
-      <c r="AH1" s="22"/>
-      <c r="AI1" s="22"/>
-      <c r="AJ1" s="22"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="22"/>
-      <c r="AQ1" s="22"/>
-      <c r="AR1" s="22" t="s">
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="23"/>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="23"/>
-      <c r="AV1" s="23"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
     </row>
     <row r="2" spans="1:49" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -26103,151 +26310,151 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="3" max="3" width="56.25" customWidth="1"/>
-    <col min="4" max="4" width="12.875" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="56.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="25.375" customWidth="1"/>
-    <col min="7" max="7" width="21.875" customWidth="1"/>
-    <col min="8" max="8" width="14.375" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.625" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.25" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.375" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.875" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.875" customWidth="1"/>
-    <col min="29" max="29" width="14.375" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.625" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.25" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.375" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.75" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.875" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.875" customWidth="1"/>
-    <col min="50" max="50" width="14.375" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.625" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.25" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.375" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.75" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.875" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.85546875" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.85546875" customWidth="1"/>
+    <col min="50" max="50" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.85546875" customWidth="1" outlineLevel="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="I1" s="22" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="I1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22" t="s">
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22" t="s">
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AD1" s="22" t="s">
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AD1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="22"/>
-      <c r="AG1" s="22"/>
-      <c r="AH1" s="22"/>
-      <c r="AI1" s="22"/>
-      <c r="AJ1" s="22"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="22"/>
-      <c r="AQ1" s="22"/>
-      <c r="AR1" s="22" t="s">
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="23"/>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="23"/>
-      <c r="AV1" s="23"/>
-      <c r="AY1" s="22" t="s">
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
+      <c r="AY1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="22"/>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22" t="s">
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="30"/>
+      <c r="BF1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="BG1" s="22"/>
-      <c r="BH1" s="22"/>
-      <c r="BI1" s="22"/>
-      <c r="BJ1" s="22"/>
-      <c r="BK1" s="22"/>
-      <c r="BL1" s="22"/>
-      <c r="BM1" s="22" t="s">
+      <c r="BG1" s="30"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="BN1" s="23"/>
-      <c r="BO1" s="23"/>
-      <c r="BP1" s="23"/>
-      <c r="BQ1" s="23"/>
+      <c r="BN1" s="31"/>
+      <c r="BO1" s="31"/>
+      <c r="BP1" s="31"/>
+      <c r="BQ1" s="31"/>
     </row>
     <row r="2" spans="1:70" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -28348,7 +28555,7 @@
       </c>
       <c r="BR11" s="13"/>
     </row>
-    <row r="12" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
@@ -28556,9 +28763,9 @@
       <c r="BQ12" s="10">
         <v>192</v>
       </c>
-      <c r="BR12" s="24"/>
+      <c r="BR12" s="21"/>
     </row>
-    <row r="13" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>8</v>
       </c>
@@ -28766,218 +28973,218 @@
       <c r="BQ13" s="10">
         <v>132</v>
       </c>
-      <c r="BR13" s="24"/>
+      <c r="BR13" s="21"/>
     </row>
-    <row r="14" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+    <row r="14" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="25">
-        <v>2</v>
-      </c>
-      <c r="C14" s="25" t="s">
+      <c r="B14" s="22">
+        <v>2</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="22">
         <v>3</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="22">
         <v>4</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="22">
         <v>-1</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="25">
-        <v>805</v>
-      </c>
-      <c r="I14" s="25" t="s">
+      <c r="H14" s="22">
+        <v>805</v>
+      </c>
+      <c r="I14" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="J14" s="25">
-        <v>805</v>
-      </c>
-      <c r="K14" s="25">
-        <v>0</v>
-      </c>
-      <c r="L14" s="25">
-        <v>0</v>
-      </c>
-      <c r="M14" s="25">
+      <c r="J14" s="22">
+        <v>805</v>
+      </c>
+      <c r="K14" s="22">
+        <v>0</v>
+      </c>
+      <c r="L14" s="22">
+        <v>0</v>
+      </c>
+      <c r="M14" s="22">
         <v>0.94409937899999996</v>
       </c>
-      <c r="N14" s="25">
-        <v>0</v>
-      </c>
-      <c r="O14" s="25">
+      <c r="N14" s="22">
+        <v>0</v>
+      </c>
+      <c r="O14" s="22">
         <v>45</v>
       </c>
-      <c r="P14" s="25" t="s">
+      <c r="P14" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="Q14" s="25">
-        <v>805</v>
-      </c>
-      <c r="R14" s="25">
+      <c r="Q14" s="22">
+        <v>805</v>
+      </c>
+      <c r="R14" s="22">
         <v>0.85714285700000004</v>
       </c>
-      <c r="S14" s="25">
-        <v>0</v>
-      </c>
-      <c r="T14" s="25">
+      <c r="S14" s="22">
+        <v>0</v>
+      </c>
+      <c r="T14" s="22">
         <v>8.6956521999999994E-2</v>
       </c>
-      <c r="U14" s="25">
-        <v>0</v>
-      </c>
-      <c r="V14" s="25">
+      <c r="U14" s="22">
+        <v>0</v>
+      </c>
+      <c r="V14" s="22">
         <v>45</v>
       </c>
-      <c r="W14" s="25" t="s">
+      <c r="W14" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="X14" s="25">
+      <c r="X14" s="22">
         <v>760</v>
       </c>
-      <c r="Y14" s="25">
+      <c r="Y14" s="22">
         <v>0.86739130399999997</v>
       </c>
-      <c r="Z14" s="25">
+      <c r="Z14" s="22">
         <v>45</v>
       </c>
-      <c r="AA14" s="25">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="25" t="s">
+      <c r="AA14" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AC14" s="25">
-        <v>805</v>
-      </c>
-      <c r="AD14" s="25" t="s">
+      <c r="AC14" s="22">
+        <v>805</v>
+      </c>
+      <c r="AD14" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="AE14" s="25">
-        <v>805</v>
-      </c>
-      <c r="AF14" s="25">
+      <c r="AE14" s="22">
+        <v>805</v>
+      </c>
+      <c r="AF14" s="22">
         <v>1</v>
       </c>
-      <c r="AG14" s="25">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="25">
-        <v>0</v>
-      </c>
-      <c r="AI14" s="25">
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="25">
-        <v>0</v>
-      </c>
-      <c r="AK14" s="25" t="s">
+      <c r="AG14" s="22">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="22">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="22">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="22">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="AL14" s="25">
-        <v>805</v>
-      </c>
-      <c r="AM14" s="25">
+      <c r="AL14" s="22">
+        <v>805</v>
+      </c>
+      <c r="AM14" s="22">
         <v>1</v>
       </c>
-      <c r="AN14" s="25">
-        <v>0</v>
-      </c>
-      <c r="AO14" s="25">
-        <v>0</v>
-      </c>
-      <c r="AP14" s="25">
-        <v>0</v>
-      </c>
-      <c r="AQ14" s="25">
-        <v>0</v>
-      </c>
-      <c r="AR14" s="25" t="s">
+      <c r="AN14" s="22">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="22">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="22">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="22">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="AS14" s="25">
-        <v>805</v>
-      </c>
-      <c r="AT14" s="25">
+      <c r="AS14" s="22">
+        <v>805</v>
+      </c>
+      <c r="AT14" s="22">
         <v>1</v>
       </c>
-      <c r="AU14" s="25">
-        <v>0</v>
-      </c>
-      <c r="AV14" s="25">
-        <v>0</v>
-      </c>
-      <c r="AW14" s="25" t="s">
+      <c r="AU14" s="22">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="22">
+        <v>0</v>
+      </c>
+      <c r="AW14" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="AX14" s="25">
-        <v>805</v>
-      </c>
-      <c r="AY14" s="25" t="s">
+      <c r="AX14" s="22">
+        <v>805</v>
+      </c>
+      <c r="AY14" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="AZ14" s="25">
+      <c r="AZ14" s="22">
         <v>829</v>
       </c>
-      <c r="BA14" s="25">
-        <v>0</v>
-      </c>
-      <c r="BB14" s="25">
+      <c r="BA14" s="22">
+        <v>0</v>
+      </c>
+      <c r="BB14" s="22">
         <v>2.8950542999999999E-2</v>
       </c>
-      <c r="BC14" s="25">
+      <c r="BC14" s="22">
         <v>0.73703256900000003</v>
       </c>
-      <c r="BD14" s="25">
-        <v>0</v>
-      </c>
-      <c r="BE14" s="25">
+      <c r="BD14" s="22">
+        <v>0</v>
+      </c>
+      <c r="BE14" s="22">
         <v>194</v>
       </c>
-      <c r="BF14" s="25" t="s">
+      <c r="BF14" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="BG14" s="25">
+      <c r="BG14" s="22">
         <v>829</v>
       </c>
-      <c r="BH14" s="25">
+      <c r="BH14" s="22">
         <v>0.73703256900000003</v>
       </c>
-      <c r="BI14" s="25">
+      <c r="BI14" s="22">
         <v>2.8950542999999999E-2</v>
       </c>
-      <c r="BJ14" s="25">
-        <v>0</v>
-      </c>
-      <c r="BK14" s="25">
-        <v>0</v>
-      </c>
-      <c r="BL14" s="25">
+      <c r="BJ14" s="22">
+        <v>0</v>
+      </c>
+      <c r="BK14" s="22">
+        <v>0</v>
+      </c>
+      <c r="BL14" s="22">
         <v>194</v>
       </c>
-      <c r="BM14" s="25" t="s">
+      <c r="BM14" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="BN14" s="25">
+      <c r="BN14" s="22">
         <v>707</v>
       </c>
-      <c r="BO14" s="25">
+      <c r="BO14" s="22">
         <v>0.66259711399999999</v>
       </c>
-      <c r="BP14" s="25">
+      <c r="BP14" s="22">
         <v>194</v>
       </c>
-      <c r="BQ14" s="25">
+      <c r="BQ14" s="22">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>8</v>
       </c>
@@ -29185,218 +29392,218 @@
       <c r="BQ15" s="10">
         <v>0</v>
       </c>
-      <c r="BR15" s="24"/>
+      <c r="BR15" s="21"/>
     </row>
-    <row r="16" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+    <row r="16" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="25">
-        <v>2</v>
-      </c>
-      <c r="C16" s="25" t="s">
+      <c r="B16" s="22">
+        <v>2</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="22">
         <v>3</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="22">
         <v>4</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="22">
         <v>-1</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="25">
-        <v>805</v>
-      </c>
-      <c r="I16" s="25" t="s">
+      <c r="H16" s="22">
+        <v>805</v>
+      </c>
+      <c r="I16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="J16" s="25">
-        <v>805</v>
-      </c>
-      <c r="K16" s="25">
-        <v>0</v>
-      </c>
-      <c r="L16" s="25">
-        <v>0</v>
-      </c>
-      <c r="M16" s="25">
+      <c r="J16" s="22">
+        <v>805</v>
+      </c>
+      <c r="K16" s="22">
+        <v>0</v>
+      </c>
+      <c r="L16" s="22">
+        <v>0</v>
+      </c>
+      <c r="M16" s="22">
         <v>1</v>
       </c>
-      <c r="N16" s="25">
-        <v>0</v>
-      </c>
-      <c r="O16" s="25">
-        <v>0</v>
-      </c>
-      <c r="P16" s="25" t="s">
+      <c r="N16" s="22">
+        <v>0</v>
+      </c>
+      <c r="O16" s="22">
+        <v>0</v>
+      </c>
+      <c r="P16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="Q16" s="25">
-        <v>805</v>
-      </c>
-      <c r="R16" s="25">
+      <c r="Q16" s="22">
+        <v>805</v>
+      </c>
+      <c r="R16" s="22">
         <v>2.6086956521700001E-2</v>
       </c>
-      <c r="S16" s="25">
-        <v>0</v>
-      </c>
-      <c r="T16" s="25">
+      <c r="S16" s="22">
+        <v>0</v>
+      </c>
+      <c r="T16" s="22">
         <v>0.97391304347800001</v>
       </c>
-      <c r="U16" s="25">
-        <v>0</v>
-      </c>
-      <c r="V16" s="25">
-        <v>0</v>
-      </c>
-      <c r="W16" s="25" t="s">
+      <c r="U16" s="22">
+        <v>0</v>
+      </c>
+      <c r="V16" s="22">
+        <v>0</v>
+      </c>
+      <c r="W16" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="X16" s="25">
-        <v>805</v>
-      </c>
-      <c r="Y16" s="25">
+      <c r="X16" s="22">
+        <v>805</v>
+      </c>
+      <c r="Y16" s="22">
         <v>0.91956521739099994</v>
       </c>
-      <c r="Z16" s="25">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="25">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="25" t="s">
+      <c r="Z16" s="22">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AC16" s="25">
-        <v>805</v>
-      </c>
-      <c r="AD16" s="25" t="s">
+      <c r="AC16" s="22">
+        <v>805</v>
+      </c>
+      <c r="AD16" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="AE16" s="25">
+      <c r="AE16" s="22">
         <v>811</v>
       </c>
-      <c r="AF16" s="25">
+      <c r="AF16" s="22">
         <v>0.99260172626400001</v>
       </c>
-      <c r="AG16" s="25">
+      <c r="AG16" s="22">
         <v>7.3982737361300002E-3</v>
       </c>
-      <c r="AH16" s="25">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="25">
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="25">
-        <v>0</v>
-      </c>
-      <c r="AK16" s="25" t="s">
+      <c r="AH16" s="22">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="22">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="22">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="AL16" s="25">
+      <c r="AL16" s="22">
         <v>811</v>
       </c>
-      <c r="AM16" s="25">
+      <c r="AM16" s="22">
         <v>0.99260172626400001</v>
       </c>
-      <c r="AN16" s="25">
+      <c r="AN16" s="22">
         <v>7.3982737361300002E-3</v>
       </c>
-      <c r="AO16" s="25">
-        <v>0</v>
-      </c>
-      <c r="AP16" s="25">
-        <v>0</v>
-      </c>
-      <c r="AQ16" s="25">
-        <v>0</v>
-      </c>
-      <c r="AR16" s="25" t="s">
+      <c r="AO16" s="22">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="22">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="22">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AS16" s="25">
+      <c r="AS16" s="22">
         <v>829</v>
       </c>
-      <c r="AT16" s="25">
+      <c r="AT16" s="22">
         <v>0.97014475271400002</v>
       </c>
-      <c r="AU16" s="25">
-        <v>0</v>
-      </c>
-      <c r="AV16" s="25">
+      <c r="AU16" s="22">
+        <v>0</v>
+      </c>
+      <c r="AV16" s="22">
         <v>24</v>
       </c>
-      <c r="AW16" s="25" t="s">
+      <c r="AW16" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="AX16" s="25">
-        <v>805</v>
-      </c>
-      <c r="AY16" s="25" t="s">
+      <c r="AX16" s="22">
+        <v>805</v>
+      </c>
+      <c r="AY16" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="AZ16" s="25">
-        <v>805</v>
-      </c>
-      <c r="BA16" s="25">
-        <v>0</v>
-      </c>
-      <c r="BB16" s="25">
-        <v>0</v>
-      </c>
-      <c r="BC16" s="25">
+      <c r="AZ16" s="22">
+        <v>805</v>
+      </c>
+      <c r="BA16" s="22">
+        <v>0</v>
+      </c>
+      <c r="BB16" s="22">
+        <v>0</v>
+      </c>
+      <c r="BC16" s="22">
         <v>0.90931677018599999</v>
       </c>
-      <c r="BD16" s="25">
+      <c r="BD16" s="22">
         <v>1.2422360248399999E-3</v>
       </c>
-      <c r="BE16" s="25">
+      <c r="BE16" s="22">
         <v>72</v>
       </c>
-      <c r="BF16" s="25" t="s">
+      <c r="BF16" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="BG16" s="25">
-        <v>805</v>
-      </c>
-      <c r="BH16" s="25">
+      <c r="BG16" s="22">
+        <v>805</v>
+      </c>
+      <c r="BH16" s="22">
         <v>0.70683229813699999</v>
       </c>
-      <c r="BI16" s="25">
-        <v>0</v>
-      </c>
-      <c r="BJ16" s="25">
+      <c r="BI16" s="22">
+        <v>0</v>
+      </c>
+      <c r="BJ16" s="22">
         <v>0.2</v>
       </c>
-      <c r="BK16" s="25">
+      <c r="BK16" s="22">
         <v>3.7267080745299998E-3</v>
       </c>
-      <c r="BL16" s="25">
+      <c r="BL16" s="22">
         <v>72</v>
       </c>
-      <c r="BM16" s="25" t="s">
+      <c r="BM16" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="BN16" s="25">
+      <c r="BN16" s="22">
         <v>733</v>
       </c>
-      <c r="BO16" s="25">
+      <c r="BO16" s="22">
         <v>0.75931677018599997</v>
       </c>
-      <c r="BP16" s="25">
+      <c r="BP16" s="22">
         <v>72</v>
       </c>
-      <c r="BQ16" s="25">
+      <c r="BQ16" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>8</v>
       </c>
@@ -29604,9 +29811,9 @@
       <c r="BQ17" s="10">
         <v>0</v>
       </c>
-      <c r="BR17" s="24"/>
+      <c r="BR17" s="21"/>
     </row>
-    <row r="18" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>8</v>
       </c>
@@ -29814,9 +30021,9 @@
       <c r="BQ18" s="10">
         <v>0</v>
       </c>
-      <c r="BR18" s="24"/>
+      <c r="BR18" s="21"/>
     </row>
-    <row r="19" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>8</v>
       </c>
@@ -30024,9 +30231,9 @@
       <c r="BQ19" s="10">
         <v>0</v>
       </c>
-      <c r="BR19" s="24"/>
+      <c r="BR19" s="21"/>
     </row>
-    <row r="20" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
@@ -30234,9 +30441,9 @@
       <c r="BQ20" s="10">
         <v>0</v>
       </c>
-      <c r="BR20" s="24"/>
+      <c r="BR20" s="21"/>
     </row>
-    <row r="21" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>8</v>
       </c>
@@ -30444,9 +30651,9 @@
       <c r="BQ21" s="10">
         <v>0</v>
       </c>
-      <c r="BR21" s="24"/>
+      <c r="BR21" s="21"/>
     </row>
-    <row r="22" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>8</v>
       </c>
@@ -30654,9 +30861,9 @@
       <c r="BQ22" s="10">
         <v>12</v>
       </c>
-      <c r="BR22" s="24"/>
+      <c r="BR22" s="21"/>
     </row>
-    <row r="23" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>8</v>
       </c>
@@ -30864,9 +31071,9 @@
       <c r="BQ23" s="10">
         <v>40</v>
       </c>
-      <c r="BR23" s="24"/>
+      <c r="BR23" s="21"/>
     </row>
-    <row r="24" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>8</v>
       </c>
@@ -31074,9 +31281,9 @@
       <c r="BQ24" s="10">
         <v>16</v>
       </c>
-      <c r="BR24" s="24"/>
+      <c r="BR24" s="21"/>
     </row>
-    <row r="25" spans="1:70" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:70" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>8</v>
       </c>
@@ -31284,7 +31491,7 @@
       <c r="BQ25" s="10">
         <v>4</v>
       </c>
-      <c r="BR25" s="24"/>
+      <c r="BR25" s="21"/>
     </row>
     <row r="26" spans="1:70" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -36121,16 +36328,16 @@
     <sortCondition ref="C3:C48"/>
   </sortState>
   <mergeCells count="10">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AR1:AV1"/>
     <mergeCell ref="AY1:BE1"/>
     <mergeCell ref="BF1:BL1"/>
     <mergeCell ref="BM1:BQ1"/>
     <mergeCell ref="AD1:AJ1"/>
     <mergeCell ref="AK1:AQ1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AR1:AV1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36148,196 +36355,196 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="67" customWidth="1"/>
-    <col min="4" max="4" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="25.375" customWidth="1"/>
-    <col min="7" max="7" width="21.875" customWidth="1"/>
-    <col min="8" max="8" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="70" max="70" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="72" max="72" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="74" max="74" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="75" max="76" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="77" max="77" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="78" max="78" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="79" max="79" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="80" max="80" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="81" max="81" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="82" max="83" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="84" max="84" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="85" max="85" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="86" max="86" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="88" max="88" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="89" max="89" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="90" max="90" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="70" max="70" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="14.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="72" max="72" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="74" max="74" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="75" max="76" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="77" max="77" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="78" max="78" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="79" max="79" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="80" max="80" width="14.140625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="81" max="81" width="9.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="82" max="83" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="84" max="84" width="11.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="85" max="85" width="12.42578125" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="86" max="86" width="15.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="12.28515625" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="88" max="88" width="17.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="89" max="89" width="14.7109375" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="90" max="90" width="15.85546875" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="91" max="91" width="9" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="I1" s="22" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="I1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22" t="s">
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22" t="s">
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AD1" s="22" t="s">
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AD1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="22"/>
-      <c r="AG1" s="22"/>
-      <c r="AH1" s="22"/>
-      <c r="AI1" s="22"/>
-      <c r="AJ1" s="22"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="22"/>
-      <c r="AQ1" s="22"/>
-      <c r="AR1" s="22" t="s">
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="23"/>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="23"/>
-      <c r="AV1" s="23"/>
-      <c r="AY1" s="22" t="s">
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
+      <c r="AY1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="22"/>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22" t="s">
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="30"/>
+      <c r="BF1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="BG1" s="22"/>
-      <c r="BH1" s="22"/>
-      <c r="BI1" s="22"/>
-      <c r="BJ1" s="22"/>
-      <c r="BK1" s="22"/>
-      <c r="BL1" s="22"/>
-      <c r="BM1" s="22" t="s">
+      <c r="BG1" s="30"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="BN1" s="23"/>
-      <c r="BO1" s="23"/>
-      <c r="BP1" s="23"/>
-      <c r="BQ1" s="23"/>
-      <c r="BT1" s="22" t="s">
+      <c r="BN1" s="31"/>
+      <c r="BO1" s="31"/>
+      <c r="BP1" s="31"/>
+      <c r="BQ1" s="31"/>
+      <c r="BT1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="BU1" s="22"/>
-      <c r="BV1" s="22"/>
-      <c r="BW1" s="22"/>
-      <c r="BX1" s="22"/>
-      <c r="BY1" s="22"/>
-      <c r="BZ1" s="22"/>
-      <c r="CA1" s="22" t="s">
+      <c r="BU1" s="30"/>
+      <c r="BV1" s="30"/>
+      <c r="BW1" s="30"/>
+      <c r="BX1" s="30"/>
+      <c r="BY1" s="30"/>
+      <c r="BZ1" s="30"/>
+      <c r="CA1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="CB1" s="22"/>
-      <c r="CC1" s="22"/>
-      <c r="CD1" s="22"/>
-      <c r="CE1" s="22"/>
-      <c r="CF1" s="22"/>
-      <c r="CG1" s="22"/>
-      <c r="CH1" s="22" t="s">
+      <c r="CB1" s="30"/>
+      <c r="CC1" s="30"/>
+      <c r="CD1" s="30"/>
+      <c r="CE1" s="30"/>
+      <c r="CF1" s="30"/>
+      <c r="CG1" s="30"/>
+      <c r="CH1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="CI1" s="23"/>
-      <c r="CJ1" s="23"/>
-      <c r="CK1" s="23"/>
-      <c r="CL1" s="23"/>
+      <c r="CI1" s="31"/>
+      <c r="CJ1" s="31"/>
+      <c r="CK1" s="31"/>
+      <c r="CL1" s="31"/>
     </row>
     <row r="2" spans="1:91" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -40974,12 +41181,6 @@
     <sortCondition ref="C3:C18"/>
   </sortState>
   <mergeCells count="13">
-    <mergeCell ref="AK1:AQ1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AD1:AJ1"/>
     <mergeCell ref="CH1:CL1"/>
     <mergeCell ref="AR1:AV1"/>
     <mergeCell ref="AY1:BE1"/>
@@ -40987,6 +41188,12 @@
     <mergeCell ref="BM1:BQ1"/>
     <mergeCell ref="BT1:BZ1"/>
     <mergeCell ref="CA1:CG1"/>
+    <mergeCell ref="AK1:AQ1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AD1:AJ1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -40996,248 +41203,247 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DI12"/>
+  <dimension ref="A1:DI14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="A3:XFD5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="3" max="3" width="87.75" customWidth="1"/>
-    <col min="4" max="4" width="12.875" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="87.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="25.375" customWidth="1"/>
-    <col min="7" max="7" width="21.875" customWidth="1"/>
-    <col min="8" max="8" width="14.375" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="11" max="11" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="12" max="13" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="14" max="14" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="15" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="16" max="16" width="15.25" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.125" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="9.375" customWidth="1" outlineLevel="2"/>
-    <col min="19" max="20" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="21" max="21" width="11.375" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="12.375" customWidth="1" outlineLevel="2"/>
-    <col min="23" max="23" width="15.625" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="12.25" customWidth="1" outlineLevel="2"/>
-    <col min="25" max="25" width="17.375" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.75" customWidth="1" outlineLevel="2"/>
-    <col min="27" max="27" width="15.875" customWidth="1" outlineLevel="2"/>
-    <col min="28" max="28" width="21.875" customWidth="1"/>
-    <col min="29" max="29" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="30" max="30" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="32" max="32" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="33" max="34" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="35" max="35" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="36" max="36" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="37" max="37" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="39" max="39" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="40" max="41" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="42" max="42" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="43" max="43" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="44" max="44" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="46" max="46" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="48" max="48" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="49" max="49" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="51" max="51" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="53" max="53" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="54" max="55" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="56" max="56" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="57" max="57" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="58" max="58" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="60" max="60" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="61" max="62" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="63" max="63" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="64" max="64" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="65" max="65" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="67" max="67" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="69" max="69" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="70" max="70" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="72" max="72" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="74" max="74" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="75" max="76" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="77" max="77" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="78" max="78" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="79" max="79" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="80" max="80" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="81" max="81" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="82" max="83" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="84" max="84" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="85" max="85" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="86" max="86" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="88" max="88" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="89" max="89" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="90" max="90" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="91" max="91" width="21.875" customWidth="1" collapsed="1"/>
-    <col min="92" max="92" width="14.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="93" max="93" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="94" max="94" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="95" max="95" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="96" max="97" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="98" max="98" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="99" max="99" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="100" max="100" width="15.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="101" max="101" width="14.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="102" max="102" width="9.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="103" max="104" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="105" max="105" width="11.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="106" max="106" width="12.375" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="107" max="107" width="15.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="108" max="108" width="12.25" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="109" max="109" width="17.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="110" max="110" width="14.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="111" max="111" width="15.875" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="112" max="112" width="9" collapsed="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="13" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="19" max="20" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="21" max="21" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="22" max="22" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="23" max="23" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="25" max="25" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="28" max="28" width="21.85546875" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="30" max="30" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="32" max="32" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="33" max="34" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="35" max="35" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="36" max="36" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="37" max="37" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="39" max="39" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="40" max="41" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="43" max="43" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="44" max="44" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="46" max="46" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="48" max="48" width="15.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="49" max="49" width="21.85546875" customWidth="1"/>
+    <col min="50" max="50" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="51" max="51" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="53" max="53" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="54" max="55" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="56" max="56" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="57" max="57" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="58" max="58" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="60" max="60" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="61" max="62" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="63" max="63" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="64" max="64" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="65" max="65" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="67" max="67" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="69" max="69" width="15.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="70" max="70" width="21.85546875" customWidth="1"/>
+    <col min="71" max="71" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="72" max="72" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="74" max="74" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="75" max="76" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="77" max="77" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="78" max="78" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="79" max="79" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="80" max="80" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="81" max="81" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="82" max="83" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="84" max="84" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="85" max="85" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="86" max="86" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="88" max="88" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="89" max="89" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="90" max="90" width="15.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="91" max="91" width="21.85546875" customWidth="1"/>
+    <col min="92" max="92" width="14.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="93" max="93" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="94" max="94" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="95" max="95" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="96" max="97" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="98" max="98" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="99" max="99" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="100" max="100" width="15.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="101" max="101" width="14.140625" customWidth="1" outlineLevel="2"/>
+    <col min="102" max="102" width="9.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="103" max="104" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="105" max="105" width="11.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="106" max="106" width="12.42578125" customWidth="1" outlineLevel="2"/>
+    <col min="107" max="107" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="108" max="108" width="12.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="109" max="109" width="17.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="110" max="110" width="14.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="111" max="111" width="15.85546875" customWidth="1" outlineLevel="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:113" x14ac:dyDescent="0.25">
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="I1" s="22" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="I1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22" t="s">
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22" t="s">
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AD1" s="22" t="s">
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AD1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="22"/>
-      <c r="AG1" s="22"/>
-      <c r="AH1" s="22"/>
-      <c r="AI1" s="22"/>
-      <c r="AJ1" s="22"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="22"/>
-      <c r="AQ1" s="22"/>
-      <c r="AR1" s="22" t="s">
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="23"/>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="23"/>
-      <c r="AV1" s="23"/>
-      <c r="AY1" s="22" t="s">
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
+      <c r="AY1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="22"/>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22" t="s">
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="30"/>
+      <c r="BF1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="BG1" s="22"/>
-      <c r="BH1" s="22"/>
-      <c r="BI1" s="22"/>
-      <c r="BJ1" s="22"/>
-      <c r="BK1" s="22"/>
-      <c r="BL1" s="22"/>
-      <c r="BM1" s="22" t="s">
+      <c r="BG1" s="30"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="BN1" s="23"/>
-      <c r="BO1" s="23"/>
-      <c r="BP1" s="23"/>
-      <c r="BQ1" s="23"/>
-      <c r="BT1" s="22" t="s">
+      <c r="BN1" s="31"/>
+      <c r="BO1" s="31"/>
+      <c r="BP1" s="31"/>
+      <c r="BQ1" s="31"/>
+      <c r="BT1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="BU1" s="22"/>
-      <c r="BV1" s="22"/>
-      <c r="BW1" s="22"/>
-      <c r="BX1" s="22"/>
-      <c r="BY1" s="22"/>
-      <c r="BZ1" s="22"/>
-      <c r="CA1" s="22" t="s">
+      <c r="BU1" s="30"/>
+      <c r="BV1" s="30"/>
+      <c r="BW1" s="30"/>
+      <c r="BX1" s="30"/>
+      <c r="BY1" s="30"/>
+      <c r="BZ1" s="30"/>
+      <c r="CA1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="CB1" s="22"/>
-      <c r="CC1" s="22"/>
-      <c r="CD1" s="22"/>
-      <c r="CE1" s="22"/>
-      <c r="CF1" s="22"/>
-      <c r="CG1" s="22"/>
-      <c r="CH1" s="22" t="s">
+      <c r="CB1" s="30"/>
+      <c r="CC1" s="30"/>
+      <c r="CD1" s="30"/>
+      <c r="CE1" s="30"/>
+      <c r="CF1" s="30"/>
+      <c r="CG1" s="30"/>
+      <c r="CH1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="CI1" s="23"/>
-      <c r="CJ1" s="23"/>
-      <c r="CK1" s="23"/>
-      <c r="CL1" s="23"/>
-      <c r="CO1" s="22" t="s">
+      <c r="CI1" s="31"/>
+      <c r="CJ1" s="31"/>
+      <c r="CK1" s="31"/>
+      <c r="CL1" s="31"/>
+      <c r="CO1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="CP1" s="22"/>
-      <c r="CQ1" s="22"/>
-      <c r="CR1" s="22"/>
-      <c r="CS1" s="22"/>
-      <c r="CT1" s="22"/>
-      <c r="CU1" s="22"/>
-      <c r="CV1" s="22" t="s">
+      <c r="CP1" s="30"/>
+      <c r="CQ1" s="30"/>
+      <c r="CR1" s="30"/>
+      <c r="CS1" s="30"/>
+      <c r="CT1" s="30"/>
+      <c r="CU1" s="30"/>
+      <c r="CV1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="CW1" s="22"/>
-      <c r="CX1" s="22"/>
-      <c r="CY1" s="22"/>
-      <c r="CZ1" s="22"/>
-      <c r="DA1" s="22"/>
-      <c r="DB1" s="22"/>
-      <c r="DC1" s="22" t="s">
+      <c r="CW1" s="30"/>
+      <c r="CX1" s="30"/>
+      <c r="CY1" s="30"/>
+      <c r="CZ1" s="30"/>
+      <c r="DA1" s="30"/>
+      <c r="DB1" s="30"/>
+      <c r="DC1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="DD1" s="23"/>
-      <c r="DE1" s="23"/>
-      <c r="DF1" s="23"/>
-      <c r="DG1" s="23"/>
+      <c r="DD1" s="31"/>
+      <c r="DE1" s="31"/>
+      <c r="DF1" s="31"/>
+      <c r="DG1" s="31"/>
     </row>
     <row r="2" spans="1:113" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -42585,7 +42791,7 @@
       <c r="DH5" s="6"/>
       <c r="DI5" s="6"/>
     </row>
-    <row r="6" spans="1:113" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:113" s="19" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -44943,6 +45149,343 @@
       </c>
       <c r="DH12" s="6"/>
       <c r="DI12" s="6"/>
+    </row>
+    <row r="14" spans="1:113" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5">
+        <v>5</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="5">
+        <v>805</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="5">
+        <v>805</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0.99006211180100001</v>
+      </c>
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+      <c r="O14" s="5">
+        <v>8</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>805</v>
+      </c>
+      <c r="R14" s="5">
+        <v>0.99006211180100001</v>
+      </c>
+      <c r="S14" s="5">
+        <v>0</v>
+      </c>
+      <c r="T14" s="5">
+        <v>0</v>
+      </c>
+      <c r="U14" s="5">
+        <v>0</v>
+      </c>
+      <c r="V14" s="5">
+        <v>8</v>
+      </c>
+      <c r="W14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X14" s="5">
+        <v>797</v>
+      </c>
+      <c r="Y14" s="5">
+        <v>0.98819875776400001</v>
+      </c>
+      <c r="Z14" s="5">
+        <v>8</v>
+      </c>
+      <c r="AA14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC14" s="5">
+        <v>540</v>
+      </c>
+      <c r="AD14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE14" s="5">
+        <v>540</v>
+      </c>
+      <c r="AF14" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL14" s="5">
+        <v>540</v>
+      </c>
+      <c r="AM14" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS14" s="5">
+        <v>540</v>
+      </c>
+      <c r="AT14" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX14" s="5">
+        <v>805</v>
+      </c>
+      <c r="AY14" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ14" s="5">
+        <v>813</v>
+      </c>
+      <c r="BA14" s="5">
+        <v>0.99015990159900003</v>
+      </c>
+      <c r="BB14" s="5">
+        <v>9.8400984009799995E-3</v>
+      </c>
+      <c r="BC14" s="5">
+        <v>0</v>
+      </c>
+      <c r="BD14" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE14" s="5">
+        <v>0</v>
+      </c>
+      <c r="BF14" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="BG14" s="5">
+        <v>813</v>
+      </c>
+      <c r="BH14" s="5">
+        <v>0.99015990159900003</v>
+      </c>
+      <c r="BI14" s="5">
+        <v>9.8400984009799995E-3</v>
+      </c>
+      <c r="BJ14" s="5">
+        <v>0</v>
+      </c>
+      <c r="BK14" s="5">
+        <v>0</v>
+      </c>
+      <c r="BL14" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM14" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="BN14" s="5">
+        <v>837</v>
+      </c>
+      <c r="BO14" s="5">
+        <v>0.96057347670299997</v>
+      </c>
+      <c r="BP14" s="5">
+        <v>0</v>
+      </c>
+      <c r="BQ14" s="5">
+        <v>32</v>
+      </c>
+      <c r="BR14" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="BS14" s="5">
+        <v>3300</v>
+      </c>
+      <c r="BT14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="BU14" s="5">
+        <v>3300</v>
+      </c>
+      <c r="BV14" s="5">
+        <v>0.99878787878800002</v>
+      </c>
+      <c r="BW14" s="5">
+        <v>0</v>
+      </c>
+      <c r="BX14" s="5">
+        <v>1.21212121212E-3</v>
+      </c>
+      <c r="BY14" s="5">
+        <v>0</v>
+      </c>
+      <c r="BZ14" s="5">
+        <v>0</v>
+      </c>
+      <c r="CA14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="CB14" s="5">
+        <v>3300</v>
+      </c>
+      <c r="CC14" s="5">
+        <v>0.99878787878800002</v>
+      </c>
+      <c r="CD14" s="5">
+        <v>0</v>
+      </c>
+      <c r="CE14" s="5">
+        <v>1.21212121212E-3</v>
+      </c>
+      <c r="CF14" s="5">
+        <v>0</v>
+      </c>
+      <c r="CG14" s="5">
+        <v>0</v>
+      </c>
+      <c r="CH14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="CI14" s="5">
+        <v>3300</v>
+      </c>
+      <c r="CJ14" s="5">
+        <v>0.99833333333300001</v>
+      </c>
+      <c r="CK14" s="5">
+        <v>0</v>
+      </c>
+      <c r="CL14" s="5">
+        <v>0</v>
+      </c>
+      <c r="CM14" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="CN14" s="5">
+        <v>805</v>
+      </c>
+      <c r="CO14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="CP14" s="5">
+        <v>805</v>
+      </c>
+      <c r="CQ14" s="5">
+        <v>1</v>
+      </c>
+      <c r="CR14" s="5">
+        <v>0</v>
+      </c>
+      <c r="CS14" s="5">
+        <v>0</v>
+      </c>
+      <c r="CT14" s="5">
+        <v>0</v>
+      </c>
+      <c r="CU14" s="5">
+        <v>0</v>
+      </c>
+      <c r="CV14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="CW14" s="5">
+        <v>805</v>
+      </c>
+      <c r="CX14" s="5">
+        <v>1</v>
+      </c>
+      <c r="CY14" s="5">
+        <v>0</v>
+      </c>
+      <c r="CZ14" s="5">
+        <v>0</v>
+      </c>
+      <c r="DA14" s="5">
+        <v>0</v>
+      </c>
+      <c r="DB14" s="5">
+        <v>0</v>
+      </c>
+      <c r="DC14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="DD14" s="5">
+        <v>805</v>
+      </c>
+      <c r="DE14" s="5">
+        <v>1</v>
+      </c>
+      <c r="DF14" s="5">
+        <v>0</v>
+      </c>
+      <c r="DG14" s="5">
+        <v>0</v>
+      </c>
+      <c r="DH14" s="6"/>
+      <c r="DI14" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A3:DI12">
@@ -44951,12 +45494,6 @@
     <sortCondition ref="B3:B12"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AY1:BE1"/>
-    <mergeCell ref="AR1:AV1"/>
     <mergeCell ref="CO1:CU1"/>
     <mergeCell ref="CV1:DB1"/>
     <mergeCell ref="DC1:DG1"/>
@@ -44967,6 +45504,12 @@
     <mergeCell ref="BT1:BZ1"/>
     <mergeCell ref="BM1:BQ1"/>
     <mergeCell ref="BF1:BL1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AY1:BE1"/>
+    <mergeCell ref="AR1:AV1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating the analysis in the mixed bag solver results page.
</commit_message>
<xml_diff>
--- a/Results/Mixed Bag Solver Puzzle Results.xlsx
+++ b/Results/Mixed Bag Solver Puzzle Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="2805" windowWidth="27960" windowHeight="12480" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="2010" yWindow="2805" windowWidth="27960" windowHeight="12480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cho Best Buddies" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3284" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3290" uniqueCount="192">
   <si>
     <t>Solver Type</t>
   </si>
@@ -592,6 +592,15 @@
   <si>
     <t># Solved Pieces</t>
   </si>
+  <si>
+    <t>Average Best Buddy Density</t>
+  </si>
+  <si>
+    <t>Incorrect Puzzle Count</t>
+  </si>
+  <si>
+    <t>Correct Puzzle Count</t>
+  </si>
 </sst>
 </file>
 
@@ -758,7 +767,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -974,6 +983,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -1174,7 +1189,7 @@
     <xf numFmtId="0" fontId="4" fillId="36" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1253,6 +1268,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="39" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="37" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -4626,6 +4663,27 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="BT1:BZ1"/>
+    <mergeCell ref="CA1:CG1"/>
+    <mergeCell ref="BM1:BQ1"/>
+    <mergeCell ref="DQ1:DW1"/>
+    <mergeCell ref="DX1:EB1"/>
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="AY1:BE1"/>
+    <mergeCell ref="BF1:BL1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AD1:AJ1"/>
+    <mergeCell ref="AK1:AQ1"/>
+    <mergeCell ref="HD1:HH1"/>
+    <mergeCell ref="FN1:FR1"/>
+    <mergeCell ref="FU1:GA1"/>
+    <mergeCell ref="GB1:GH1"/>
+    <mergeCell ref="GI1:GM1"/>
+    <mergeCell ref="GP1:GV1"/>
+    <mergeCell ref="GW1:HC1"/>
     <mergeCell ref="FG1:FM1"/>
     <mergeCell ref="CH1:CL1"/>
     <mergeCell ref="CO1:CU1"/>
@@ -4636,27 +4694,6 @@
     <mergeCell ref="ES1:EW1"/>
     <mergeCell ref="EE1:EK1"/>
     <mergeCell ref="EL1:ER1"/>
-    <mergeCell ref="HD1:HH1"/>
-    <mergeCell ref="FN1:FR1"/>
-    <mergeCell ref="FU1:GA1"/>
-    <mergeCell ref="GB1:GH1"/>
-    <mergeCell ref="GI1:GM1"/>
-    <mergeCell ref="GP1:GV1"/>
-    <mergeCell ref="GW1:HC1"/>
-    <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="AY1:BE1"/>
-    <mergeCell ref="BF1:BL1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AD1:AJ1"/>
-    <mergeCell ref="AK1:AQ1"/>
-    <mergeCell ref="BT1:BZ1"/>
-    <mergeCell ref="CA1:CG1"/>
-    <mergeCell ref="BM1:BQ1"/>
-    <mergeCell ref="DQ1:DW1"/>
-    <mergeCell ref="DX1:EB1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4667,7 +4704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -4846,10 +4883,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5001,423 +5038,423 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="6" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="39">
         <v>1516</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="39">
         <v>96.97</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="39">
         <v>70.19</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="39">
         <v>97.42</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="40">
         <f t="shared" si="0"/>
         <v>92.553191489361694</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="39">
         <v>39</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="39">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="10">
         <v>1462</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="10">
         <v>98.5</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="10">
         <v>67.69</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="10">
         <v>98.97</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="42">
         <f t="shared" si="0"/>
         <v>92.553191489361694</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="10">
         <v>15</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="10">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+    <row r="8" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="39">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="39">
         <v>1950</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="39">
         <v>99.69</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="39">
         <v>90.28</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="39">
         <v>99.85</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="40">
         <f t="shared" si="0"/>
         <v>96.808510638297875</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="39">
         <v>3</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="39">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="9" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="39">
         <v>1134</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="39">
         <v>93.83</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="39">
         <v>52.5</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="39">
         <v>94.49</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="40">
         <f t="shared" si="0"/>
         <v>91.489361702127653</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="39">
         <v>62</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="39">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="10" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="10">
         <v>1356</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="10">
         <v>95.72</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="10">
         <v>62.78</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="10">
         <v>95.79</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="42">
         <f t="shared" si="0"/>
         <v>98.936170212765958</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="10">
         <v>57</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+    <row r="11" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="10">
         <v>1662</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="10">
         <v>98.56</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="10">
         <v>76.94</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="10">
         <v>99.3</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="42">
         <f t="shared" si="0"/>
         <v>86.170212765957444</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="10">
         <v>11</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="10">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="12" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="39">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="39">
         <v>1740</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="39">
         <v>99.54</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="39">
         <v>80.56</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="39">
         <v>99.65</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="40">
         <f t="shared" si="0"/>
         <v>97.872340425531917</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="39">
         <v>6</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="39">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+    <row r="13" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="39">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="39">
         <v>1434</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="39">
         <v>98.19</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="39">
         <v>66.39</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="39">
         <v>98.74</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="40">
         <f t="shared" si="0"/>
         <v>91.489361702127653</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="39">
         <v>18</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="39">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+    <row r="14" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="39">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="39">
         <v>1742</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="39">
         <v>98.74</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="39">
         <v>80.650000000000006</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="39">
         <v>99.02</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="40">
         <f t="shared" si="0"/>
         <v>94.680851063829792</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="39">
         <v>17</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="39">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+    <row r="15" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="39">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="39">
         <v>1826</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="39">
         <v>99.01</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="39">
         <v>84.54</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="39">
         <v>99.56</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="40">
         <f t="shared" si="0"/>
         <v>89.361702127659569</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="39">
         <v>8</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="39">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+    <row r="16" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="39">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="39">
         <v>1978</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="39">
         <v>99.09</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="39">
         <v>91.57</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="39">
         <v>99.59</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="40">
         <f t="shared" si="0"/>
         <v>89.361702127659569</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="39">
         <v>8</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="39">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+    <row r="17" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="39">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="39">
         <v>1912</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="39">
         <v>99.37</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="39">
         <v>88.52</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="39">
         <v>99.63</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="40">
         <f t="shared" si="0"/>
         <v>94.680851063829792</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="39">
         <v>7</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="39">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+    <row r="18" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="10">
         <v>1242</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="10">
         <v>95.97</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="10">
         <v>57.5</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="10">
         <v>96.52</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="42">
         <f t="shared" si="0"/>
         <v>92.553191489361694</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="10">
         <v>43</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="10">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+    <row r="19" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="39">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="39">
         <v>1314</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="39">
         <v>98.17</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="39">
         <v>60.83</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="39">
         <v>98.25</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="40">
         <f t="shared" si="0"/>
         <v>98.936170212765958</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="39">
         <v>23</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="39">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+    <row r="20" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="39">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="39">
         <v>1644</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="39">
         <v>98.54</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="39">
         <v>76.11</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="39">
         <v>98.9</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="40">
         <f t="shared" si="0"/>
         <v>93.61702127659575</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="39">
         <v>18</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="39">
         <v>6</v>
       </c>
     </row>
@@ -5449,7 +5486,39 @@
         <v>8</v>
       </c>
     </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="B25" s="37"/>
+      <c r="C25" s="38">
+        <f>AVERAGE(D7,D10,D11,D18)</f>
+        <v>66.227499999999992</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="B26" s="37"/>
+      <c r="C26" s="38">
+        <f>AVERAGE(D2:D6,D8:D9,D12:D17,D19:D21)</f>
+        <v>74.462499999999977</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+  </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5458,10 +5527,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6060,7 +6129,39 @@
         <v>15</v>
       </c>
     </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" s="37"/>
+      <c r="C24" s="38">
+        <f>AVERAGE(D17,D13,D4)</f>
+        <v>62.133333333333326</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="37"/>
+      <c r="C25" s="38">
+        <f>AVERAGE(D2,D3,D5:D12,D14:D16,D18:D21)</f>
+        <v>74.02823529411765</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+  </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6314,8 +6415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F29" sqref="A25:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -36328,16 +36429,16 @@
     <sortCondition ref="C3:C48"/>
   </sortState>
   <mergeCells count="10">
+    <mergeCell ref="AY1:BE1"/>
+    <mergeCell ref="BF1:BL1"/>
+    <mergeCell ref="BM1:BQ1"/>
+    <mergeCell ref="AD1:AJ1"/>
+    <mergeCell ref="AK1:AQ1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="P1:V1"/>
     <mergeCell ref="W1:AA1"/>
     <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="AY1:BE1"/>
-    <mergeCell ref="BF1:BL1"/>
-    <mergeCell ref="BM1:BQ1"/>
-    <mergeCell ref="AD1:AJ1"/>
-    <mergeCell ref="AK1:AQ1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41181,6 +41282,12 @@
     <sortCondition ref="C3:C18"/>
   </sortState>
   <mergeCells count="13">
+    <mergeCell ref="AK1:AQ1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AD1:AJ1"/>
     <mergeCell ref="CH1:CL1"/>
     <mergeCell ref="AR1:AV1"/>
     <mergeCell ref="AY1:BE1"/>
@@ -41188,12 +41295,6 @@
     <mergeCell ref="BM1:BQ1"/>
     <mergeCell ref="BT1:BZ1"/>
     <mergeCell ref="CA1:CG1"/>
-    <mergeCell ref="AK1:AQ1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AD1:AJ1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45494,6 +45595,12 @@
     <sortCondition ref="B3:B12"/>
   </sortState>
   <mergeCells count="16">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AY1:BE1"/>
+    <mergeCell ref="AR1:AV1"/>
     <mergeCell ref="CO1:CU1"/>
     <mergeCell ref="CV1:DB1"/>
     <mergeCell ref="DC1:DG1"/>
@@ -45504,12 +45611,6 @@
     <mergeCell ref="BT1:BZ1"/>
     <mergeCell ref="BM1:BQ1"/>
     <mergeCell ref="BF1:BL1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AY1:BE1"/>
-    <mergeCell ref="AR1:AV1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>